<commit_message>
bake migration AddDateToContracts contract_date:date
</commit_message>
<xml_diff>
--- a/document/sql_creator.xlsx
+++ b/document/sql_creator.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="176">
   <si>
     <t>属性</t>
     <rPh sb="0" eb="2">
@@ -938,6 +938,17 @@
   </si>
   <si>
     <t>company_code</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>契約日</t>
+    <rPh sb="0" eb="3">
+      <t>ケイヤクビ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>contract_date</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1383,7 +1394,27 @@
     <cellStyle name="メモ" xfId="1" builtinId="10"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="76">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2337,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J158"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -3788,11 +3819,11 @@
       <c r="G65" s="37"/>
       <c r="H65" s="38"/>
       <c r="I65" s="40" t="str">
-        <f t="shared" ref="I65:I72" si="10">"," &amp; IF(A65="","","/* ") &amp; "`" &amp; C65 &amp; "` " &amp; D65 &amp; IF(E65&gt;0,"(" &amp; E65 &amp; ") "," ") &amp; IF(F65&lt;&gt;"","NOT NULL ","") &amp; IF(G65="","","DEFAULT '" &amp; G65 &amp; "' ") &amp; IF(A65="",""," */")</f>
+        <f t="shared" ref="I65:I73" si="10">"," &amp; IF(A65="","","/* ") &amp; "`" &amp; C65 &amp; "` " &amp; D65 &amp; IF(E65&gt;0,"(" &amp; E65 &amp; ") "," ") &amp; IF(F65&lt;&gt;"","NOT NULL ","") &amp; IF(G65="","","DEFAULT '" &amp; G65 &amp; "' ") &amp; IF(A65="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT NOT NULL </v>
       </c>
       <c r="J65" s="41" t="str">
-        <f t="shared" ref="J65:J72" si="11">"," &amp; IF(A65="","","/* ") &amp; "`" &amp; C65 &amp; "` " &amp; D65 &amp; IF(E65&gt;0,"(" &amp; E65 &amp; ") "," ") &amp; IF(F65&lt;&gt;"","NOT NULL ","") &amp; IF(G65="","","DEFAULT '" &amp; G65 &amp; "' ") &amp; IF(A65="",""," */")</f>
+        <f t="shared" ref="J65:J73" si="11">"," &amp; IF(A65="","","/* ") &amp; "`" &amp; C65 &amp; "` " &amp; D65 &amp; IF(E65&gt;0,"(" &amp; E65 &amp; ") "," ") &amp; IF(F65&lt;&gt;"","NOT NULL ","") &amp; IF(G65="","","DEFAULT '" &amp; G65 &amp; "' ") &amp; IF(A65="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT NOT NULL </v>
       </c>
     </row>
@@ -3823,37 +3854,37 @@
     <row r="67" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A67" s="34"/>
       <c r="B67" s="39" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E67" s="36"/>
       <c r="F67" s="35"/>
       <c r="G67" s="37"/>
       <c r="H67" s="38"/>
       <c r="I67" s="40" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">,`contractname_id` INT </v>
+        <f t="shared" ref="I67" si="12">"," &amp; IF(A67="","","/* ") &amp; "`" &amp; C67 &amp; "` " &amp; D67 &amp; IF(E67&gt;0,"(" &amp; E67 &amp; ") "," ") &amp; IF(F67&lt;&gt;"","NOT NULL ","") &amp; IF(G67="","","DEFAULT '" &amp; G67 &amp; "' ") &amp; IF(A67="",""," */")</f>
+        <v xml:space="preserve">,`contract_date` DATE </v>
       </c>
       <c r="J67" s="41" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">,`contractname_id` INT </v>
+        <f t="shared" ref="J67" si="13">"," &amp; IF(A67="","","/* ") &amp; "`" &amp; C67 &amp; "` " &amp; D67 &amp; IF(E67&gt;0,"(" &amp; E67 &amp; ") "," ") &amp; IF(F67&lt;&gt;"","NOT NULL ","") &amp; IF(G67="","","DEFAULT '" &amp; G67 &amp; "' ") &amp; IF(A67="",""," */")</f>
+        <v xml:space="preserve">,`contract_date` DATE </v>
       </c>
     </row>
     <row r="68" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="34"/>
       <c r="B68" s="39" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="C68" s="35" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="D68" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E68" s="36"/>
       <c r="F68" s="35"/>
@@ -3861,46 +3892,44 @@
       <c r="H68" s="38"/>
       <c r="I68" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`remarks` TEXT </v>
+        <v xml:space="preserve">,`contractname_id` INT </v>
       </c>
       <c r="J68" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`remarks` TEXT </v>
+        <v xml:space="preserve">,`contractname_id` INT </v>
       </c>
     </row>
     <row r="69" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A69" s="34"/>
-      <c r="B69" s="43" t="s">
-        <v>135</v>
+      <c r="B69" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="C69" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E69" s="36">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E69" s="36"/>
       <c r="F69" s="35"/>
       <c r="G69" s="37"/>
       <c r="H69" s="38"/>
       <c r="I69" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <v xml:space="preserve">,`remarks` TEXT </v>
       </c>
       <c r="J69" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <v xml:space="preserve">,`remarks` TEXT </v>
       </c>
     </row>
     <row r="70" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A70" s="34"/>
       <c r="B70" s="43" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="C70" s="35" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="D70" s="35" t="s">
         <v>7</v>
@@ -3913,118 +3942,120 @@
       <c r="H70" s="38"/>
       <c r="I70" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J70" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="71" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A71" s="34"/>
       <c r="B71" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C71" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D71" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E71" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E71" s="36">
+        <v>256</v>
+      </c>
       <c r="F71" s="35"/>
       <c r="G71" s="37"/>
       <c r="H71" s="38"/>
       <c r="I71" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J71" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="72" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A72" s="34"/>
       <c r="B72" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C72" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D72" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" s="36">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E72" s="36"/>
       <c r="F72" s="35"/>
       <c r="G72" s="37"/>
       <c r="H72" s="38"/>
       <c r="I72" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
       <c r="J72" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
     </row>
     <row r="73" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A73" s="34"/>
       <c r="B73" s="43" t="s">
-        <v>161</v>
+        <v>52</v>
       </c>
       <c r="C73" s="35" t="s">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="D73" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E73" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E73" s="36">
+        <v>64</v>
+      </c>
       <c r="F73" s="35"/>
       <c r="G73" s="37"/>
       <c r="H73" s="38"/>
       <c r="I73" s="40" t="str">
-        <f t="shared" ref="I73:I75" si="12">"," &amp; IF(A73="","","/* ") &amp; "`" &amp; C73 &amp; "` " &amp; D73 &amp; IF(E73&gt;0,"(" &amp; E73 &amp; ") "," ") &amp; IF(F73&lt;&gt;"","NOT NULL ","") &amp; IF(G73="","","DEFAULT '" &amp; G73 &amp; "' ") &amp; IF(A73="",""," */")</f>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
       <c r="J73" s="41" t="str">
-        <f t="shared" ref="J73:J75" si="13">"," &amp; IF(A73="","","/* ") &amp; "`" &amp; C73 &amp; "` " &amp; D73 &amp; IF(E73&gt;0,"(" &amp; E73 &amp; ") "," ") &amp; IF(F73&lt;&gt;"","NOT NULL ","") &amp; IF(G73="","","DEFAULT '" &amp; G73 &amp; "' ") &amp; IF(A73="",""," */")</f>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
     <row r="74" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="34"/>
       <c r="B74" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C74" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D74" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E74" s="36"/>
       <c r="F74" s="35"/>
       <c r="G74" s="37"/>
       <c r="H74" s="38"/>
       <c r="I74" s="40" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" ref="I74:I76" si="14">"," &amp; IF(A74="","","/* ") &amp; "`" &amp; C74 &amp; "` " &amp; D74 &amp; IF(E74&gt;0,"(" &amp; E74 &amp; ") "," ") &amp; IF(F74&lt;&gt;"","NOT NULL ","") &amp; IF(G74="","","DEFAULT '" &amp; G74 &amp; "' ") &amp; IF(A74="",""," */")</f>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J74" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" ref="J74:J76" si="15">"," &amp; IF(A74="","","/* ") &amp; "`" &amp; C74 &amp; "` " &amp; D74 &amp; IF(E74&gt;0,"(" &amp; E74 &amp; ") "," ") &amp; IF(F74&lt;&gt;"","NOT NULL ","") &amp; IF(G74="","","DEFAULT '" &amp; G74 &amp; "' ") &amp; IF(A74="",""," */")</f>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="75" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A75" s="34"/>
       <c r="B75" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C75" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D75" s="35" t="s">
         <v>8</v>
@@ -4034,156 +4065,154 @@
       <c r="G75" s="37"/>
       <c r="H75" s="38"/>
       <c r="I75" s="40" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J75" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="76" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A76" s="34"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="21"/>
-      <c r="G76" s="23"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J76" s="41" t="s">
-        <v>33</v>
+      <c r="B76" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C76" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D76" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="36"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="40" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
+      </c>
+      <c r="J76" s="41" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="77" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="G77" s="3"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="25"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A78" s="2"/>
-      <c r="B78" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F78" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G78" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H78" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I78" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C78 &amp; "` ("</f>
-        <v>CREATE TABLE `orders` (</v>
-      </c>
-      <c r="J78" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C78 &amp; "` ("</f>
-        <v>CREATE TABLE `orders` (</v>
-      </c>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J77" s="41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="G78" s="3"/>
+      <c r="I78" s="25"/>
+      <c r="J78" s="25"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="2"/>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G79" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I79" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C79 &amp; "` ("</f>
+        <v>CREATE TABLE `orders` (</v>
+      </c>
+      <c r="J79" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C79 &amp; "` ("</f>
+        <v>CREATE TABLE `orders` (</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A80" s="2"/>
+      <c r="B80" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C80" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D80" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E79" s="7"/>
-      <c r="F79" s="6" t="s">
+      <c r="E80" s="7"/>
+      <c r="F80" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G79" s="8"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="28" t="s">
+      <c r="G80" s="8"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J79" s="30" t="s">
+      <c r="J80" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="34"/>
-      <c r="B80" s="32" t="s">
+    <row r="81" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="34"/>
+      <c r="B81" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C80" s="35" t="s">
+      <c r="C81" s="35" t="s">
         <v>131</v>
-      </c>
-      <c r="D80" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E80" s="36">
-        <v>20</v>
-      </c>
-      <c r="F80" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G80" s="37"/>
-      <c r="H80" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="I80" s="40" t="str">
-        <f t="shared" ref="I80:I92" si="14">"," &amp; IF(A80="","","/* ") &amp; "`" &amp; C80 &amp; "` " &amp; D80 &amp; IF(E80&gt;0,"(" &amp; E80 &amp; ") "," ") &amp; IF(F80&lt;&gt;"","NOT NULL ","") &amp; IF(G80="","","DEFAULT '" &amp; G80 &amp; "' ") &amp; IF(A80="",""," */")</f>
-        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
-      </c>
-      <c r="J80" s="41" t="str">
-        <f t="shared" ref="J80:J92" si="15">"," &amp; IF(A80="","","/* ") &amp; "`" &amp; C80 &amp; "` " &amp; D80 &amp; IF(E80&gt;0,"(" &amp; E80 &amp; ") "," ") &amp; IF(F80&lt;&gt;"","NOT NULL ","") &amp; IF(G80="","","DEFAULT '" &amp; G80 &amp; "' ") &amp; IF(A80="",""," */")</f>
-        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A81" s="2"/>
-      <c r="B81" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C81" s="35" t="s">
-        <v>132</v>
       </c>
       <c r="D81" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="36">
-        <v>256</v>
-      </c>
-      <c r="F81" s="35"/>
+        <v>20</v>
+      </c>
+      <c r="F81" s="35" t="s">
+        <v>18</v>
+      </c>
       <c r="G81" s="37"/>
-      <c r="H81" s="38"/>
+      <c r="H81" s="38" t="s">
+        <v>138</v>
+      </c>
       <c r="I81" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
+        <f t="shared" ref="I81:I93" si="16">"," &amp; IF(A81="","","/* ") &amp; "`" &amp; C81 &amp; "` " &amp; D81 &amp; IF(E81&gt;0,"(" &amp; E81 &amp; ") "," ") &amp; IF(F81&lt;&gt;"","NOT NULL ","") &amp; IF(G81="","","DEFAULT '" &amp; G81 &amp; "' ") &amp; IF(A81="",""," */")</f>
+        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
       </c>
       <c r="J81" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="34"/>
-      <c r="B82" s="39" t="s">
-        <v>113</v>
+        <f t="shared" ref="J81:J93" si="17">"," &amp; IF(A81="","","/* ") &amp; "`" &amp; C81 &amp; "` " &amp; D81 &amp; IF(E81&gt;0,"(" &amp; E81 &amp; ") "," ") &amp; IF(F81&lt;&gt;"","NOT NULL ","") &amp; IF(G81="","","DEFAULT '" &amp; G81 &amp; "' ") &amp; IF(A81="",""," */")</f>
+        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A82" s="2"/>
+      <c r="B82" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="C82" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D82" s="35" t="s">
         <v>7</v>
@@ -4195,71 +4224,71 @@
       <c r="G82" s="37"/>
       <c r="H82" s="38"/>
       <c r="I82" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
       </c>
       <c r="J82" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
       </c>
     </row>
     <row r="83" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A83" s="34"/>
       <c r="B83" s="39" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C83" s="35" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="D83" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E83" s="36">
+        <v>256</v>
+      </c>
       <c r="F83" s="35"/>
       <c r="G83" s="37"/>
       <c r="H83" s="38"/>
       <c r="I83" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`order_date` DATE </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
       </c>
       <c r="J83" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`order_date` DATE </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
       </c>
     </row>
     <row r="84" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A84" s="34"/>
       <c r="B84" s="39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C84" s="35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D84" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84" s="36">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E84" s="36"/>
       <c r="F84" s="35"/>
       <c r="G84" s="37"/>
       <c r="H84" s="38"/>
       <c r="I84" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`order_date` DATE </v>
       </c>
       <c r="J84" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`order_date` DATE </v>
       </c>
     </row>
     <row r="85" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A85" s="34"/>
       <c r="B85" s="39" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C85" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D85" s="35" t="s">
         <v>7</v>
@@ -4271,21 +4300,21 @@
       <c r="G85" s="37"/>
       <c r="H85" s="38"/>
       <c r="I85" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
       </c>
       <c r="J85" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="86" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A86" s="34"/>
       <c r="B86" s="39" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C86" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D86" s="35" t="s">
         <v>7</v>
@@ -4295,49 +4324,51 @@
       </c>
       <c r="F86" s="35"/>
       <c r="G86" s="37"/>
-      <c r="H86" s="38" t="s">
-        <v>134</v>
-      </c>
+      <c r="H86" s="38"/>
       <c r="I86" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
       </c>
       <c r="J86" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="87" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A87" s="34"/>
       <c r="B87" s="39" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C87" s="35" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D87" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E87" s="36">
+        <v>20</v>
+      </c>
       <c r="F87" s="35"/>
       <c r="G87" s="37"/>
-      <c r="H87" s="38"/>
+      <c r="H87" s="38" t="s">
+        <v>134</v>
+      </c>
       <c r="I87" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`delivery_date` DATE </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
       </c>
       <c r="J87" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`delivery_date` DATE </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="88" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A88" s="34"/>
       <c r="B88" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C88" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D88" s="35" t="s">
         <v>9</v>
@@ -4347,149 +4378,149 @@
       <c r="G88" s="37"/>
       <c r="H88" s="38"/>
       <c r="I88" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`sales_date` DATE </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`delivery_date` DATE </v>
       </c>
       <c r="J88" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`sales_date` DATE </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`delivery_date` DATE </v>
       </c>
     </row>
     <row r="89" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A89" s="34"/>
       <c r="B89" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C89" s="35" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D89" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89" s="36">
-        <v>64</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E89" s="36"/>
       <c r="F89" s="35"/>
       <c r="G89" s="37"/>
       <c r="H89" s="38"/>
       <c r="I89" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`sales_date` DATE </v>
       </c>
       <c r="J89" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`sales_date` DATE </v>
       </c>
     </row>
     <row r="90" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A90" s="34"/>
       <c r="B90" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C90" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E90" s="36">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="F90" s="35"/>
       <c r="G90" s="37"/>
       <c r="H90" s="38"/>
       <c r="I90" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
       </c>
       <c r="J90" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
       </c>
     </row>
     <row r="91" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A91" s="34"/>
       <c r="B91" s="39" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C91" s="35" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="D91" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E91" s="36">
-        <v>20</v>
+        <v>256</v>
       </c>
       <c r="F91" s="35"/>
       <c r="G91" s="37"/>
       <c r="H91" s="38"/>
       <c r="I91" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
       </c>
       <c r="J91" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
       </c>
     </row>
     <row r="92" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A92" s="34"/>
       <c r="B92" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="D92" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E92" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F92" s="35"/>
       <c r="G92" s="37"/>
       <c r="H92" s="38"/>
       <c r="I92" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
       </c>
       <c r="J92" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
       </c>
     </row>
     <row r="93" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A93" s="34"/>
       <c r="B93" s="39" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="C93" s="35" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="D93" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E93" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E93" s="36">
+        <v>256</v>
+      </c>
       <c r="F93" s="35"/>
       <c r="G93" s="37"/>
       <c r="H93" s="38"/>
       <c r="I93" s="40" t="str">
-        <f t="shared" ref="I93:I94" si="16">"," &amp; IF(A93="","","/* ") &amp; "`" &amp; C93 &amp; "` " &amp; D93 &amp; IF(E93&gt;0,"(" &amp; E93 &amp; ") "," ") &amp; IF(F93&lt;&gt;"","NOT NULL ","") &amp; IF(G93="","","DEFAULT '" &amp; G93 &amp; "' ") &amp; IF(A93="",""," */")</f>
-        <v xml:space="preserve">,`quantity` INT </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
       <c r="J93" s="41" t="str">
-        <f t="shared" ref="J93:J94" si="17">"," &amp; IF(A93="","","/* ") &amp; "`" &amp; C93 &amp; "` " &amp; D93 &amp; IF(E93&gt;0,"(" &amp; E93 &amp; ") "," ") &amp; IF(F93&lt;&gt;"","NOT NULL ","") &amp; IF(G93="","","DEFAULT '" &amp; G93 &amp; "' ") &amp; IF(A93="",""," */")</f>
-        <v xml:space="preserve">,`quantity` INT </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="94" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A94" s="34"/>
       <c r="B94" s="39" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C94" s="35" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="D94" s="35" t="s">
         <v>5</v>
@@ -4499,100 +4530,100 @@
       <c r="G94" s="37"/>
       <c r="H94" s="38"/>
       <c r="I94" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="I94:I95" si="18">"," &amp; IF(A94="","","/* ") &amp; "`" &amp; C94 &amp; "` " &amp; D94 &amp; IF(E94&gt;0,"(" &amp; E94 &amp; ") "," ") &amp; IF(F94&lt;&gt;"","NOT NULL ","") &amp; IF(G94="","","DEFAULT '" &amp; G94 &amp; "' ") &amp; IF(A94="",""," */")</f>
+        <v xml:space="preserve">,`quantity` INT </v>
+      </c>
+      <c r="J94" s="41" t="str">
+        <f t="shared" ref="J94:J95" si="19">"," &amp; IF(A94="","","/* ") &amp; "`" &amp; C94 &amp; "` " &amp; D94 &amp; IF(E94&gt;0,"(" &amp; E94 &amp; ") "," ") &amp; IF(F94&lt;&gt;"","NOT NULL ","") &amp; IF(G94="","","DEFAULT '" &amp; G94 &amp; "' ") &amp; IF(A94="",""," */")</f>
+        <v xml:space="preserve">,`quantity` INT </v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A95" s="34"/>
+      <c r="B95" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="D95" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95" s="36"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="38"/>
+      <c r="I95" s="40" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">,`price` INT </v>
       </c>
-      <c r="J94" s="41" t="str">
-        <f t="shared" si="17"/>
+      <c r="J95" s="41" t="str">
+        <f t="shared" si="19"/>
         <v xml:space="preserve">,`price` INT </v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A95" s="2"/>
-      <c r="B95" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E95" s="7">
-        <v>256</v>
-      </c>
-      <c r="F95" s="6"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="9"/>
-      <c r="I95" s="27" t="str">
-        <f>"," &amp; IF(A95="","","/* ") &amp; "`" &amp; C95 &amp; "` " &amp; D95 &amp; IF(E95&gt;0,"(" &amp; E95 &amp; ") "," ") &amp; IF(F95&lt;&gt;"","NOT NULL ","") &amp; IF(G95="","","DEFAULT '" &amp; G95 &amp; "' ") &amp; IF(A95="",""," */")</f>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
-      </c>
-      <c r="J95" s="29" t="str">
-        <f>"," &amp; IF(A95="","","/* ") &amp; "`" &amp; C95 &amp; "` " &amp; D95 &amp; IF(E95&gt;0,"(" &amp; E95 &amp; ") "," ") &amp; IF(F95&lt;&gt;"","NOT NULL ","") &amp; IF(G95="","","DEFAULT '" &amp; G95 &amp; "' ") &amp; IF(A95="",""," */")</f>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" s="2"/>
       <c r="B96" s="20" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E96" s="7">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="8"/>
       <c r="H96" s="9"/>
       <c r="I96" s="27" t="str">
         <f>"," &amp; IF(A96="","","/* ") &amp; "`" &amp; C96 &amp; "` " &amp; D96 &amp; IF(E96&gt;0,"(" &amp; E96 &amp; ") "," ") &amp; IF(F96&lt;&gt;"","NOT NULL ","") &amp; IF(G96="","","DEFAULT '" &amp; G96 &amp; "' ") &amp; IF(A96="",""," */")</f>
-        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
       <c r="J96" s="29" t="str">
         <f>"," &amp; IF(A96="","","/* ") &amp; "`" &amp; C96 &amp; "` " &amp; D96 &amp; IF(E96&gt;0,"(" &amp; E96 &amp; ") "," ") &amp; IF(F96&lt;&gt;"","NOT NULL ","") &amp; IF(G96="","","DEFAULT '" &amp; G96 &amp; "' ") &amp; IF(A96="",""," */")</f>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A97" s="2"/>
+      <c r="B97" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="7">
+        <v>128</v>
+      </c>
+      <c r="F97" s="6"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="27" t="str">
+        <f>"," &amp; IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; IF(A97="",""," */")</f>
         <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
-    </row>
-    <row r="97" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="34"/>
-      <c r="B97" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C97" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="D97" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E97" s="36"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="37"/>
-      <c r="H97" s="38"/>
-      <c r="I97" s="40" t="str">
+      <c r="J97" s="29" t="str">
         <f>"," &amp; IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; IF(A97="",""," */")</f>
-        <v xml:space="preserve">,`product_detail` TEXT </v>
-      </c>
-      <c r="J97" s="41" t="str">
-        <f>"," &amp; IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; IF(A97="",""," */")</f>
-        <v xml:space="preserve">,`product_detail` TEXT </v>
+        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
     </row>
     <row r="98" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A98" s="34"/>
       <c r="B98" s="39" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C98" s="35" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D98" s="35" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E98" s="36"/>
       <c r="F98" s="35"/>
@@ -4600,46 +4631,44 @@
       <c r="H98" s="38"/>
       <c r="I98" s="40" t="str">
         <f>"," &amp; IF(A98="","","/* ") &amp; "`" &amp; C98 &amp; "` " &amp; D98 &amp; IF(E98&gt;0,"(" &amp; E98 &amp; ") "," ") &amp; IF(F98&lt;&gt;"","NOT NULL ","") &amp; IF(G98="","","DEFAULT '" &amp; G98 &amp; "' ") &amp; IF(A98="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`product_detail` TEXT </v>
       </c>
       <c r="J98" s="41" t="str">
         <f>"," &amp; IF(A98="","","/* ") &amp; "`" &amp; C98 &amp; "` " &amp; D98 &amp; IF(E98&gt;0,"(" &amp; E98 &amp; ") "," ") &amp; IF(F98&lt;&gt;"","NOT NULL ","") &amp; IF(G98="","","DEFAULT '" &amp; G98 &amp; "' ") &amp; IF(A98="",""," */")</f>
+        <v xml:space="preserve">,`product_detail` TEXT </v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A99" s="34"/>
+      <c r="B99" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C99" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D99" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E99" s="36"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="38"/>
+      <c r="I99" s="40" t="str">
+        <f>"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
         <v xml:space="preserve">,`status_id` INT </v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A99" s="2"/>
-      <c r="B99" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E99" s="7">
-        <v>256</v>
-      </c>
-      <c r="F99" s="6"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="27" t="str">
-        <f t="shared" ref="I99:I105" si="18">"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
-      </c>
-      <c r="J99" s="29" t="str">
-        <f t="shared" ref="J99:J105" si="19">"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+      <c r="J99" s="41" t="str">
+        <f>"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" s="2"/>
       <c r="B100" s="43" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>7</v>
@@ -4651,119 +4680,121 @@
       <c r="G100" s="8"/>
       <c r="H100" s="9"/>
       <c r="I100" s="27" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" ref="I100:I106" si="20">"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J100" s="29" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" ref="J100:J106" si="21">"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" s="2"/>
       <c r="B101" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E101" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="E101" s="7">
+        <v>256</v>
+      </c>
       <c r="F101" s="6"/>
       <c r="G101" s="8"/>
       <c r="H101" s="9"/>
       <c r="I101" s="27" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J101" s="29" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="2"/>
       <c r="B102" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E102" s="7">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E102" s="7"/>
       <c r="F102" s="6"/>
       <c r="G102" s="8"/>
       <c r="H102" s="9"/>
       <c r="I102" s="27" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+      <c r="J102" s="29" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A103" s="2"/>
+      <c r="B103" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" s="7">
+        <v>64</v>
+      </c>
+      <c r="F103" s="6"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="27" t="str">
+        <f t="shared" si="20"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
-      <c r="J102" s="29" t="str">
-        <f t="shared" si="19"/>
+      <c r="J103" s="29" t="str">
+        <f t="shared" si="21"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="34"/>
-      <c r="B103" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="C103" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D103" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E103" s="36"/>
-      <c r="F103" s="35"/>
-      <c r="G103" s="37"/>
-      <c r="H103" s="38"/>
-      <c r="I103" s="40" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-      <c r="J103" s="41" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="104" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A104" s="34"/>
       <c r="B104" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C104" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D104" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E104" s="36"/>
       <c r="F104" s="35"/>
       <c r="G104" s="37"/>
       <c r="H104" s="38"/>
       <c r="I104" s="40" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J104" s="41" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="105" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A105" s="34"/>
       <c r="B105" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C105" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D105" s="35" t="s">
         <v>8</v>
@@ -4773,144 +4804,144 @@
       <c r="G105" s="37"/>
       <c r="H105" s="38"/>
       <c r="I105" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+      <c r="J105" s="41" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A106" s="34"/>
+      <c r="B106" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C106" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D106" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="36"/>
+      <c r="F106" s="35"/>
+      <c r="G106" s="37"/>
+      <c r="H106" s="38"/>
+      <c r="I106" s="40" t="str">
+        <f t="shared" si="20"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-      <c r="J105" s="41" t="str">
-        <f t="shared" si="19"/>
+      <c r="J106" s="41" t="str">
+        <f t="shared" si="21"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A106" s="2"/>
-      <c r="B106" s="21"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="22"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="23"/>
-      <c r="H106" s="21"/>
-      <c r="I106" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J106" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A107" s="2"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="23"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J107" s="29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108" s="2"/>
-      <c r="B108" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C108" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D108" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F108" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G108" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H108" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I108" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C108 &amp; "` ("</f>
-        <v>CREATE TABLE `licenses` (</v>
-      </c>
-      <c r="J108" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C108 &amp; "` ("</f>
-        <v>CREATE TABLE `licenses` (</v>
-      </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" s="2"/>
-      <c r="B109" s="20" t="s">
+      <c r="B109" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C109" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D109" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F109" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G109" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H109" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I109" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C109 &amp; "` ("</f>
+        <v>CREATE TABLE `licenses` (</v>
+      </c>
+      <c r="J109" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C109 &amp; "` ("</f>
+        <v>CREATE TABLE `licenses` (</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A110" s="2"/>
+      <c r="B110" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="C110" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D109" s="6" t="s">
+      <c r="D110" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E109" s="7"/>
-      <c r="F109" s="6" t="s">
+      <c r="E110" s="7"/>
+      <c r="F110" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G109" s="8"/>
-      <c r="H109" s="9"/>
-      <c r="I109" s="28" t="s">
+      <c r="G110" s="8"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J109" s="30" t="s">
+      <c r="J110" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="34"/>
-      <c r="B110" s="39" t="s">
+    <row r="111" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A111" s="34"/>
+      <c r="B111" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C110" s="35" t="s">
+      <c r="C111" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D110" s="35" t="s">
+      <c r="D111" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E110" s="36"/>
-      <c r="F110" s="35"/>
-      <c r="G110" s="37"/>
-      <c r="H110" s="38"/>
-      <c r="I110" s="40" t="str">
-        <f>"," &amp; IF(A110="","","/* ") &amp; "`" &amp; C110 &amp; "` " &amp; D110 &amp; IF(E110&gt;0,"(" &amp; E110 &amp; ") "," ") &amp; IF(F110&lt;&gt;"","NOT NULL ","") &amp; IF(G110="","","DEFAULT '" &amp; G110 &amp; "' ") &amp; IF(A110="",""," */")</f>
+      <c r="E111" s="36"/>
+      <c r="F111" s="35"/>
+      <c r="G111" s="37"/>
+      <c r="H111" s="38"/>
+      <c r="I111" s="40" t="str">
+        <f>"," &amp; IF(A111="","","/* ") &amp; "`" &amp; C111 &amp; "` " &amp; D111 &amp; IF(E111&gt;0,"(" &amp; E111 &amp; ") "," ") &amp; IF(F111&lt;&gt;"","NOT NULL ","") &amp; IF(G111="","","DEFAULT '" &amp; G111 &amp; "' ") &amp; IF(A111="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT </v>
       </c>
-      <c r="J110" s="41" t="str">
-        <f>"," &amp; IF(A110="","","/* ") &amp; "`" &amp; C110 &amp; "` " &amp; D110 &amp; IF(E110&gt;0,"(" &amp; E110 &amp; ") "," ") &amp; IF(F110&lt;&gt;"","NOT NULL ","") &amp; IF(G110="","","DEFAULT '" &amp; G110 &amp; "' ") &amp; IF(A110="",""," */")</f>
+      <c r="J111" s="41" t="str">
+        <f>"," &amp; IF(A111="","","/* ") &amp; "`" &amp; C111 &amp; "` " &amp; D111 &amp; IF(E111&gt;0,"(" &amp; E111 &amp; ") "," ") &amp; IF(F111&lt;&gt;"","NOT NULL ","") &amp; IF(G111="","","DEFAULT '" &amp; G111 &amp; "' ") &amp; IF(A111="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT </v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A111" s="2"/>
-      <c r="B111" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E111" s="7"/>
-      <c r="F111" s="6"/>
-      <c r="G111" s="8"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="27" t="str">
-        <f>"," &amp; IF(A111="","","/* ") &amp; "`" &amp; C111 &amp; "` " &amp; D111 &amp; IF(E111&gt;0,"(" &amp; E111 &amp; ") "," ") &amp; IF(F111&lt;&gt;"","NOT NULL ","") &amp; IF(G111="","","DEFAULT '" &amp; G111 &amp; "' ") &amp; IF(A111="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
-      </c>
-      <c r="J111" s="29" t="str">
-        <f>"," &amp; IF(A111="","","/* ") &amp; "`" &amp; C111 &amp; "` " &amp; D111 &amp; IF(E111&gt;0,"(" &amp; E111 &amp; ") "," ") &amp; IF(F111&lt;&gt;"","NOT NULL ","") &amp; IF(G111="","","DEFAULT '" &amp; G111 &amp; "' ") &amp; IF(A111="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A112" s="2"/>
       <c r="B112" s="20" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>5</v>
@@ -4921,20 +4952,20 @@
       <c r="H112" s="9"/>
       <c r="I112" s="27" t="str">
         <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
       <c r="J112" s="29" t="str">
         <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A113" s="2"/>
       <c r="B113" s="20" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>5</v>
@@ -4945,220 +4976,220 @@
       <c r="H113" s="9"/>
       <c r="I113" s="27" t="str">
         <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
       <c r="J113" s="29" t="str">
         <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A114" s="2"/>
       <c r="B114" s="20" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E114" s="7"/>
       <c r="F114" s="6"/>
       <c r="G114" s="8"/>
       <c r="H114" s="9"/>
       <c r="I114" s="27" t="str">
-        <f t="shared" ref="I114:I120" si="20">"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
       <c r="J114" s="29" t="str">
-        <f t="shared" ref="J114:J120" si="21">"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A115" s="2"/>
       <c r="B115" s="20" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E115" s="7">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E115" s="7"/>
       <c r="F115" s="6"/>
       <c r="G115" s="8"/>
       <c r="H115" s="9"/>
       <c r="I115" s="27" t="str">
-        <f>"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
+        <f t="shared" ref="I115:I121" si="22">"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
+      </c>
+      <c r="J115" s="29" t="str">
+        <f t="shared" ref="J115:J121" si="23">"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A116" s="2"/>
+      <c r="B116" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" s="7">
+        <v>20</v>
+      </c>
+      <c r="F116" s="6"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="27" t="str">
+        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
         <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
-      <c r="J115" s="29" t="str">
-        <f>"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
+      <c r="J116" s="29" t="str">
+        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
         <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A116" s="34"/>
-      <c r="B116" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="C116" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D116" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E116" s="36">
-        <v>20</v>
-      </c>
-      <c r="F116" s="35"/>
-      <c r="G116" s="37"/>
-      <c r="H116" s="38"/>
-      <c r="I116" s="40" t="str">
-        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
-      </c>
-      <c r="J116" s="41" t="str">
-        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="117" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A117" s="34"/>
       <c r="B117" s="39" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="C117" s="35" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D117" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E117" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F117" s="35"/>
       <c r="G117" s="37"/>
       <c r="H117" s="38"/>
       <c r="I117" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+      </c>
+      <c r="J117" s="41" t="str">
+        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A118" s="34"/>
+      <c r="B118" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C118" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D118" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" s="36">
+        <v>256</v>
+      </c>
+      <c r="F118" s="35"/>
+      <c r="G118" s="37"/>
+      <c r="H118" s="38"/>
+      <c r="I118" s="40" t="str">
+        <f t="shared" si="22"/>
         <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
-      <c r="J117" s="41" t="str">
-        <f t="shared" si="21"/>
+      <c r="J118" s="41" t="str">
+        <f t="shared" si="23"/>
         <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A118" s="2"/>
-      <c r="B118" s="20" t="s">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A119" s="2"/>
+      <c r="B119" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C119" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D118" s="6" t="s">
+      <c r="D119" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E118" s="7">
+      <c r="E119" s="7">
         <v>256</v>
       </c>
-      <c r="F118" s="6"/>
-      <c r="G118" s="8"/>
-      <c r="H118" s="9"/>
-      <c r="I118" s="27" t="str">
-        <f t="shared" si="20"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="27" t="str">
+        <f t="shared" si="22"/>
         <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
-      <c r="J118" s="29" t="str">
-        <f t="shared" si="21"/>
+      <c r="J119" s="29" t="str">
+        <f t="shared" si="23"/>
         <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
     </row>
-    <row r="119" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A119" s="34"/>
-      <c r="B119" s="39" t="s">
+    <row r="120" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A120" s="34"/>
+      <c r="B120" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="C119" s="35" t="s">
+      <c r="C120" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="D119" s="35" t="s">
+      <c r="D120" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E119" s="36"/>
-      <c r="F119" s="35"/>
-      <c r="G119" s="37"/>
-      <c r="H119" s="38"/>
-      <c r="I119" s="40" t="str">
-        <f t="shared" ref="I119" si="22">"," &amp; IF(A119="","","/* ") &amp; "`" &amp; C119 &amp; "` " &amp; D119 &amp; IF(E119&gt;0,"(" &amp; E119 &amp; ") "," ") &amp; IF(F119&lt;&gt;"","NOT NULL ","") &amp; IF(G119="","","DEFAULT '" &amp; G119 &amp; "' ") &amp; IF(A119="",""," */")</f>
+      <c r="E120" s="36"/>
+      <c r="F120" s="35"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="38"/>
+      <c r="I120" s="40" t="str">
+        <f t="shared" ref="I120" si="24">"," &amp; IF(A120="","","/* ") &amp; "`" &amp; C120 &amp; "` " &amp; D120 &amp; IF(E120&gt;0,"(" &amp; E120 &amp; ") "," ") &amp; IF(F120&lt;&gt;"","NOT NULL ","") &amp; IF(G120="","","DEFAULT '" &amp; G120 &amp; "' ") &amp; IF(A120="",""," */")</f>
         <v xml:space="preserve">,`language_id` INT </v>
       </c>
-      <c r="J119" s="41" t="str">
-        <f t="shared" ref="J119" si="23">"," &amp; IF(A119="","","/* ") &amp; "`" &amp; C119 &amp; "` " &amp; D119 &amp; IF(E119&gt;0,"(" &amp; E119 &amp; ") "," ") &amp; IF(F119&lt;&gt;"","NOT NULL ","") &amp; IF(G119="","","DEFAULT '" &amp; G119 &amp; "' ") &amp; IF(A119="",""," */")</f>
+      <c r="J120" s="41" t="str">
+        <f t="shared" ref="J120" si="25">"," &amp; IF(A120="","","/* ") &amp; "`" &amp; C120 &amp; "` " &amp; D120 &amp; IF(E120&gt;0,"(" &amp; E120 &amp; ") "," ") &amp; IF(F120&lt;&gt;"","NOT NULL ","") &amp; IF(G120="","","DEFAULT '" &amp; G120 &amp; "' ") &amp; IF(A120="",""," */")</f>
         <v xml:space="preserve">,`language_id` INT </v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A120" s="2"/>
-      <c r="B120" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E120" s="7"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="8"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="27" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
-      </c>
-      <c r="J120" s="29" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A121" s="2"/>
       <c r="B121" s="20" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E121" s="7"/>
       <c r="F121" s="6"/>
       <c r="G121" s="8"/>
       <c r="H121" s="9"/>
       <c r="I121" s="27" t="str">
-        <f t="shared" ref="I121" si="24">"," &amp; IF(A121="","","/* ") &amp; "`" &amp; C121 &amp; "` " &amp; D121 &amp; IF(E121&gt;0,"(" &amp; E121 &amp; ") "," ") &amp; IF(F121&lt;&gt;"","NOT NULL ","") &amp; IF(G121="","","DEFAULT '" &amp; G121 &amp; "' ") &amp; IF(A121="",""," */")</f>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
       <c r="J121" s="29" t="str">
-        <f t="shared" ref="J121" si="25">"," &amp; IF(A121="","","/* ") &amp; "`" &amp; C121 &amp; "` " &amp; D121 &amp; IF(E121&gt;0,"(" &amp; E121 &amp; ") "," ") &amp; IF(F121&lt;&gt;"","NOT NULL ","") &amp; IF(G121="","","DEFAULT '" &amp; G121 &amp; "' ") &amp; IF(A121="",""," */")</f>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A122" s="2"/>
       <c r="B122" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>9</v>
@@ -5168,97 +5199,95 @@
       <c r="G122" s="8"/>
       <c r="H122" s="9"/>
       <c r="I122" s="27" t="str">
-        <f>"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
+        <f t="shared" ref="I122" si="26">"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
+        <v xml:space="preserve">,`startdate` DATE </v>
+      </c>
+      <c r="J122" s="29" t="str">
+        <f t="shared" ref="J122" si="27">"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
+        <v xml:space="preserve">,`startdate` DATE </v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A123" s="2"/>
+      <c r="B123" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="7"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="27" t="str">
+        <f>"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
         <v xml:space="preserve">,`enddate` DATE </v>
       </c>
-      <c r="J122" s="29" t="str">
-        <f>"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
+      <c r="J123" s="29" t="str">
+        <f>"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
         <v xml:space="preserve">,`enddate` DATE </v>
       </c>
     </row>
-    <row r="123" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A123" s="34"/>
-      <c r="B123" s="39" t="s">
+    <row r="124" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A124" s="34"/>
+      <c r="B124" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="C123" s="35" t="s">
+      <c r="C124" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="D123" s="35" t="s">
+      <c r="D124" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E123" s="36">
+      <c r="E124" s="36">
         <v>256</v>
       </c>
-      <c r="F123" s="35"/>
-      <c r="G123" s="37"/>
-      <c r="H123" s="38"/>
-      <c r="I123" s="40" t="str">
-        <f t="shared" ref="I123" si="26">"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
+      <c r="F124" s="35"/>
+      <c r="G124" s="37"/>
+      <c r="H124" s="38"/>
+      <c r="I124" s="40" t="str">
+        <f t="shared" ref="I124" si="28">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
         <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
-      <c r="J123" s="41" t="str">
-        <f t="shared" ref="J123" si="27">"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
+      <c r="J124" s="41" t="str">
+        <f t="shared" ref="J124" si="29">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
         <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A124" s="2"/>
-      <c r="B124" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D124" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E124" s="7"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="8"/>
-      <c r="H124" s="9"/>
-      <c r="I124" s="27" t="str">
-        <f t="shared" ref="I124:I131" si="28">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
-        <v xml:space="preserve">,`notice` TEXT </v>
-      </c>
-      <c r="J124" s="29" t="str">
-        <f t="shared" ref="J124:J131" si="29">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
-        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A125" s="2"/>
-      <c r="B125" s="43" t="s">
-        <v>87</v>
+      <c r="B125" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E125" s="7">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E125" s="7"/>
       <c r="F125" s="6"/>
       <c r="G125" s="8"/>
       <c r="H125" s="9"/>
       <c r="I125" s="27" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" ref="I125:I132" si="30">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
       <c r="J125" s="29" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" ref="J125:J132" si="31">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A126" s="2"/>
       <c r="B126" s="43" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>7</v>
@@ -5270,119 +5299,121 @@
       <c r="G126" s="8"/>
       <c r="H126" s="9"/>
       <c r="I126" s="27" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J126" s="29" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A127" s="2"/>
       <c r="B127" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E127" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="E127" s="7">
+        <v>256</v>
+      </c>
       <c r="F127" s="6"/>
       <c r="G127" s="8"/>
       <c r="H127" s="9"/>
       <c r="I127" s="27" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J127" s="29" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A128" s="2"/>
       <c r="B128" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E128" s="7">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E128" s="7"/>
       <c r="F128" s="6"/>
       <c r="G128" s="8"/>
       <c r="H128" s="9"/>
       <c r="I128" s="27" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+      <c r="J128" s="29" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A129" s="2"/>
+      <c r="B129" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" s="7">
+        <v>64</v>
+      </c>
+      <c r="F129" s="6"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="9"/>
+      <c r="I129" s="27" t="str">
+        <f t="shared" si="30"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
-      <c r="J128" s="29" t="str">
-        <f t="shared" si="29"/>
+      <c r="J129" s="29" t="str">
+        <f t="shared" si="31"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
-    <row r="129" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A129" s="34"/>
-      <c r="B129" s="43" t="s">
+    <row r="130" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A130" s="34"/>
+      <c r="B130" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="C129" s="35" t="s">
+      <c r="C130" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="D129" s="35" t="s">
+      <c r="D130" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="E129" s="36"/>
-      <c r="F129" s="35"/>
-      <c r="G129" s="37"/>
-      <c r="H129" s="38"/>
-      <c r="I129" s="40" t="str">
-        <f t="shared" si="28"/>
+      <c r="E130" s="36"/>
+      <c r="F130" s="35"/>
+      <c r="G130" s="37"/>
+      <c r="H130" s="38"/>
+      <c r="I130" s="40" t="str">
+        <f t="shared" si="30"/>
         <v xml:space="preserve">,`user_id` INT </v>
       </c>
-      <c r="J129" s="41" t="str">
-        <f t="shared" si="29"/>
+      <c r="J130" s="41" t="str">
+        <f t="shared" si="31"/>
         <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A130" s="2"/>
-      <c r="B130" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E130" s="7"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="8"/>
-      <c r="H130" s="9"/>
-      <c r="I130" s="27" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
-      </c>
-      <c r="J130" s="29" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131" s="2"/>
       <c r="B131" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>8</v>
@@ -5392,120 +5423,120 @@
       <c r="G131" s="8"/>
       <c r="H131" s="9"/>
       <c r="I131" s="27" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J131" s="29" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" s="2"/>
-      <c r="B132" s="21"/>
-      <c r="C132" s="21"/>
-      <c r="D132" s="21"/>
-      <c r="E132" s="22"/>
-      <c r="F132" s="21"/>
-      <c r="G132" s="23"/>
-      <c r="H132" s="21"/>
-      <c r="I132" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J132" s="29" t="s">
-        <v>33</v>
+      <c r="B132" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" s="7"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="27" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
+      </c>
+      <c r="J132" s="29" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" s="2"/>
+      <c r="B133" s="21"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="22"/>
+      <c r="F133" s="21"/>
+      <c r="G133" s="23"/>
+      <c r="H133" s="21"/>
+      <c r="I133" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J133" s="29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" s="2"/>
-      <c r="B134" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C134" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D134" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E134" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F134" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G134" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H134" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I134" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C134 &amp; "` ("</f>
-        <v>CREATE TABLE `licensehistories` (</v>
-      </c>
-      <c r="J134" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C134 &amp; "` ("</f>
-        <v>CREATE TABLE `licensehistories` (</v>
-      </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" s="2"/>
-      <c r="B135" s="20" t="s">
+      <c r="B135" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C135" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D135" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E135" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F135" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G135" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H135" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I135" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C135 &amp; "` ("</f>
+        <v>CREATE TABLE `licensehistories` (</v>
+      </c>
+      <c r="J135" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C135 &amp; "` ("</f>
+        <v>CREATE TABLE `licensehistories` (</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A136" s="2"/>
+      <c r="B136" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C135" s="6" t="s">
+      <c r="C136" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D135" s="6" t="s">
+      <c r="D136" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E135" s="7"/>
-      <c r="F135" s="6" t="s">
+      <c r="E136" s="7"/>
+      <c r="F136" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G135" s="8"/>
-      <c r="H135" s="9"/>
-      <c r="I135" s="28" t="s">
+      <c r="G136" s="8"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J135" s="30" t="s">
+      <c r="J136" s="30" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A136" s="34"/>
-      <c r="B136" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C136" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D136" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E136" s="36"/>
-      <c r="F136" s="35"/>
-      <c r="G136" s="37"/>
-      <c r="H136" s="38"/>
-      <c r="I136" s="40" t="str">
-        <f>"," &amp; IF(A136="","","/* ") &amp; "`" &amp; C136 &amp; "` " &amp; D136 &amp; IF(E136&gt;0,"(" &amp; E136 &amp; ") "," ") &amp; IF(F136&lt;&gt;"","NOT NULL ","") &amp; IF(G136="","","DEFAULT '" &amp; G136 &amp; "' ") &amp; IF(A136="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT </v>
-      </c>
-      <c r="J136" s="41" t="str">
-        <f>"," &amp; IF(A136="","","/* ") &amp; "`" &amp; C136 &amp; "` " &amp; D136 &amp; IF(E136&gt;0,"(" &amp; E136 &amp; ") "," ") &amp; IF(F136&lt;&gt;"","NOT NULL ","") &amp; IF(G136="","","DEFAULT '" &amp; G136 &amp; "' ") &amp; IF(A136="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT </v>
       </c>
     </row>
     <row r="137" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A137" s="34"/>
       <c r="B137" s="39" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C137" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D137" s="35" t="s">
         <v>5</v>
@@ -5516,20 +5547,20 @@
       <c r="H137" s="38"/>
       <c r="I137" s="40" t="str">
         <f>"," &amp; IF(A137="","","/* ") &amp; "`" &amp; C137 &amp; "` " &amp; D137 &amp; IF(E137&gt;0,"(" &amp; E137 &amp; ") "," ") &amp; IF(F137&lt;&gt;"","NOT NULL ","") &amp; IF(G137="","","DEFAULT '" &amp; G137 &amp; "' ") &amp; IF(A137="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <v xml:space="preserve">,`client_id` INT </v>
       </c>
       <c r="J137" s="41" t="str">
         <f>"," &amp; IF(A137="","","/* ") &amp; "`" &amp; C137 &amp; "` " &amp; D137 &amp; IF(E137&gt;0,"(" &amp; E137 &amp; ") "," ") &amp; IF(F137&lt;&gt;"","NOT NULL ","") &amp; IF(G137="","","DEFAULT '" &amp; G137 &amp; "' ") &amp; IF(A137="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <v xml:space="preserve">,`client_id` INT </v>
       </c>
     </row>
     <row r="138" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A138" s="34"/>
       <c r="B138" s="39" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C138" s="35" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D138" s="35" t="s">
         <v>5</v>
@@ -5540,20 +5571,20 @@
       <c r="H138" s="38"/>
       <c r="I138" s="40" t="str">
         <f>"," &amp; IF(A138="","","/* ") &amp; "`" &amp; C138 &amp; "` " &amp; D138 &amp; IF(E138&gt;0,"(" &amp; E138 &amp; ") "," ") &amp; IF(F138&lt;&gt;"","NOT NULL ","") &amp; IF(G138="","","DEFAULT '" &amp; G138 &amp; "' ") &amp; IF(A138="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
       <c r="J138" s="41" t="str">
         <f>"," &amp; IF(A138="","","/* ") &amp; "`" &amp; C138 &amp; "` " &amp; D138 &amp; IF(E138&gt;0,"(" &amp; E138 &amp; ") "," ") &amp; IF(F138&lt;&gt;"","NOT NULL ","") &amp; IF(G138="","","DEFAULT '" &amp; G138 &amp; "' ") &amp; IF(A138="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="139" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A139" s="34"/>
       <c r="B139" s="39" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C139" s="35" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D139" s="35" t="s">
         <v>5</v>
@@ -5564,70 +5595,68 @@
       <c r="H139" s="38"/>
       <c r="I139" s="40" t="str">
         <f>"," &amp; IF(A139="","","/* ") &amp; "`" &amp; C139 &amp; "` " &amp; D139 &amp; IF(E139&gt;0,"(" &amp; E139 &amp; ") "," ") &amp; IF(F139&lt;&gt;"","NOT NULL ","") &amp; IF(G139="","","DEFAULT '" &amp; G139 &amp; "' ") &amp; IF(A139="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
       <c r="J139" s="41" t="str">
         <f>"," &amp; IF(A139="","","/* ") &amp; "`" &amp; C139 &amp; "` " &amp; D139 &amp; IF(E139&gt;0,"(" &amp; E139 &amp; ") "," ") &amp; IF(F139&lt;&gt;"","NOT NULL ","") &amp; IF(G139="","","DEFAULT '" &amp; G139 &amp; "' ") &amp; IF(A139="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
     </row>
     <row r="140" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A140" s="34"/>
       <c r="B140" s="39" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C140" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D140" s="35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E140" s="36"/>
       <c r="F140" s="35"/>
       <c r="G140" s="37"/>
       <c r="H140" s="38"/>
       <c r="I140" s="40" t="str">
-        <f t="shared" ref="I140" si="30">"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
       <c r="J140" s="41" t="str">
-        <f t="shared" ref="J140" si="31">"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="141" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A141" s="34"/>
       <c r="B141" s="39" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C141" s="35" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D141" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E141" s="36">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E141" s="36"/>
       <c r="F141" s="35"/>
       <c r="G141" s="37"/>
       <c r="H141" s="38"/>
       <c r="I141" s="40" t="str">
-        <f>"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
-        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
+        <f t="shared" ref="I141" si="32">"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
       </c>
       <c r="J141" s="41" t="str">
-        <f>"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
-        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
+        <f t="shared" ref="J141" si="33">"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
       </c>
     </row>
     <row r="142" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A142" s="34"/>
       <c r="B142" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C142" s="35" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="D142" s="35" t="s">
         <v>7</v>
@@ -5640,46 +5669,46 @@
       <c r="H142" s="38"/>
       <c r="I142" s="40" t="str">
         <f>"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
       <c r="J142" s="41" t="str">
         <f>"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="143" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A143" s="34"/>
       <c r="B143" s="39" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="C143" s="35" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D143" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E143" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F143" s="35"/>
       <c r="G143" s="37"/>
       <c r="H143" s="38"/>
       <c r="I143" s="40" t="str">
-        <f t="shared" ref="I143:I147" si="32">"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f>"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
       <c r="J143" s="41" t="str">
-        <f t="shared" ref="J143:J147" si="33">"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f>"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="144" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A144" s="34"/>
       <c r="B144" s="39" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="C144" s="35" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="D144" s="35" t="s">
         <v>7</v>
@@ -5691,93 +5720,95 @@
       <c r="G144" s="37"/>
       <c r="H144" s="38"/>
       <c r="I144" s="40" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
+        <f t="shared" ref="I144:I148" si="34">"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
       <c r="J144" s="41" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
+        <f t="shared" ref="J144:J148" si="35">"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="145" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A145" s="34"/>
       <c r="B145" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C145" s="35" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="D145" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E145" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E145" s="36">
+        <v>256</v>
+      </c>
       <c r="F145" s="35"/>
       <c r="G145" s="37"/>
       <c r="H145" s="38"/>
       <c r="I145" s="40" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">,`language_id` INT </v>
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
       <c r="J145" s="41" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve">,`language_id` INT </v>
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="146" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A146" s="34"/>
       <c r="B146" s="39" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="C146" s="35" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="D146" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E146" s="36"/>
       <c r="F146" s="35"/>
       <c r="G146" s="37"/>
       <c r="H146" s="38"/>
       <c r="I146" s="40" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">,`language_id` INT </v>
       </c>
       <c r="J146" s="41" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">,`language_id` INT </v>
       </c>
     </row>
     <row r="147" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A147" s="34"/>
       <c r="B147" s="39" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C147" s="35" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D147" s="35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E147" s="36"/>
       <c r="F147" s="35"/>
       <c r="G147" s="37"/>
       <c r="H147" s="38"/>
       <c r="I147" s="40" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
       <c r="J147" s="41" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="148" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A148" s="34"/>
       <c r="B148" s="39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C148" s="35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D148" s="35" t="s">
         <v>9</v>
@@ -5787,97 +5818,95 @@
       <c r="G148" s="37"/>
       <c r="H148" s="38"/>
       <c r="I148" s="40" t="str">
-        <f>"," &amp; IF(A148="","","/* ") &amp; "`" &amp; C148 &amp; "` " &amp; D148 &amp; IF(E148&gt;0,"(" &amp; E148 &amp; ") "," ") &amp; IF(F148&lt;&gt;"","NOT NULL ","") &amp; IF(G148="","","DEFAULT '" &amp; G148 &amp; "' ") &amp; IF(A148="",""," */")</f>
-        <v xml:space="preserve">,`enddate` DATE </v>
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">,`startdate` DATE </v>
       </c>
       <c r="J148" s="41" t="str">
-        <f>"," &amp; IF(A148="","","/* ") &amp; "`" &amp; C148 &amp; "` " &amp; D148 &amp; IF(E148&gt;0,"(" &amp; E148 &amp; ") "," ") &amp; IF(F148&lt;&gt;"","NOT NULL ","") &amp; IF(G148="","","DEFAULT '" &amp; G148 &amp; "' ") &amp; IF(A148="",""," */")</f>
-        <v xml:space="preserve">,`enddate` DATE </v>
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">,`startdate` DATE </v>
       </c>
     </row>
     <row r="149" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A149" s="34"/>
       <c r="B149" s="39" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="C149" s="35" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="D149" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E149" s="36">
-        <v>256</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E149" s="36"/>
       <c r="F149" s="35"/>
       <c r="G149" s="37"/>
       <c r="H149" s="38"/>
       <c r="I149" s="40" t="str">
-        <f t="shared" ref="I149:I157" si="34">"," &amp; IF(A149="","","/* ") &amp; "`" &amp; C149 &amp; "` " &amp; D149 &amp; IF(E149&gt;0,"(" &amp; E149 &amp; ") "," ") &amp; IF(F149&lt;&gt;"","NOT NULL ","") &amp; IF(G149="","","DEFAULT '" &amp; G149 &amp; "' ") &amp; IF(A149="",""," */")</f>
-        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
+        <f>"," &amp; IF(A149="","","/* ") &amp; "`" &amp; C149 &amp; "` " &amp; D149 &amp; IF(E149&gt;0,"(" &amp; E149 &amp; ") "," ") &amp; IF(F149&lt;&gt;"","NOT NULL ","") &amp; IF(G149="","","DEFAULT '" &amp; G149 &amp; "' ") &amp; IF(A149="",""," */")</f>
+        <v xml:space="preserve">,`enddate` DATE </v>
       </c>
       <c r="J149" s="41" t="str">
-        <f t="shared" ref="J149:J157" si="35">"," &amp; IF(A149="","","/* ") &amp; "`" &amp; C149 &amp; "` " &amp; D149 &amp; IF(E149&gt;0,"(" &amp; E149 &amp; ") "," ") &amp; IF(F149&lt;&gt;"","NOT NULL ","") &amp; IF(G149="","","DEFAULT '" &amp; G149 &amp; "' ") &amp; IF(A149="",""," */")</f>
-        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
+        <f>"," &amp; IF(A149="","","/* ") &amp; "`" &amp; C149 &amp; "` " &amp; D149 &amp; IF(E149&gt;0,"(" &amp; E149 &amp; ") "," ") &amp; IF(F149&lt;&gt;"","NOT NULL ","") &amp; IF(G149="","","DEFAULT '" &amp; G149 &amp; "' ") &amp; IF(A149="",""," */")</f>
+        <v xml:space="preserve">,`enddate` DATE </v>
       </c>
     </row>
     <row r="150" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A150" s="34"/>
       <c r="B150" s="39" t="s">
-        <v>29</v>
+        <v>153</v>
       </c>
       <c r="C150" s="35" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="D150" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E150" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E150" s="36">
+        <v>256</v>
+      </c>
       <c r="F150" s="35"/>
       <c r="G150" s="37"/>
       <c r="H150" s="38"/>
       <c r="I150" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`notice` TEXT </v>
+        <f t="shared" ref="I150:I158" si="36">"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
+        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
       <c r="J150" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`notice` TEXT </v>
+        <f t="shared" ref="J150:J158" si="37">"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
+        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
     </row>
     <row r="151" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A151" s="34"/>
-      <c r="B151" s="43" t="s">
-        <v>87</v>
+      <c r="B151" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="C151" s="35" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="D151" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E151" s="36">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E151" s="36"/>
       <c r="F151" s="35"/>
       <c r="G151" s="37"/>
       <c r="H151" s="38"/>
       <c r="I151" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
       <c r="J151" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="152" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A152" s="34"/>
       <c r="B152" s="43" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C152" s="35" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="D152" s="35" t="s">
         <v>7</v>
@@ -5889,119 +5918,121 @@
       <c r="G152" s="37"/>
       <c r="H152" s="38"/>
       <c r="I152" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J152" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="153" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A153" s="34"/>
       <c r="B153" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C153" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D153" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E153" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E153" s="36">
+        <v>256</v>
+      </c>
       <c r="F153" s="35"/>
       <c r="G153" s="37"/>
       <c r="H153" s="38"/>
       <c r="I153" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J153" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="154" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A154" s="34"/>
       <c r="B154" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C154" s="35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D154" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E154" s="36">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E154" s="36"/>
       <c r="F154" s="35"/>
       <c r="G154" s="37"/>
       <c r="H154" s="38"/>
       <c r="I154" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
       <c r="J154" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
     </row>
     <row r="155" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A155" s="34"/>
       <c r="B155" s="43" t="s">
-        <v>161</v>
+        <v>52</v>
       </c>
       <c r="C155" s="35" t="s">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="D155" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E155" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E155" s="36">
+        <v>64</v>
+      </c>
       <c r="F155" s="35"/>
       <c r="G155" s="37"/>
       <c r="H155" s="38"/>
       <c r="I155" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
       <c r="J155" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
     <row r="156" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A156" s="34"/>
       <c r="B156" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C156" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D156" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E156" s="36"/>
       <c r="F156" s="35"/>
       <c r="G156" s="37"/>
       <c r="H156" s="38"/>
       <c r="I156" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J156" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="157" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A157" s="34"/>
       <c r="B157" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C157" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D157" s="35" t="s">
         <v>8</v>
@@ -6011,404 +6042,433 @@
       <c r="G157" s="37"/>
       <c r="H157" s="38"/>
       <c r="I157" s="40" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+      <c r="J157" s="41" t="str">
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A158" s="34"/>
+      <c r="B158" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C158" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D158" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" s="36"/>
+      <c r="F158" s="35"/>
+      <c r="G158" s="37"/>
+      <c r="H158" s="38"/>
+      <c r="I158" s="40" t="str">
+        <f t="shared" si="36"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-      <c r="J157" s="41" t="str">
-        <f t="shared" si="35"/>
+      <c r="J158" s="41" t="str">
+        <f t="shared" si="37"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A158" s="2"/>
-      <c r="B158" s="21"/>
-      <c r="C158" s="21"/>
-      <c r="D158" s="21"/>
-      <c r="E158" s="22"/>
-      <c r="F158" s="21"/>
-      <c r="G158" s="23"/>
-      <c r="H158" s="21"/>
-      <c r="I158" s="28" t="s">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A159" s="2"/>
+      <c r="B159" s="21"/>
+      <c r="C159" s="21"/>
+      <c r="D159" s="21"/>
+      <c r="E159" s="22"/>
+      <c r="F159" s="21"/>
+      <c r="G159" s="23"/>
+      <c r="H159" s="21"/>
+      <c r="I159" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J158" s="29" t="s">
+      <c r="J159" s="29" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="expression" dxfId="73" priority="186">
+    <cfRule type="expression" dxfId="75" priority="187">
       <formula>A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A7 A41:A42 A132:A133 A78:A80 A121:A122 A13:A14 A82:A92 A96:A97 A31:A33 A35 A106:A109 A115:A116">
-    <cfRule type="cellIs" dxfId="72" priority="185" operator="greaterThan">
+  <conditionalFormatting sqref="A5:A7 A41:A42 A133:A134 A79:A81 A122:A123 A13:A14 A83:A93 A97:A98 A31:A33 A35 A107:A110 A116:A117">
+    <cfRule type="cellIs" dxfId="74" priority="186" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A11:A12">
-    <cfRule type="cellIs" dxfId="71" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="185" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="cellIs" dxfId="70" priority="183" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="184" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="69" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="183" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:A38">
-    <cfRule type="cellIs" dxfId="68" priority="178" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99:A102">
-    <cfRule type="cellIs" dxfId="67" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="179" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100:A103">
+    <cfRule type="cellIs" dxfId="69" priority="177" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A125">
+    <cfRule type="cellIs" dxfId="68" priority="176" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="cellIs" dxfId="67" priority="170" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="cellIs" dxfId="66" priority="168" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:A62 A43:A44 A46">
+    <cfRule type="cellIs" dxfId="65" priority="169" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52 A54">
+    <cfRule type="cellIs" dxfId="64" priority="163" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55 A57">
+    <cfRule type="cellIs" dxfId="63" priority="162" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="cellIs" dxfId="62" priority="161" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="cellIs" dxfId="61" priority="160" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="cellIs" dxfId="60" priority="159" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="cellIs" dxfId="59" priority="158" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A121">
+    <cfRule type="cellIs" dxfId="58" priority="155" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A119">
+    <cfRule type="cellIs" dxfId="57" priority="154" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A126:A129">
+    <cfRule type="cellIs" dxfId="56" priority="153" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A131:A132">
+    <cfRule type="cellIs" dxfId="55" priority="152" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A159 A135">
+    <cfRule type="cellIs" dxfId="54" priority="151" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115">
+    <cfRule type="cellIs" dxfId="53" priority="145" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="cellIs" dxfId="52" priority="137" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="cellIs" dxfId="51" priority="136" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A112">
+    <cfRule type="cellIs" dxfId="50" priority="135" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A113">
+    <cfRule type="cellIs" dxfId="49" priority="134" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:A20 A15:A17">
+    <cfRule type="cellIs" dxfId="48" priority="123" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="cellIs" dxfId="47" priority="119" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="cellIs" dxfId="46" priority="97" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
+    <cfRule type="cellIs" dxfId="45" priority="118" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A136">
+    <cfRule type="cellIs" dxfId="44" priority="107" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="cellIs" dxfId="43" priority="89" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" dxfId="42" priority="96" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="cellIs" dxfId="41" priority="95" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="cellIs" dxfId="40" priority="94" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="cellIs" dxfId="39" priority="93" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A118">
+    <cfRule type="cellIs" dxfId="38" priority="92" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A120">
+    <cfRule type="cellIs" dxfId="37" priority="91" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A124">
-    <cfRule type="cellIs" dxfId="66" priority="175" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="cellIs" dxfId="65" priority="169" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="64" priority="167" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:A62 A43:A44 A46">
-    <cfRule type="cellIs" dxfId="63" priority="168" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52 A54">
-    <cfRule type="cellIs" dxfId="62" priority="162" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55 A57">
-    <cfRule type="cellIs" dxfId="61" priority="161" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="60" priority="160" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="cellIs" dxfId="59" priority="159" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="cellIs" dxfId="58" priority="158" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="cellIs" dxfId="57" priority="157" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A120">
-    <cfRule type="cellIs" dxfId="56" priority="154" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A118">
-    <cfRule type="cellIs" dxfId="55" priority="153" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A125:A128">
-    <cfRule type="cellIs" dxfId="54" priority="152" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A130:A131">
-    <cfRule type="cellIs" dxfId="53" priority="151" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A158 A134">
-    <cfRule type="cellIs" dxfId="52" priority="150" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A114">
-    <cfRule type="cellIs" dxfId="51" priority="144" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="cellIs" dxfId="50" priority="136" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="cellIs" dxfId="49" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="90" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111">
-    <cfRule type="cellIs" dxfId="48" priority="134" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A112">
-    <cfRule type="cellIs" dxfId="47" priority="133" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:A20 A15:A17">
-    <cfRule type="cellIs" dxfId="46" priority="122" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="cellIs" dxfId="45" priority="118" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="cellIs" dxfId="44" priority="96" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A113">
-    <cfRule type="cellIs" dxfId="43" priority="117" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A135">
-    <cfRule type="cellIs" dxfId="42" priority="106" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="41" priority="88" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="cellIs" dxfId="40" priority="95" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="cellIs" dxfId="39" priority="94" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="cellIs" dxfId="38" priority="93" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="cellIs" dxfId="37" priority="92" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A117">
-    <cfRule type="cellIs" dxfId="36" priority="91" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A119">
-    <cfRule type="cellIs" dxfId="35" priority="90" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A123">
-    <cfRule type="cellIs" dxfId="34" priority="89" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A110">
-    <cfRule type="cellIs" dxfId="33" priority="74" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A136">
-    <cfRule type="cellIs" dxfId="32" priority="44" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A147:A148 A141:A142">
-    <cfRule type="cellIs" dxfId="31" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="75" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A137">
+    <cfRule type="cellIs" dxfId="34" priority="45" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A148:A149 A142:A143">
+    <cfRule type="cellIs" dxfId="33" priority="58" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A151">
+    <cfRule type="cellIs" dxfId="32" priority="57" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A147">
+    <cfRule type="cellIs" dxfId="31" priority="56" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A145">
+    <cfRule type="cellIs" dxfId="30" priority="55" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A152:A155">
+    <cfRule type="cellIs" dxfId="29" priority="54" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A157:A158">
+    <cfRule type="cellIs" dxfId="28" priority="53" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A141">
+    <cfRule type="cellIs" dxfId="27" priority="52" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A138">
+    <cfRule type="cellIs" dxfId="26" priority="51" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A139">
+    <cfRule type="cellIs" dxfId="25" priority="50" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A140">
+    <cfRule type="cellIs" dxfId="24" priority="49" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A144">
+    <cfRule type="cellIs" dxfId="23" priority="48" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A146">
+    <cfRule type="cellIs" dxfId="22" priority="47" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150">
-    <cfRule type="cellIs" dxfId="30" priority="56" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A146">
-    <cfRule type="cellIs" dxfId="29" priority="55" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A144">
-    <cfRule type="cellIs" dxfId="28" priority="54" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A151:A154">
-    <cfRule type="cellIs" dxfId="27" priority="53" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A156:A157">
-    <cfRule type="cellIs" dxfId="26" priority="52" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A140">
-    <cfRule type="cellIs" dxfId="25" priority="51" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A137">
-    <cfRule type="cellIs" dxfId="24" priority="50" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A138">
-    <cfRule type="cellIs" dxfId="23" priority="49" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A139">
-    <cfRule type="cellIs" dxfId="22" priority="48" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A143">
-    <cfRule type="cellIs" dxfId="21" priority="47" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A145">
-    <cfRule type="cellIs" dxfId="20" priority="46" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A149">
-    <cfRule type="cellIs" dxfId="19" priority="45" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="cellIs" dxfId="18" priority="25" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76:A77 A63:A64 A67">
-    <cfRule type="cellIs" dxfId="17" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="46" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77:A78 A63:A64 A68">
+    <cfRule type="cellIs" dxfId="19" priority="44" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A25 A21:A22">
-    <cfRule type="cellIs" dxfId="16" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="cellIs" dxfId="16" priority="36" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:A73">
     <cfRule type="cellIs" dxfId="15" priority="21" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" dxfId="14" priority="35" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69:A72">
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="greaterThan">
+  <conditionalFormatting sqref="A69">
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="cellIs" dxfId="11" priority="32" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104:A105">
-    <cfRule type="cellIs" dxfId="10" priority="31" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A74:A75">
-    <cfRule type="cellIs" dxfId="9" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="33" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105:A106">
+    <cfRule type="cellIs" dxfId="12" priority="32" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75:A76">
+    <cfRule type="cellIs" dxfId="11" priority="31" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:A60">
-    <cfRule type="cellIs" dxfId="8" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="30" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A40">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="29" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="cellIs" dxfId="6" priority="27" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A155">
-    <cfRule type="cellIs" dxfId="4" priority="23" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A129">
-    <cfRule type="cellIs" dxfId="3" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="28" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="cellIs" dxfId="7" priority="27" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A156">
+    <cfRule type="cellIs" dxfId="6" priority="24" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A130">
+    <cfRule type="cellIs" dxfId="5" priority="25" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:A30 A26:A27">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D12 D16:D18 D32:D40 D44:D60 D135:D157 D109:D131 D22:D23 D64:D75 D27:D28 D79:D105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D12 D16:D18 D32:D40 D44:D60 D136:D158 D110:D132 D22:D23 D80:D106 D27:D28 D64:D76">
       <formula1>TYPE</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
different associations for the clientstable
</commit_message>
<xml_diff>
--- a/document/sql_creator.xlsx
+++ b/document/sql_creator.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="178">
   <si>
     <t>属性</t>
     <rPh sb="0" eb="2">
@@ -949,6 +949,17 @@
   </si>
   <si>
     <t>contract_date</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>partner_id</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>パートナー区分</t>
+    <rPh sb="5" eb="7">
+      <t>クブン</t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -2368,10 +2379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J159"/>
+  <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -3124,7 +3135,7 @@
     <row r="36" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="34"/>
       <c r="B36" s="39" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="C36" s="35" t="s">
         <v>157</v>
@@ -3134,75 +3145,77 @@
       </c>
       <c r="E36" s="36"/>
       <c r="F36" s="35"/>
-      <c r="G36" s="37"/>
+      <c r="G36" s="37">
+        <v>0</v>
+      </c>
       <c r="H36" s="38"/>
       <c r="I36" s="40" t="str">
         <f>"," &amp; IF(A36="","","/* ") &amp; "`" &amp; C36 &amp; "` " &amp; D36 &amp; IF(E36&gt;0,"(" &amp; E36 &amp; ") "," ") &amp; IF(F36&lt;&gt;"","NOT NULL ","") &amp; IF(G36="","","DEFAULT '" &amp; G36 &amp; "' ") &amp; IF(A36="",""," */")</f>
-        <v xml:space="preserve">,`partner_flag` INT </v>
+        <v xml:space="preserve">,`partner_flag` INT DEFAULT '0' </v>
       </c>
       <c r="J36" s="41" t="str">
         <f>"," &amp; IF(A36="","","/* ") &amp; "`" &amp; C36 &amp; "` " &amp; D36 &amp; IF(E36&gt;0,"(" &amp; E36 &amp; ") "," ") &amp; IF(F36&lt;&gt;"","NOT NULL ","") &amp; IF(G36="","","DEFAULT '" &amp; G36 &amp; "' ") &amp; IF(A36="",""," */")</f>
-        <v xml:space="preserve">,`partner_flag` INT </v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A37" s="2"/>
-      <c r="B37" s="20" t="s">
+        <v xml:space="preserve">,`partner_flag` INT DEFAULT '0' </v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="34"/>
+      <c r="B37" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="36"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="40" t="str">
+        <f>"," &amp; IF(A37="","","/* ") &amp; "`" &amp; C37 &amp; "` " &amp; D37 &amp; IF(E37&gt;0,"(" &amp; E37 &amp; ") "," ") &amp; IF(F37&lt;&gt;"","NOT NULL ","") &amp; IF(G37="","","DEFAULT '" &amp; G37 &amp; "' ") &amp; IF(A37="",""," */")</f>
+        <v xml:space="preserve">,`partner_id` INT </v>
+      </c>
+      <c r="J37" s="41" t="str">
+        <f>"," &amp; IF(A37="","","/* ") &amp; "`" &amp; C37 &amp; "` " &amp; D37 &amp; IF(E37&gt;0,"(" &amp; E37 &amp; ") "," ") &amp; IF(F37&lt;&gt;"","NOT NULL ","") &amp; IF(G37="","","DEFAULT '" &amp; G37 &amp; "' ") &amp; IF(A37="",""," */")</f>
+        <v xml:space="preserve">,`partner_id` INT </v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="2"/>
+      <c r="B38" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="27" t="str">
-        <f t="shared" ref="I37:I40" si="2">"," &amp; IF(A37="","","/* ") &amp; "`" &amp; C37 &amp; "` " &amp; D37 &amp; IF(E37&gt;0,"(" &amp; E37 &amp; ") "," ") &amp; IF(F37&lt;&gt;"","NOT NULL ","") &amp; IF(G37="","","DEFAULT '" &amp; G37 &amp; "' ") &amp; IF(A37="",""," */")</f>
+      <c r="E38" s="7"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="27" t="str">
+        <f t="shared" ref="I38:I41" si="2">"," &amp; IF(A38="","","/* ") &amp; "`" &amp; C38 &amp; "` " &amp; D38 &amp; IF(E38&gt;0,"(" &amp; E38 &amp; ") "," ") &amp; IF(F38&lt;&gt;"","NOT NULL ","") &amp; IF(G38="","","DEFAULT '" &amp; G38 &amp; "' ") &amp; IF(A38="",""," */")</f>
         <v xml:space="preserve">,`remarks` TEXT </v>
       </c>
-      <c r="J37" s="29" t="str">
-        <f t="shared" ref="J37:J40" si="3">"," &amp; IF(A37="","","/* ") &amp; "`" &amp; C37 &amp; "` " &amp; D37 &amp; IF(E37&gt;0,"(" &amp; E37 &amp; ") "," ") &amp; IF(F37&lt;&gt;"","NOT NULL ","") &amp; IF(G37="","","DEFAULT '" &amp; G37 &amp; "' ") &amp; IF(A37="",""," */")</f>
+      <c r="J38" s="29" t="str">
+        <f t="shared" ref="J38:J41" si="3">"," &amp; IF(A38="","","/* ") &amp; "`" &amp; C38 &amp; "` " &amp; D38 &amp; IF(E38&gt;0,"(" &amp; E38 &amp; ") "," ") &amp; IF(F38&lt;&gt;"","NOT NULL ","") &amp; IF(G38="","","DEFAULT '" &amp; G38 &amp; "' ") &amp; IF(A38="",""," */")</f>
         <v xml:space="preserve">,`remarks` TEXT </v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="34"/>
-      <c r="B38" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D38" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="40" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-      <c r="J38" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="39" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="34"/>
       <c r="B39" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E39" s="36"/>
       <c r="F39" s="35"/>
@@ -3210,20 +3223,20 @@
       <c r="H39" s="38"/>
       <c r="I39" s="40" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J39" s="41" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="40" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="34"/>
       <c r="B40" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D40" s="35" t="s">
         <v>8</v>
@@ -3234,329 +3247,327 @@
       <c r="H40" s="38"/>
       <c r="I40" s="40" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J40" s="41" t="str">
         <f t="shared" si="3"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="34"/>
+      <c r="B41" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="36"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="40" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A41" s="2"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J41" s="29" t="s">
-        <v>33</v>
+      <c r="J41" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J42" s="29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="2"/>
-      <c r="B43" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I43" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C43 &amp; "` ("</f>
-        <v>CREATE TABLE `customers` (</v>
-      </c>
-      <c r="J43" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C43 &amp; "` ("</f>
-        <v>CREATE TABLE `customers` (</v>
-      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="2"/>
-      <c r="B44" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" s="30" t="s">
-        <v>20</v>
+      <c r="B44" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C44 &amp; "` ("</f>
+        <v>CREATE TABLE `customers` (</v>
+      </c>
+      <c r="J44" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C44 &amp; "` ("</f>
+        <v>CREATE TABLE `customers` (</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="2"/>
       <c r="B45" s="20" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="6" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="9"/>
-      <c r="I45" s="27" t="str">
-        <f t="shared" ref="I45:I51" si="4">"," &amp; IF(A45="","","/* ") &amp; "`" &amp; C45 &amp; "` " &amp; D45 &amp; IF(E45&gt;0,"(" &amp; E45 &amp; ") "," ") &amp; IF(F45&lt;&gt;"","NOT NULL ","") &amp; IF(G45="","","DEFAULT '" &amp; G45 &amp; "' ") &amp; IF(A45="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
-      </c>
-      <c r="J45" s="29" t="str">
-        <f t="shared" ref="J45:J51" si="5">"," &amp; IF(A45="","","/* ") &amp; "`" &amp; C45 &amp; "` " &amp; D45 &amp; IF(E45&gt;0,"(" &amp; E45 &amp; ") "," ") &amp; IF(F45&lt;&gt;"","NOT NULL ","") &amp; IF(G45="","","DEFAULT '" &amp; G45 &amp; "' ") &amp; IF(A45="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
+      <c r="I45" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" s="30" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="2"/>
       <c r="B46" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="7">
-        <v>128</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E46" s="7"/>
       <c r="F46" s="6" t="s">
         <v>136</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="9"/>
       <c r="I46" s="27" t="str">
+        <f t="shared" ref="I46:I52" si="4">"," &amp; IF(A46="","","/* ") &amp; "`" &amp; C46 &amp; "` " &amp; D46 &amp; IF(E46&gt;0,"(" &amp; E46 &amp; ") "," ") &amp; IF(F46&lt;&gt;"","NOT NULL ","") &amp; IF(G46="","","DEFAULT '" &amp; G46 &amp; "' ") &amp; IF(A46="",""," */")</f>
+        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
+      </c>
+      <c r="J46" s="29" t="str">
+        <f t="shared" ref="J46:J52" si="5">"," &amp; IF(A46="","","/* ") &amp; "`" &amp; C46 &amp; "` " &amp; D46 &amp; IF(E46&gt;0,"(" &amp; E46 &amp; ") "," ") &amp; IF(F46&lt;&gt;"","NOT NULL ","") &amp; IF(G46="","","DEFAULT '" &amp; G46 &amp; "' ") &amp; IF(A46="",""," */")</f>
+        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" s="2"/>
+      <c r="B47" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="7">
+        <v>128</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="27" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">,`customer_name` VARCHAR(128) NOT NULL </v>
       </c>
-      <c r="J46" s="29" t="str">
+      <c r="J47" s="29" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">,`customer_name` VARCHAR(128) NOT NULL </v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="34"/>
-      <c r="B47" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="D47" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="36">
-        <v>512</v>
-      </c>
-      <c r="F47" s="35"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="40" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">,`address` VARCHAR(512) </v>
-      </c>
-      <c r="J47" s="41" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">,`address` VARCHAR(512) </v>
       </c>
     </row>
     <row r="48" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="34"/>
       <c r="B48" s="39" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D48" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="36">
-        <v>4</v>
+        <v>512</v>
       </c>
       <c r="F48" s="35"/>
       <c r="G48" s="37"/>
       <c r="H48" s="38"/>
       <c r="I48" s="40" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">,`identity2` VARCHAR(4) </v>
+        <v xml:space="preserve">,`address` VARCHAR(512) </v>
       </c>
       <c r="J48" s="41" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">,`address` VARCHAR(512) </v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="34"/>
+      <c r="B49" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="36">
+        <v>4</v>
+      </c>
+      <c r="F49" s="35"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="40" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">,`identity2` VARCHAR(4) </v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A49" s="2"/>
-      <c r="B49" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="7">
-        <v>256</v>
-      </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="27" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
-      </c>
-      <c r="J49" s="29" t="str">
+      <c r="J49" s="41" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
+        <v xml:space="preserve">,`identity2` VARCHAR(4) </v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="2"/>
       <c r="B50" s="20" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="7">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="8"/>
       <c r="H50" s="9"/>
       <c r="I50" s="27" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
       <c r="J50" s="29" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="2"/>
       <c r="B51" s="20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="E51" s="7">
+        <v>128</v>
+      </c>
       <c r="F51" s="6"/>
       <c r="G51" s="8"/>
       <c r="H51" s="9"/>
       <c r="I51" s="27" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">,`remarks` TEXT </v>
+        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
       <c r="J51" s="29" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">,`remarks` TEXT </v>
+        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="2"/>
       <c r="B52" s="20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="7">
-        <v>128</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E52" s="7"/>
       <c r="F52" s="6"/>
       <c r="G52" s="8"/>
       <c r="H52" s="9"/>
       <c r="I52" s="27" t="str">
-        <f t="shared" ref="I52:I54" si="6">"," &amp; IF(A52="","","/* ") &amp; "`" &amp; C52 &amp; "` " &amp; D52 &amp; IF(E52&gt;0,"(" &amp; E52 &amp; ") "," ") &amp; IF(F52&lt;&gt;"","NOT NULL ","") &amp; IF(G52="","","DEFAULT '" &amp; G52 &amp; "' ") &amp; IF(A52="",""," */")</f>
-        <v xml:space="preserve">,`admin_name1` VARCHAR(128) </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">,`remarks` TEXT </v>
       </c>
       <c r="J52" s="29" t="str">
-        <f t="shared" ref="J52:J54" si="7">"," &amp; IF(A52="","","/* ") &amp; "`" &amp; C52 &amp; "` " &amp; D52 &amp; IF(E52&gt;0,"(" &amp; E52 &amp; ") "," ") &amp; IF(F52&lt;&gt;"","NOT NULL ","") &amp; IF(G52="","","DEFAULT '" &amp; G52 &amp; "' ") &amp; IF(A52="",""," */")</f>
-        <v xml:space="preserve">,`admin_name1` VARCHAR(128) </v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">,`remarks` TEXT </v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="2"/>
       <c r="B53" s="20" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="7">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="8"/>
       <c r="H53" s="9"/>
       <c r="I53" s="27" t="str">
-        <f>"," &amp; IF(A53="","","/* ") &amp; "`" &amp; C53 &amp; "` " &amp; D53 &amp; IF(E53&gt;0,"(" &amp; E53 &amp; ") "," ") &amp; IF(F53&lt;&gt;"","NOT NULL ","") &amp; IF(G53="","","DEFAULT '" &amp; G53 &amp; "' ") &amp; IF(A53="",""," */")</f>
-        <v xml:space="preserve">,`div1` VARCHAR(256) </v>
+        <f t="shared" ref="I53:I55" si="6">"," &amp; IF(A53="","","/* ") &amp; "`" &amp; C53 &amp; "` " &amp; D53 &amp; IF(E53&gt;0,"(" &amp; E53 &amp; ") "," ") &amp; IF(F53&lt;&gt;"","NOT NULL ","") &amp; IF(G53="","","DEFAULT '" &amp; G53 &amp; "' ") &amp; IF(A53="",""," */")</f>
+        <v xml:space="preserve">,`admin_name1` VARCHAR(128) </v>
       </c>
       <c r="J53" s="29" t="str">
-        <f>"," &amp; IF(A53="","","/* ") &amp; "`" &amp; C53 &amp; "` " &amp; D53 &amp; IF(E53&gt;0,"(" &amp; E53 &amp; ") "," ") &amp; IF(F53&lt;&gt;"","NOT NULL ","") &amp; IF(G53="","","DEFAULT '" &amp; G53 &amp; "' ") &amp; IF(A53="",""," */")</f>
-        <v xml:space="preserve">,`div1` VARCHAR(256) </v>
+        <f t="shared" ref="J53:J55" si="7">"," &amp; IF(A53="","","/* ") &amp; "`" &amp; C53 &amp; "` " &amp; D53 &amp; IF(E53&gt;0,"(" &amp; E53 &amp; ") "," ") &amp; IF(F53&lt;&gt;"","NOT NULL ","") &amp; IF(G53="","","DEFAULT '" &amp; G53 &amp; "' ") &amp; IF(A53="",""," */")</f>
+        <v xml:space="preserve">,`admin_name1` VARCHAR(128) </v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="2"/>
       <c r="B54" s="20" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>7</v>
@@ -3568,73 +3579,73 @@
       <c r="G54" s="8"/>
       <c r="H54" s="9"/>
       <c r="I54" s="27" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">,`mail1` VARCHAR(256) </v>
+        <f>"," &amp; IF(A54="","","/* ") &amp; "`" &amp; C54 &amp; "` " &amp; D54 &amp; IF(E54&gt;0,"(" &amp; E54 &amp; ") "," ") &amp; IF(F54&lt;&gt;"","NOT NULL ","") &amp; IF(G54="","","DEFAULT '" &amp; G54 &amp; "' ") &amp; IF(A54="",""," */")</f>
+        <v xml:space="preserve">,`div1` VARCHAR(256) </v>
       </c>
       <c r="J54" s="29" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">,`mail1` VARCHAR(256) </v>
+        <f>"," &amp; IF(A54="","","/* ") &amp; "`" &amp; C54 &amp; "` " &amp; D54 &amp; IF(E54&gt;0,"(" &amp; E54 &amp; ") "," ") &amp; IF(F54&lt;&gt;"","NOT NULL ","") &amp; IF(G54="","","DEFAULT '" &amp; G54 &amp; "' ") &amp; IF(A54="",""," */")</f>
+        <v xml:space="preserve">,`div1` VARCHAR(256) </v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="2"/>
       <c r="B55" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="7">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="8"/>
       <c r="H55" s="9"/>
       <c r="I55" s="27" t="str">
-        <f t="shared" ref="I55:I60" si="8">"," &amp; IF(A55="","","/* ") &amp; "`" &amp; C55 &amp; "` " &amp; D55 &amp; IF(E55&gt;0,"(" &amp; E55 &amp; ") "," ") &amp; IF(F55&lt;&gt;"","NOT NULL ","") &amp; IF(G55="","","DEFAULT '" &amp; G55 &amp; "' ") &amp; IF(A55="",""," */")</f>
-        <v xml:space="preserve">,`admin_name2` VARCHAR(128) </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">,`mail1` VARCHAR(256) </v>
       </c>
       <c r="J55" s="29" t="str">
-        <f t="shared" ref="J55:J60" si="9">"," &amp; IF(A55="","","/* ") &amp; "`" &amp; C55 &amp; "` " &amp; D55 &amp; IF(E55&gt;0,"(" &amp; E55 &amp; ") "," ") &amp; IF(F55&lt;&gt;"","NOT NULL ","") &amp; IF(G55="","","DEFAULT '" &amp; G55 &amp; "' ") &amp; IF(A55="",""," */")</f>
-        <v xml:space="preserve">,`admin_name2` VARCHAR(128) </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">,`mail1` VARCHAR(256) </v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="2"/>
       <c r="B56" s="20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="7">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="8"/>
       <c r="H56" s="9"/>
       <c r="I56" s="27" t="str">
-        <f>"," &amp; IF(A56="","","/* ") &amp; "`" &amp; C56 &amp; "` " &amp; D56 &amp; IF(E56&gt;0,"(" &amp; E56 &amp; ") "," ") &amp; IF(F56&lt;&gt;"","NOT NULL ","") &amp; IF(G56="","","DEFAULT '" &amp; G56 &amp; "' ") &amp; IF(A56="",""," */")</f>
-        <v xml:space="preserve">,`div2` VARCHAR(256) </v>
+        <f t="shared" ref="I56:I61" si="8">"," &amp; IF(A56="","","/* ") &amp; "`" &amp; C56 &amp; "` " &amp; D56 &amp; IF(E56&gt;0,"(" &amp; E56 &amp; ") "," ") &amp; IF(F56&lt;&gt;"","NOT NULL ","") &amp; IF(G56="","","DEFAULT '" &amp; G56 &amp; "' ") &amp; IF(A56="",""," */")</f>
+        <v xml:space="preserve">,`admin_name2` VARCHAR(128) </v>
       </c>
       <c r="J56" s="29" t="str">
-        <f>"," &amp; IF(A56="","","/* ") &amp; "`" &amp; C56 &amp; "` " &amp; D56 &amp; IF(E56&gt;0,"(" &amp; E56 &amp; ") "," ") &amp; IF(F56&lt;&gt;"","NOT NULL ","") &amp; IF(G56="","","DEFAULT '" &amp; G56 &amp; "' ") &amp; IF(A56="",""," */")</f>
-        <v xml:space="preserve">,`div2` VARCHAR(256) </v>
+        <f t="shared" ref="J56:J61" si="9">"," &amp; IF(A56="","","/* ") &amp; "`" &amp; C56 &amp; "` " &amp; D56 &amp; IF(E56&gt;0,"(" &amp; E56 &amp; ") "," ") &amp; IF(F56&lt;&gt;"","NOT NULL ","") &amp; IF(G56="","","DEFAULT '" &amp; G56 &amp; "' ") &amp; IF(A56="",""," */")</f>
+        <v xml:space="preserve">,`admin_name2` VARCHAR(128) </v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="2"/>
       <c r="B57" s="20" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>7</v>
@@ -3646,48 +3657,50 @@
       <c r="G57" s="8"/>
       <c r="H57" s="9"/>
       <c r="I57" s="27" t="str">
+        <f>"," &amp; IF(A57="","","/* ") &amp; "`" &amp; C57 &amp; "` " &amp; D57 &amp; IF(E57&gt;0,"(" &amp; E57 &amp; ") "," ") &amp; IF(F57&lt;&gt;"","NOT NULL ","") &amp; IF(G57="","","DEFAULT '" &amp; G57 &amp; "' ") &amp; IF(A57="",""," */")</f>
+        <v xml:space="preserve">,`div2` VARCHAR(256) </v>
+      </c>
+      <c r="J57" s="29" t="str">
+        <f>"," &amp; IF(A57="","","/* ") &amp; "`" &amp; C57 &amp; "` " &amp; D57 &amp; IF(E57&gt;0,"(" &amp; E57 &amp; ") "," ") &amp; IF(F57&lt;&gt;"","NOT NULL ","") &amp; IF(G57="","","DEFAULT '" &amp; G57 &amp; "' ") &amp; IF(A57="",""," */")</f>
+        <v xml:space="preserve">,`div2` VARCHAR(256) </v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A58" s="2"/>
+      <c r="B58" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="7">
+        <v>256</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="27" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">,`mail2` VARCHAR(256) </v>
       </c>
-      <c r="J57" s="29" t="str">
+      <c r="J58" s="29" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">,`mail2` VARCHAR(256) </v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="34"/>
-      <c r="B58" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D58" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E58" s="36"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="40" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-      <c r="J58" s="41" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="59" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="34"/>
       <c r="B59" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E59" s="36"/>
       <c r="F59" s="35"/>
@@ -3695,20 +3708,20 @@
       <c r="H59" s="38"/>
       <c r="I59" s="40" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J59" s="41" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="60" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="34"/>
       <c r="B60" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D60" s="35" t="s">
         <v>8</v>
@@ -3719,196 +3732,196 @@
       <c r="H60" s="38"/>
       <c r="I60" s="40" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J60" s="41" t="str">
         <f t="shared" si="9"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="34"/>
+      <c r="B61" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="36"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="40" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A61" s="2"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J61" s="29" t="s">
-        <v>33</v>
+      <c r="J61" s="41" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="2"/>
-    </row>
-    <row r="63" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="34"/>
-      <c r="B63" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G63" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I63" s="40" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C63 &amp; "` ("</f>
-        <v>CREATE TABLE `contracts` (</v>
-      </c>
-      <c r="J63" s="41" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C63 &amp; "` ("</f>
-        <v>CREATE TABLE `contracts` (</v>
-      </c>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A63" s="2"/>
     </row>
     <row r="64" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="34"/>
-      <c r="B64" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" s="36"/>
-      <c r="F64" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" s="37"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="J64" s="30" t="s">
-        <v>20</v>
+      <c r="B64" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I64" s="40" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C64 &amp; "` ("</f>
+        <v>CREATE TABLE `contracts` (</v>
+      </c>
+      <c r="J64" s="41" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C64 &amp; "` ("</f>
+        <v>CREATE TABLE `contracts` (</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="34"/>
       <c r="B65" s="39" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="D65" s="35" t="s">
         <v>5</v>
       </c>
       <c r="E65" s="36"/>
       <c r="F65" s="35" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="G65" s="37"/>
       <c r="H65" s="38"/>
-      <c r="I65" s="40" t="str">
-        <f t="shared" ref="I65:I73" si="10">"," &amp; IF(A65="","","/* ") &amp; "`" &amp; C65 &amp; "` " &amp; D65 &amp; IF(E65&gt;0,"(" &amp; E65 &amp; ") "," ") &amp; IF(F65&lt;&gt;"","NOT NULL ","") &amp; IF(G65="","","DEFAULT '" &amp; G65 &amp; "' ") &amp; IF(A65="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
-      </c>
-      <c r="J65" s="41" t="str">
-        <f t="shared" ref="J65:J73" si="11">"," &amp; IF(A65="","","/* ") &amp; "`" &amp; C65 &amp; "` " &amp; D65 &amp; IF(E65&gt;0,"(" &amp; E65 &amp; ") "," ") &amp; IF(F65&lt;&gt;"","NOT NULL ","") &amp; IF(G65="","","DEFAULT '" &amp; G65 &amp; "' ") &amp; IF(A65="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
+      <c r="I65" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65" s="30" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A66" s="34"/>
       <c r="B66" s="39" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D66" s="35" t="s">
         <v>5</v>
       </c>
       <c r="E66" s="36"/>
-      <c r="F66" s="35"/>
+      <c r="F66" s="35" t="s">
+        <v>136</v>
+      </c>
       <c r="G66" s="37"/>
       <c r="H66" s="38"/>
       <c r="I66" s="40" t="str">
-        <f>"," &amp; IF(A66="","","/* ") &amp; "`" &amp; C66 &amp; "` " &amp; D66 &amp; IF(E66&gt;0,"(" &amp; E66 &amp; ") "," ") &amp; IF(F66&lt;&gt;"","NOT NULL ","") &amp; IF(G66="","","DEFAULT '" &amp; G66 &amp; "' ") &amp; IF(A66="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <f t="shared" ref="I66:I74" si="10">"," &amp; IF(A66="","","/* ") &amp; "`" &amp; C66 &amp; "` " &amp; D66 &amp; IF(E66&gt;0,"(" &amp; E66 &amp; ") "," ") &amp; IF(F66&lt;&gt;"","NOT NULL ","") &amp; IF(G66="","","DEFAULT '" &amp; G66 &amp; "' ") &amp; IF(A66="",""," */")</f>
+        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
       </c>
       <c r="J66" s="41" t="str">
-        <f>"," &amp; IF(A66="","","/* ") &amp; "`" &amp; C66 &amp; "` " &amp; D66 &amp; IF(E66&gt;0,"(" &amp; E66 &amp; ") "," ") &amp; IF(F66&lt;&gt;"","NOT NULL ","") &amp; IF(G66="","","DEFAULT '" &amp; G66 &amp; "' ") &amp; IF(A66="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <f t="shared" ref="J66:J74" si="11">"," &amp; IF(A66="","","/* ") &amp; "`" &amp; C66 &amp; "` " &amp; D66 &amp; IF(E66&gt;0,"(" &amp; E66 &amp; ") "," ") &amp; IF(F66&lt;&gt;"","NOT NULL ","") &amp; IF(G66="","","DEFAULT '" &amp; G66 &amp; "' ") &amp; IF(A66="",""," */")</f>
+        <v xml:space="preserve">,`client_id` INT NOT NULL </v>
       </c>
     </row>
     <row r="67" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A67" s="34"/>
       <c r="B67" s="39" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>175</v>
+        <v>95</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E67" s="36"/>
       <c r="F67" s="35"/>
       <c r="G67" s="37"/>
       <c r="H67" s="38"/>
       <c r="I67" s="40" t="str">
-        <f t="shared" ref="I67" si="12">"," &amp; IF(A67="","","/* ") &amp; "`" &amp; C67 &amp; "` " &amp; D67 &amp; IF(E67&gt;0,"(" &amp; E67 &amp; ") "," ") &amp; IF(F67&lt;&gt;"","NOT NULL ","") &amp; IF(G67="","","DEFAULT '" &amp; G67 &amp; "' ") &amp; IF(A67="",""," */")</f>
-        <v xml:space="preserve">,`contract_date` DATE </v>
+        <f>"," &amp; IF(A67="","","/* ") &amp; "`" &amp; C67 &amp; "` " &amp; D67 &amp; IF(E67&gt;0,"(" &amp; E67 &amp; ") "," ") &amp; IF(F67&lt;&gt;"","NOT NULL ","") &amp; IF(G67="","","DEFAULT '" &amp; G67 &amp; "' ") &amp; IF(A67="",""," */")</f>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
       <c r="J67" s="41" t="str">
-        <f t="shared" ref="J67" si="13">"," &amp; IF(A67="","","/* ") &amp; "`" &amp; C67 &amp; "` " &amp; D67 &amp; IF(E67&gt;0,"(" &amp; E67 &amp; ") "," ") &amp; IF(F67&lt;&gt;"","NOT NULL ","") &amp; IF(G67="","","DEFAULT '" &amp; G67 &amp; "' ") &amp; IF(A67="",""," */")</f>
-        <v xml:space="preserve">,`contract_date` DATE </v>
+        <f>"," &amp; IF(A67="","","/* ") &amp; "`" &amp; C67 &amp; "` " &amp; D67 &amp; IF(E67&gt;0,"(" &amp; E67 &amp; ") "," ") &amp; IF(F67&lt;&gt;"","NOT NULL ","") &amp; IF(G67="","","DEFAULT '" &amp; G67 &amp; "' ") &amp; IF(A67="",""," */")</f>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="68" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="34"/>
       <c r="B68" s="39" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C68" s="35" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D68" s="35" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E68" s="36"/>
       <c r="F68" s="35"/>
       <c r="G68" s="37"/>
       <c r="H68" s="38"/>
       <c r="I68" s="40" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">,`contractname_id` INT </v>
+        <f t="shared" ref="I68" si="12">"," &amp; IF(A68="","","/* ") &amp; "`" &amp; C68 &amp; "` " &amp; D68 &amp; IF(E68&gt;0,"(" &amp; E68 &amp; ") "," ") &amp; IF(F68&lt;&gt;"","NOT NULL ","") &amp; IF(G68="","","DEFAULT '" &amp; G68 &amp; "' ") &amp; IF(A68="",""," */")</f>
+        <v xml:space="preserve">,`contract_date` DATE </v>
       </c>
       <c r="J68" s="41" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">,`contractname_id` INT </v>
+        <f t="shared" ref="J68" si="13">"," &amp; IF(A68="","","/* ") &amp; "`" &amp; C68 &amp; "` " &amp; D68 &amp; IF(E68&gt;0,"(" &amp; E68 &amp; ") "," ") &amp; IF(F68&lt;&gt;"","NOT NULL ","") &amp; IF(G68="","","DEFAULT '" &amp; G68 &amp; "' ") &amp; IF(A68="",""," */")</f>
+        <v xml:space="preserve">,`contract_date` DATE </v>
       </c>
     </row>
     <row r="69" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A69" s="34"/>
       <c r="B69" s="39" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="C69" s="35" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E69" s="36"/>
       <c r="F69" s="35"/>
@@ -3916,46 +3929,44 @@
       <c r="H69" s="38"/>
       <c r="I69" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`remarks` TEXT </v>
+        <v xml:space="preserve">,`contractname_id` INT </v>
       </c>
       <c r="J69" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`remarks` TEXT </v>
+        <v xml:space="preserve">,`contractname_id` INT </v>
       </c>
     </row>
     <row r="70" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A70" s="34"/>
-      <c r="B70" s="43" t="s">
-        <v>135</v>
+      <c r="B70" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="C70" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D70" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E70" s="36">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E70" s="36"/>
       <c r="F70" s="35"/>
       <c r="G70" s="37"/>
       <c r="H70" s="38"/>
       <c r="I70" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <v xml:space="preserve">,`remarks` TEXT </v>
       </c>
       <c r="J70" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <v xml:space="preserve">,`remarks` TEXT </v>
       </c>
     </row>
     <row r="71" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A71" s="34"/>
       <c r="B71" s="43" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="C71" s="35" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="D71" s="35" t="s">
         <v>7</v>
@@ -3968,118 +3979,120 @@
       <c r="H71" s="38"/>
       <c r="I71" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J71" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="72" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A72" s="34"/>
       <c r="B72" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C72" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D72" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E72" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E72" s="36">
+        <v>256</v>
+      </c>
       <c r="F72" s="35"/>
       <c r="G72" s="37"/>
       <c r="H72" s="38"/>
       <c r="I72" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J72" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="73" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A73" s="34"/>
       <c r="B73" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D73" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="36">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E73" s="36"/>
       <c r="F73" s="35"/>
       <c r="G73" s="37"/>
       <c r="H73" s="38"/>
       <c r="I73" s="40" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
       <c r="J73" s="41" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
     </row>
     <row r="74" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="34"/>
       <c r="B74" s="43" t="s">
-        <v>161</v>
+        <v>52</v>
       </c>
       <c r="C74" s="35" t="s">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="D74" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E74" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E74" s="36">
+        <v>64</v>
+      </c>
       <c r="F74" s="35"/>
       <c r="G74" s="37"/>
       <c r="H74" s="38"/>
       <c r="I74" s="40" t="str">
-        <f t="shared" ref="I74:I76" si="14">"," &amp; IF(A74="","","/* ") &amp; "`" &amp; C74 &amp; "` " &amp; D74 &amp; IF(E74&gt;0,"(" &amp; E74 &amp; ") "," ") &amp; IF(F74&lt;&gt;"","NOT NULL ","") &amp; IF(G74="","","DEFAULT '" &amp; G74 &amp; "' ") &amp; IF(A74="",""," */")</f>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
       <c r="J74" s="41" t="str">
-        <f t="shared" ref="J74:J76" si="15">"," &amp; IF(A74="","","/* ") &amp; "`" &amp; C74 &amp; "` " &amp; D74 &amp; IF(E74&gt;0,"(" &amp; E74 &amp; ") "," ") &amp; IF(F74&lt;&gt;"","NOT NULL ","") &amp; IF(G74="","","DEFAULT '" &amp; G74 &amp; "' ") &amp; IF(A74="",""," */")</f>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
     <row r="75" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A75" s="34"/>
       <c r="B75" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C75" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D75" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E75" s="36"/>
       <c r="F75" s="35"/>
       <c r="G75" s="37"/>
       <c r="H75" s="38"/>
       <c r="I75" s="40" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" ref="I75:I77" si="14">"," &amp; IF(A75="","","/* ") &amp; "`" &amp; C75 &amp; "` " &amp; D75 &amp; IF(E75&gt;0,"(" &amp; E75 &amp; ") "," ") &amp; IF(F75&lt;&gt;"","NOT NULL ","") &amp; IF(G75="","","DEFAULT '" &amp; G75 &amp; "' ") &amp; IF(A75="",""," */")</f>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J75" s="41" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" ref="J75:J77" si="15">"," &amp; IF(A75="","","/* ") &amp; "`" &amp; C75 &amp; "` " &amp; D75 &amp; IF(E75&gt;0,"(" &amp; E75 &amp; ") "," ") &amp; IF(F75&lt;&gt;"","NOT NULL ","") &amp; IF(G75="","","DEFAULT '" &amp; G75 &amp; "' ") &amp; IF(A75="",""," */")</f>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="76" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A76" s="34"/>
       <c r="B76" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C76" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D76" s="35" t="s">
         <v>8</v>
@@ -4090,155 +4103,153 @@
       <c r="H76" s="38"/>
       <c r="I76" s="40" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J76" s="41" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="77" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A77" s="34"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="23"/>
-      <c r="H77" s="21"/>
-      <c r="I77" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J77" s="41" t="s">
-        <v>33</v>
+      <c r="B77" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D77" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="36"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="40" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
+      </c>
+      <c r="J77" s="41" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="78" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A78" s="34"/>
-      <c r="E78" s="34"/>
-      <c r="G78" s="3"/>
-      <c r="I78" s="25"/>
-      <c r="J78" s="25"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A79" s="2"/>
-      <c r="B79" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G79" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H79" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I79" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C79 &amp; "` ("</f>
-        <v>CREATE TABLE `orders` (</v>
-      </c>
-      <c r="J79" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C79 &amp; "` ("</f>
-        <v>CREATE TABLE `orders` (</v>
-      </c>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J78" s="41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="G79" s="3"/>
+      <c r="I79" s="25"/>
+      <c r="J79" s="25"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="2"/>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H80" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I80" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C80 &amp; "` ("</f>
+        <v>CREATE TABLE `orders` (</v>
+      </c>
+      <c r="J80" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C80 &amp; "` ("</f>
+        <v>CREATE TABLE `orders` (</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A81" s="2"/>
+      <c r="B81" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C81" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D81" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E80" s="7"/>
-      <c r="F80" s="6" t="s">
+      <c r="E81" s="7"/>
+      <c r="F81" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G80" s="8"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="28" t="s">
+      <c r="G81" s="8"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J80" s="30" t="s">
+      <c r="J81" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="34"/>
-      <c r="B81" s="32" t="s">
+    <row r="82" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="34"/>
+      <c r="B82" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C81" s="35" t="s">
+      <c r="C82" s="35" t="s">
         <v>131</v>
-      </c>
-      <c r="D81" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" s="36">
-        <v>20</v>
-      </c>
-      <c r="F81" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G81" s="37"/>
-      <c r="H81" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="I81" s="40" t="str">
-        <f t="shared" ref="I81:I93" si="16">"," &amp; IF(A81="","","/* ") &amp; "`" &amp; C81 &amp; "` " &amp; D81 &amp; IF(E81&gt;0,"(" &amp; E81 &amp; ") "," ") &amp; IF(F81&lt;&gt;"","NOT NULL ","") &amp; IF(G81="","","DEFAULT '" &amp; G81 &amp; "' ") &amp; IF(A81="",""," */")</f>
-        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
-      </c>
-      <c r="J81" s="41" t="str">
-        <f t="shared" ref="J81:J93" si="17">"," &amp; IF(A81="","","/* ") &amp; "`" &amp; C81 &amp; "` " &amp; D81 &amp; IF(E81&gt;0,"(" &amp; E81 &amp; ") "," ") &amp; IF(F81&lt;&gt;"","NOT NULL ","") &amp; IF(G81="","","DEFAULT '" &amp; G81 &amp; "' ") &amp; IF(A81="",""," */")</f>
-        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A82" s="2"/>
-      <c r="B82" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" s="35" t="s">
-        <v>132</v>
       </c>
       <c r="D82" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="36">
-        <v>256</v>
-      </c>
-      <c r="F82" s="35"/>
+        <v>20</v>
+      </c>
+      <c r="F82" s="35" t="s">
+        <v>18</v>
+      </c>
       <c r="G82" s="37"/>
-      <c r="H82" s="38"/>
+      <c r="H82" s="38" t="s">
+        <v>138</v>
+      </c>
       <c r="I82" s="40" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
+        <f t="shared" ref="I82:I94" si="16">"," &amp; IF(A82="","","/* ") &amp; "`" &amp; C82 &amp; "` " &amp; D82 &amp; IF(E82&gt;0,"(" &amp; E82 &amp; ") "," ") &amp; IF(F82&lt;&gt;"","NOT NULL ","") &amp; IF(G82="","","DEFAULT '" &amp; G82 &amp; "' ") &amp; IF(A82="",""," */")</f>
+        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
       </c>
       <c r="J82" s="41" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="34"/>
-      <c r="B83" s="39" t="s">
-        <v>113</v>
+        <f t="shared" ref="J82:J94" si="17">"," &amp; IF(A82="","","/* ") &amp; "`" &amp; C82 &amp; "` " &amp; D82 &amp; IF(E82&gt;0,"(" &amp; E82 &amp; ") "," ") &amp; IF(F82&lt;&gt;"","NOT NULL ","") &amp; IF(G82="","","DEFAULT '" &amp; G82 &amp; "' ") &amp; IF(A82="",""," */")</f>
+        <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A83" s="2"/>
+      <c r="B83" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="C83" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D83" s="35" t="s">
         <v>7</v>
@@ -4251,70 +4262,70 @@
       <c r="H83" s="38"/>
       <c r="I83" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
+        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
       </c>
       <c r="J83" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
+        <v xml:space="preserve">,`company_name1` VARCHAR(256) </v>
       </c>
     </row>
     <row r="84" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A84" s="34"/>
       <c r="B84" s="39" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C84" s="35" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="D84" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E84" s="36">
+        <v>256</v>
+      </c>
       <c r="F84" s="35"/>
       <c r="G84" s="37"/>
       <c r="H84" s="38"/>
       <c r="I84" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`order_date` DATE </v>
+        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
       </c>
       <c r="J84" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`order_date` DATE </v>
+        <v xml:space="preserve">,`company_name2` VARCHAR(256) </v>
       </c>
     </row>
     <row r="85" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A85" s="34"/>
       <c r="B85" s="39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C85" s="35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D85" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E85" s="36">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E85" s="36"/>
       <c r="F85" s="35"/>
       <c r="G85" s="37"/>
       <c r="H85" s="38"/>
       <c r="I85" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_date` DATE </v>
       </c>
       <c r="J85" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_date` DATE </v>
       </c>
     </row>
     <row r="86" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A86" s="34"/>
       <c r="B86" s="39" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C86" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D86" s="35" t="s">
         <v>7</v>
@@ -4327,20 +4338,20 @@
       <c r="H86" s="38"/>
       <c r="I86" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
       </c>
       <c r="J86" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="87" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A87" s="34"/>
       <c r="B87" s="39" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C87" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D87" s="35" t="s">
         <v>7</v>
@@ -4350,49 +4361,51 @@
       </c>
       <c r="F87" s="35"/>
       <c r="G87" s="37"/>
-      <c r="H87" s="38" t="s">
-        <v>134</v>
-      </c>
+      <c r="H87" s="38"/>
       <c r="I87" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
       </c>
       <c r="J87" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="88" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A88" s="34"/>
       <c r="B88" s="39" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C88" s="35" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D88" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E88" s="36">
+        <v>20</v>
+      </c>
       <c r="F88" s="35"/>
       <c r="G88" s="37"/>
-      <c r="H88" s="38"/>
+      <c r="H88" s="38" t="s">
+        <v>134</v>
+      </c>
       <c r="I88" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`delivery_date` DATE </v>
+        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
       </c>
       <c r="J88" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`delivery_date` DATE </v>
+        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="89" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A89" s="34"/>
       <c r="B89" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C89" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>9</v>
@@ -4403,148 +4416,148 @@
       <c r="H89" s="38"/>
       <c r="I89" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`sales_date` DATE </v>
+        <v xml:space="preserve">,`delivery_date` DATE </v>
       </c>
       <c r="J89" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`sales_date` DATE </v>
+        <v xml:space="preserve">,`delivery_date` DATE </v>
       </c>
     </row>
     <row r="90" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A90" s="34"/>
       <c r="B90" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C90" s="35" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D90" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E90" s="36">
-        <v>64</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E90" s="36"/>
       <c r="F90" s="35"/>
       <c r="G90" s="37"/>
       <c r="H90" s="38"/>
       <c r="I90" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
+        <v xml:space="preserve">,`sales_date` DATE </v>
       </c>
       <c r="J90" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
+        <v xml:space="preserve">,`sales_date` DATE </v>
       </c>
     </row>
     <row r="91" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A91" s="34"/>
       <c r="B91" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C91" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D91" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E91" s="36">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="F91" s="35"/>
       <c r="G91" s="37"/>
       <c r="H91" s="38"/>
       <c r="I91" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
+        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
       </c>
       <c r="J91" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
+        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
       </c>
     </row>
     <row r="92" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A92" s="34"/>
       <c r="B92" s="39" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="D92" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E92" s="36">
-        <v>20</v>
+        <v>256</v>
       </c>
       <c r="F92" s="35"/>
       <c r="G92" s="37"/>
       <c r="H92" s="38"/>
       <c r="I92" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
+        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
       </c>
       <c r="J92" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
+        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
       </c>
     </row>
     <row r="93" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A93" s="34"/>
       <c r="B93" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C93" s="35" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="D93" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E93" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F93" s="35"/>
       <c r="G93" s="37"/>
       <c r="H93" s="38"/>
       <c r="I93" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
       </c>
       <c r="J93" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
       </c>
     </row>
     <row r="94" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A94" s="34"/>
       <c r="B94" s="39" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="C94" s="35" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="D94" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E94" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E94" s="36">
+        <v>256</v>
+      </c>
       <c r="F94" s="35"/>
       <c r="G94" s="37"/>
       <c r="H94" s="38"/>
       <c r="I94" s="40" t="str">
-        <f t="shared" ref="I94:I95" si="18">"," &amp; IF(A94="","","/* ") &amp; "`" &amp; C94 &amp; "` " &amp; D94 &amp; IF(E94&gt;0,"(" &amp; E94 &amp; ") "," ") &amp; IF(F94&lt;&gt;"","NOT NULL ","") &amp; IF(G94="","","DEFAULT '" &amp; G94 &amp; "' ") &amp; IF(A94="",""," */")</f>
-        <v xml:space="preserve">,`quantity` INT </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
       <c r="J94" s="41" t="str">
-        <f t="shared" ref="J94:J95" si="19">"," &amp; IF(A94="","","/* ") &amp; "`" &amp; C94 &amp; "` " &amp; D94 &amp; IF(E94&gt;0,"(" &amp; E94 &amp; ") "," ") &amp; IF(F94&lt;&gt;"","NOT NULL ","") &amp; IF(G94="","","DEFAULT '" &amp; G94 &amp; "' ") &amp; IF(A94="",""," */")</f>
-        <v xml:space="preserve">,`quantity` INT </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="95" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A95" s="34"/>
       <c r="B95" s="39" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="D95" s="35" t="s">
         <v>5</v>
@@ -4554,100 +4567,100 @@
       <c r="G95" s="37"/>
       <c r="H95" s="38"/>
       <c r="I95" s="40" t="str">
+        <f t="shared" ref="I95:I96" si="18">"," &amp; IF(A95="","","/* ") &amp; "`" &amp; C95 &amp; "` " &amp; D95 &amp; IF(E95&gt;0,"(" &amp; E95 &amp; ") "," ") &amp; IF(F95&lt;&gt;"","NOT NULL ","") &amp; IF(G95="","","DEFAULT '" &amp; G95 &amp; "' ") &amp; IF(A95="",""," */")</f>
+        <v xml:space="preserve">,`quantity` INT </v>
+      </c>
+      <c r="J95" s="41" t="str">
+        <f t="shared" ref="J95:J96" si="19">"," &amp; IF(A95="","","/* ") &amp; "`" &amp; C95 &amp; "` " &amp; D95 &amp; IF(E95&gt;0,"(" &amp; E95 &amp; ") "," ") &amp; IF(F95&lt;&gt;"","NOT NULL ","") &amp; IF(G95="","","DEFAULT '" &amp; G95 &amp; "' ") &amp; IF(A95="",""," */")</f>
+        <v xml:space="preserve">,`quantity` INT </v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A96" s="34"/>
+      <c r="B96" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C96" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="D96" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" s="36"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="38"/>
+      <c r="I96" s="40" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">,`price` INT </v>
       </c>
-      <c r="J95" s="41" t="str">
+      <c r="J96" s="41" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">,`price` INT </v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A96" s="2"/>
-      <c r="B96" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E96" s="7">
-        <v>256</v>
-      </c>
-      <c r="F96" s="6"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="9"/>
-      <c r="I96" s="27" t="str">
-        <f>"," &amp; IF(A96="","","/* ") &amp; "`" &amp; C96 &amp; "` " &amp; D96 &amp; IF(E96&gt;0,"(" &amp; E96 &amp; ") "," ") &amp; IF(F96&lt;&gt;"","NOT NULL ","") &amp; IF(G96="","","DEFAULT '" &amp; G96 &amp; "' ") &amp; IF(A96="",""," */")</f>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
-      </c>
-      <c r="J96" s="29" t="str">
-        <f>"," &amp; IF(A96="","","/* ") &amp; "`" &amp; C96 &amp; "` " &amp; D96 &amp; IF(E96&gt;0,"(" &amp; E96 &amp; ") "," ") &amp; IF(F96&lt;&gt;"","NOT NULL ","") &amp; IF(G96="","","DEFAULT '" &amp; G96 &amp; "' ") &amp; IF(A96="",""," */")</f>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" s="2"/>
       <c r="B97" s="20" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E97" s="7">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="8"/>
       <c r="H97" s="9"/>
       <c r="I97" s="27" t="str">
         <f>"," &amp; IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; IF(A97="",""," */")</f>
-        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
       <c r="J97" s="29" t="str">
         <f>"," &amp; IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; IF(A97="",""," */")</f>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A98" s="2"/>
+      <c r="B98" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="7">
+        <v>128</v>
+      </c>
+      <c r="F98" s="6"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="27" t="str">
+        <f>"," &amp; IF(A98="","","/* ") &amp; "`" &amp; C98 &amp; "` " &amp; D98 &amp; IF(E98&gt;0,"(" &amp; E98 &amp; ") "," ") &amp; IF(F98&lt;&gt;"","NOT NULL ","") &amp; IF(G98="","","DEFAULT '" &amp; G98 &amp; "' ") &amp; IF(A98="",""," */")</f>
         <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
-    </row>
-    <row r="98" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="34"/>
-      <c r="B98" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C98" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="D98" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E98" s="36"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="37"/>
-      <c r="H98" s="38"/>
-      <c r="I98" s="40" t="str">
+      <c r="J98" s="29" t="str">
         <f>"," &amp; IF(A98="","","/* ") &amp; "`" &amp; C98 &amp; "` " &amp; D98 &amp; IF(E98&gt;0,"(" &amp; E98 &amp; ") "," ") &amp; IF(F98&lt;&gt;"","NOT NULL ","") &amp; IF(G98="","","DEFAULT '" &amp; G98 &amp; "' ") &amp; IF(A98="",""," */")</f>
-        <v xml:space="preserve">,`product_detail` TEXT </v>
-      </c>
-      <c r="J98" s="41" t="str">
-        <f>"," &amp; IF(A98="","","/* ") &amp; "`" &amp; C98 &amp; "` " &amp; D98 &amp; IF(E98&gt;0,"(" &amp; E98 &amp; ") "," ") &amp; IF(F98&lt;&gt;"","NOT NULL ","") &amp; IF(G98="","","DEFAULT '" &amp; G98 &amp; "' ") &amp; IF(A98="",""," */")</f>
-        <v xml:space="preserve">,`product_detail` TEXT </v>
+        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
     </row>
     <row r="99" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A99" s="34"/>
       <c r="B99" s="39" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C99" s="35" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D99" s="35" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E99" s="36"/>
       <c r="F99" s="35"/>
@@ -4655,46 +4668,44 @@
       <c r="H99" s="38"/>
       <c r="I99" s="40" t="str">
         <f>"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`product_detail` TEXT </v>
       </c>
       <c r="J99" s="41" t="str">
         <f>"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
+        <v xml:space="preserve">,`product_detail` TEXT </v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="34"/>
+      <c r="B100" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D100" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E100" s="36"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="38"/>
+      <c r="I100" s="40" t="str">
+        <f>"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
         <v xml:space="preserve">,`status_id` INT </v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A100" s="2"/>
-      <c r="B100" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E100" s="7">
-        <v>256</v>
-      </c>
-      <c r="F100" s="6"/>
-      <c r="G100" s="8"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="27" t="str">
-        <f t="shared" ref="I100:I106" si="20">"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
-      </c>
-      <c r="J100" s="29" t="str">
-        <f t="shared" ref="J100:J106" si="21">"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+      <c r="J100" s="41" t="str">
+        <f>"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" s="2"/>
       <c r="B101" s="43" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>7</v>
@@ -4706,98 +4717,100 @@
       <c r="G101" s="8"/>
       <c r="H101" s="9"/>
       <c r="I101" s="27" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" ref="I101:I107" si="20">"," &amp; IF(A101="","","/* ") &amp; "`" &amp; C101 &amp; "` " &amp; D101 &amp; IF(E101&gt;0,"(" &amp; E101 &amp; ") "," ") &amp; IF(F101&lt;&gt;"","NOT NULL ","") &amp; IF(G101="","","DEFAULT '" &amp; G101 &amp; "' ") &amp; IF(A101="",""," */")</f>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J101" s="29" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" ref="J101:J107" si="21">"," &amp; IF(A101="","","/* ") &amp; "`" &amp; C101 &amp; "` " &amp; D101 &amp; IF(E101&gt;0,"(" &amp; E101 &amp; ") "," ") &amp; IF(F101&lt;&gt;"","NOT NULL ","") &amp; IF(G101="","","DEFAULT '" &amp; G101 &amp; "' ") &amp; IF(A101="",""," */")</f>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="2"/>
       <c r="B102" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E102" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="E102" s="7">
+        <v>256</v>
+      </c>
       <c r="F102" s="6"/>
       <c r="G102" s="8"/>
       <c r="H102" s="9"/>
       <c r="I102" s="27" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J102" s="29" t="str">
         <f t="shared" si="21"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="2"/>
       <c r="B103" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E103" s="7">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E103" s="7"/>
       <c r="F103" s="6"/>
       <c r="G103" s="8"/>
       <c r="H103" s="9"/>
       <c r="I103" s="27" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
       <c r="J103" s="29" t="str">
         <f t="shared" si="21"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A104" s="2"/>
+      <c r="B104" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="7">
+        <v>64</v>
+      </c>
+      <c r="F104" s="6"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="27" t="str">
+        <f t="shared" si="20"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
-    </row>
-    <row r="104" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="34"/>
-      <c r="B104" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="C104" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D104" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E104" s="36"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="37"/>
-      <c r="H104" s="38"/>
-      <c r="I104" s="40" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-      <c r="J104" s="41" t="str">
+      <c r="J104" s="29" t="str">
         <f t="shared" si="21"/>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
     <row r="105" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A105" s="34"/>
       <c r="B105" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C105" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D105" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E105" s="36"/>
       <c r="F105" s="35"/>
@@ -4805,20 +4818,20 @@
       <c r="H105" s="38"/>
       <c r="I105" s="40" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J105" s="41" t="str">
         <f t="shared" si="21"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="106" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A106" s="34"/>
       <c r="B106" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C106" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D106" s="35" t="s">
         <v>8</v>
@@ -4829,143 +4842,143 @@
       <c r="H106" s="38"/>
       <c r="I106" s="40" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J106" s="41" t="str">
         <f t="shared" si="21"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A107" s="34"/>
+      <c r="B107" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C107" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D107" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="36"/>
+      <c r="F107" s="35"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="38"/>
+      <c r="I107" s="40" t="str">
+        <f t="shared" si="20"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A107" s="2"/>
-      <c r="B107" s="21"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="23"/>
-      <c r="H107" s="21"/>
-      <c r="I107" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J107" s="29" t="s">
-        <v>33</v>
+      <c r="J107" s="41" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108" s="2"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="23"/>
+      <c r="H108" s="21"/>
+      <c r="I108" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J108" s="29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" s="2"/>
-      <c r="B109" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C109" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D109" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F109" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G109" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H109" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I109" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C109 &amp; "` ("</f>
-        <v>CREATE TABLE `licenses` (</v>
-      </c>
-      <c r="J109" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C109 &amp; "` ("</f>
-        <v>CREATE TABLE `licenses` (</v>
-      </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A110" s="2"/>
-      <c r="B110" s="20" t="s">
+      <c r="B110" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C110" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F110" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G110" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H110" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I110" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C110 &amp; "` ("</f>
+        <v>CREATE TABLE `licenses` (</v>
+      </c>
+      <c r="J110" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C110 &amp; "` ("</f>
+        <v>CREATE TABLE `licenses` (</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A111" s="2"/>
+      <c r="B111" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C111" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D110" s="6" t="s">
+      <c r="D111" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E110" s="7"/>
-      <c r="F110" s="6" t="s">
+      <c r="E111" s="7"/>
+      <c r="F111" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G110" s="8"/>
-      <c r="H110" s="9"/>
-      <c r="I110" s="28" t="s">
+      <c r="G111" s="8"/>
+      <c r="H111" s="9"/>
+      <c r="I111" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J110" s="30" t="s">
+      <c r="J111" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A111" s="34"/>
-      <c r="B111" s="39" t="s">
+    <row r="112" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A112" s="34"/>
+      <c r="B112" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C111" s="35" t="s">
+      <c r="C112" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D111" s="35" t="s">
+      <c r="D112" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E111" s="36"/>
-      <c r="F111" s="35"/>
-      <c r="G111" s="37"/>
-      <c r="H111" s="38"/>
-      <c r="I111" s="40" t="str">
-        <f>"," &amp; IF(A111="","","/* ") &amp; "`" &amp; C111 &amp; "` " &amp; D111 &amp; IF(E111&gt;0,"(" &amp; E111 &amp; ") "," ") &amp; IF(F111&lt;&gt;"","NOT NULL ","") &amp; IF(G111="","","DEFAULT '" &amp; G111 &amp; "' ") &amp; IF(A111="",""," */")</f>
+      <c r="E112" s="36"/>
+      <c r="F112" s="35"/>
+      <c r="G112" s="37"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="40" t="str">
+        <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT </v>
       </c>
-      <c r="J111" s="41" t="str">
-        <f>"," &amp; IF(A111="","","/* ") &amp; "`" &amp; C111 &amp; "` " &amp; D111 &amp; IF(E111&gt;0,"(" &amp; E111 &amp; ") "," ") &amp; IF(F111&lt;&gt;"","NOT NULL ","") &amp; IF(G111="","","DEFAULT '" &amp; G111 &amp; "' ") &amp; IF(A111="",""," */")</f>
+      <c r="J112" s="41" t="str">
+        <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT </v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A112" s="2"/>
-      <c r="B112" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E112" s="7"/>
-      <c r="F112" s="6"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="9"/>
-      <c r="I112" s="27" t="str">
-        <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
-      </c>
-      <c r="J112" s="29" t="str">
-        <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A113" s="2"/>
       <c r="B113" s="20" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>5</v>
@@ -4976,20 +4989,20 @@
       <c r="H113" s="9"/>
       <c r="I113" s="27" t="str">
         <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
       <c r="J113" s="29" t="str">
         <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A114" s="2"/>
       <c r="B114" s="20" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>5</v>
@@ -5000,220 +5013,220 @@
       <c r="H114" s="9"/>
       <c r="I114" s="27" t="str">
         <f>"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
       <c r="J114" s="29" t="str">
         <f>"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A115" s="2"/>
       <c r="B115" s="20" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E115" s="7"/>
       <c r="F115" s="6"/>
       <c r="G115" s="8"/>
       <c r="H115" s="9"/>
       <c r="I115" s="27" t="str">
-        <f t="shared" ref="I115:I121" si="22">"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
       <c r="J115" s="29" t="str">
-        <f t="shared" ref="J115:J121" si="23">"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A116" s="2"/>
       <c r="B116" s="20" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E116" s="7">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E116" s="7"/>
       <c r="F116" s="6"/>
       <c r="G116" s="8"/>
       <c r="H116" s="9"/>
       <c r="I116" s="27" t="str">
-        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
+        <f t="shared" ref="I116:I122" si="22">"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
+      </c>
+      <c r="J116" s="29" t="str">
+        <f t="shared" ref="J116:J122" si="23">"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A117" s="2"/>
+      <c r="B117" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="7">
+        <v>20</v>
+      </c>
+      <c r="F117" s="6"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="27" t="str">
+        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
         <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
-      <c r="J116" s="29" t="str">
-        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
+      <c r="J117" s="29" t="str">
+        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
         <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A117" s="34"/>
-      <c r="B117" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="C117" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D117" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E117" s="36">
-        <v>20</v>
-      </c>
-      <c r="F117" s="35"/>
-      <c r="G117" s="37"/>
-      <c r="H117" s="38"/>
-      <c r="I117" s="40" t="str">
-        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
-      </c>
-      <c r="J117" s="41" t="str">
-        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="118" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A118" s="34"/>
       <c r="B118" s="39" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="C118" s="35" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D118" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E118" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F118" s="35"/>
       <c r="G118" s="37"/>
       <c r="H118" s="38"/>
       <c r="I118" s="40" t="str">
+        <f>"," &amp; IF(A118="","","/* ") &amp; "`" &amp; C118 &amp; "` " &amp; D118 &amp; IF(E118&gt;0,"(" &amp; E118 &amp; ") "," ") &amp; IF(F118&lt;&gt;"","NOT NULL ","") &amp; IF(G118="","","DEFAULT '" &amp; G118 &amp; "' ") &amp; IF(A118="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+      </c>
+      <c r="J118" s="41" t="str">
+        <f>"," &amp; IF(A118="","","/* ") &amp; "`" &amp; C118 &amp; "` " &amp; D118 &amp; IF(E118&gt;0,"(" &amp; E118 &amp; ") "," ") &amp; IF(F118&lt;&gt;"","NOT NULL ","") &amp; IF(G118="","","DEFAULT '" &amp; G118 &amp; "' ") &amp; IF(A118="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A119" s="34"/>
+      <c r="B119" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C119" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D119" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="36">
+        <v>256</v>
+      </c>
+      <c r="F119" s="35"/>
+      <c r="G119" s="37"/>
+      <c r="H119" s="38"/>
+      <c r="I119" s="40" t="str">
         <f t="shared" si="22"/>
         <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
-      <c r="J118" s="41" t="str">
+      <c r="J119" s="41" t="str">
         <f t="shared" si="23"/>
         <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A119" s="2"/>
-      <c r="B119" s="20" t="s">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A120" s="2"/>
+      <c r="B120" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C119" s="6" t="s">
+      <c r="C120" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D119" s="6" t="s">
+      <c r="D120" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E119" s="7">
+      <c r="E120" s="7">
         <v>256</v>
       </c>
-      <c r="F119" s="6"/>
-      <c r="G119" s="8"/>
-      <c r="H119" s="9"/>
-      <c r="I119" s="27" t="str">
+      <c r="F120" s="6"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="27" t="str">
         <f t="shared" si="22"/>
         <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
-      <c r="J119" s="29" t="str">
+      <c r="J120" s="29" t="str">
         <f t="shared" si="23"/>
         <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
     </row>
-    <row r="120" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A120" s="34"/>
-      <c r="B120" s="39" t="s">
+    <row r="121" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A121" s="34"/>
+      <c r="B121" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="C120" s="35" t="s">
+      <c r="C121" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="D120" s="35" t="s">
+      <c r="D121" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E120" s="36"/>
-      <c r="F120" s="35"/>
-      <c r="G120" s="37"/>
-      <c r="H120" s="38"/>
-      <c r="I120" s="40" t="str">
-        <f t="shared" ref="I120" si="24">"," &amp; IF(A120="","","/* ") &amp; "`" &amp; C120 &amp; "` " &amp; D120 &amp; IF(E120&gt;0,"(" &amp; E120 &amp; ") "," ") &amp; IF(F120&lt;&gt;"","NOT NULL ","") &amp; IF(G120="","","DEFAULT '" &amp; G120 &amp; "' ") &amp; IF(A120="",""," */")</f>
+      <c r="E121" s="36"/>
+      <c r="F121" s="35"/>
+      <c r="G121" s="37"/>
+      <c r="H121" s="38"/>
+      <c r="I121" s="40" t="str">
+        <f t="shared" ref="I121" si="24">"," &amp; IF(A121="","","/* ") &amp; "`" &amp; C121 &amp; "` " &amp; D121 &amp; IF(E121&gt;0,"(" &amp; E121 &amp; ") "," ") &amp; IF(F121&lt;&gt;"","NOT NULL ","") &amp; IF(G121="","","DEFAULT '" &amp; G121 &amp; "' ") &amp; IF(A121="",""," */")</f>
         <v xml:space="preserve">,`language_id` INT </v>
       </c>
-      <c r="J120" s="41" t="str">
-        <f t="shared" ref="J120" si="25">"," &amp; IF(A120="","","/* ") &amp; "`" &amp; C120 &amp; "` " &amp; D120 &amp; IF(E120&gt;0,"(" &amp; E120 &amp; ") "," ") &amp; IF(F120&lt;&gt;"","NOT NULL ","") &amp; IF(G120="","","DEFAULT '" &amp; G120 &amp; "' ") &amp; IF(A120="",""," */")</f>
+      <c r="J121" s="41" t="str">
+        <f t="shared" ref="J121" si="25">"," &amp; IF(A121="","","/* ") &amp; "`" &amp; C121 &amp; "` " &amp; D121 &amp; IF(E121&gt;0,"(" &amp; E121 &amp; ") "," ") &amp; IF(F121&lt;&gt;"","NOT NULL ","") &amp; IF(G121="","","DEFAULT '" &amp; G121 &amp; "' ") &amp; IF(A121="",""," */")</f>
         <v xml:space="preserve">,`language_id` INT </v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A121" s="2"/>
-      <c r="B121" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E121" s="7"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="8"/>
-      <c r="H121" s="9"/>
-      <c r="I121" s="27" t="str">
-        <f t="shared" si="22"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
-      </c>
-      <c r="J121" s="29" t="str">
-        <f t="shared" si="23"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A122" s="2"/>
       <c r="B122" s="20" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E122" s="7"/>
       <c r="F122" s="6"/>
       <c r="G122" s="8"/>
       <c r="H122" s="9"/>
       <c r="I122" s="27" t="str">
-        <f t="shared" ref="I122" si="26">"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
       <c r="J122" s="29" t="str">
-        <f t="shared" ref="J122" si="27">"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A123" s="2"/>
       <c r="B123" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>9</v>
@@ -5223,97 +5236,95 @@
       <c r="G123" s="8"/>
       <c r="H123" s="9"/>
       <c r="I123" s="27" t="str">
-        <f>"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
+        <f t="shared" ref="I123" si="26">"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
+        <v xml:space="preserve">,`startdate` DATE </v>
+      </c>
+      <c r="J123" s="29" t="str">
+        <f t="shared" ref="J123" si="27">"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
+        <v xml:space="preserve">,`startdate` DATE </v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A124" s="2"/>
+      <c r="B124" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="7"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="8"/>
+      <c r="H124" s="9"/>
+      <c r="I124" s="27" t="str">
+        <f>"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
         <v xml:space="preserve">,`enddate` DATE </v>
       </c>
-      <c r="J123" s="29" t="str">
-        <f>"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
+      <c r="J124" s="29" t="str">
+        <f>"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
         <v xml:space="preserve">,`enddate` DATE </v>
       </c>
     </row>
-    <row r="124" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A124" s="34"/>
-      <c r="B124" s="39" t="s">
+    <row r="125" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A125" s="34"/>
+      <c r="B125" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="C124" s="35" t="s">
+      <c r="C125" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="D124" s="35" t="s">
+      <c r="D125" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E124" s="36">
+      <c r="E125" s="36">
         <v>256</v>
       </c>
-      <c r="F124" s="35"/>
-      <c r="G124" s="37"/>
-      <c r="H124" s="38"/>
-      <c r="I124" s="40" t="str">
-        <f t="shared" ref="I124" si="28">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
+      <c r="F125" s="35"/>
+      <c r="G125" s="37"/>
+      <c r="H125" s="38"/>
+      <c r="I125" s="40" t="str">
+        <f t="shared" ref="I125" si="28">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
         <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
-      <c r="J124" s="41" t="str">
-        <f t="shared" ref="J124" si="29">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
+      <c r="J125" s="41" t="str">
+        <f t="shared" ref="J125" si="29">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
         <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A125" s="2"/>
-      <c r="B125" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D125" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E125" s="7"/>
-      <c r="F125" s="6"/>
-      <c r="G125" s="8"/>
-      <c r="H125" s="9"/>
-      <c r="I125" s="27" t="str">
-        <f t="shared" ref="I125:I132" si="30">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
-        <v xml:space="preserve">,`notice` TEXT </v>
-      </c>
-      <c r="J125" s="29" t="str">
-        <f t="shared" ref="J125:J132" si="31">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
-        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A126" s="2"/>
-      <c r="B126" s="43" t="s">
-        <v>87</v>
+      <c r="B126" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E126" s="7">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E126" s="7"/>
       <c r="F126" s="6"/>
       <c r="G126" s="8"/>
       <c r="H126" s="9"/>
       <c r="I126" s="27" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" ref="I126:I133" si="30">"," &amp; IF(A126="","","/* ") &amp; "`" &amp; C126 &amp; "` " &amp; D126 &amp; IF(E126&gt;0,"(" &amp; E126 &amp; ") "," ") &amp; IF(F126&lt;&gt;"","NOT NULL ","") &amp; IF(G126="","","DEFAULT '" &amp; G126 &amp; "' ") &amp; IF(A126="",""," */")</f>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
       <c r="J126" s="29" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" ref="J126:J133" si="31">"," &amp; IF(A126="","","/* ") &amp; "`" &amp; C126 &amp; "` " &amp; D126 &amp; IF(E126&gt;0,"(" &amp; E126 &amp; ") "," ") &amp; IF(F126&lt;&gt;"","NOT NULL ","") &amp; IF(G126="","","DEFAULT '" &amp; G126 &amp; "' ") &amp; IF(A126="",""," */")</f>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A127" s="2"/>
       <c r="B127" s="43" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>7</v>
@@ -5326,118 +5337,120 @@
       <c r="H127" s="9"/>
       <c r="I127" s="27" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J127" s="29" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A128" s="2"/>
       <c r="B128" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E128" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="E128" s="7">
+        <v>256</v>
+      </c>
       <c r="F128" s="6"/>
       <c r="G128" s="8"/>
       <c r="H128" s="9"/>
       <c r="I128" s="27" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J128" s="29" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129" s="2"/>
       <c r="B129" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E129" s="7">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E129" s="7"/>
       <c r="F129" s="6"/>
       <c r="G129" s="8"/>
       <c r="H129" s="9"/>
       <c r="I129" s="27" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
       <c r="J129" s="29" t="str">
         <f t="shared" si="31"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A130" s="2"/>
+      <c r="B130" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E130" s="7">
+        <v>64</v>
+      </c>
+      <c r="F130" s="6"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="9"/>
+      <c r="I130" s="27" t="str">
+        <f t="shared" si="30"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
-    </row>
-    <row r="130" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A130" s="34"/>
-      <c r="B130" s="43" t="s">
+      <c r="J130" s="29" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A131" s="34"/>
+      <c r="B131" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="C130" s="35" t="s">
+      <c r="C131" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="D130" s="35" t="s">
+      <c r="D131" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="E130" s="36"/>
-      <c r="F130" s="35"/>
-      <c r="G130" s="37"/>
-      <c r="H130" s="38"/>
-      <c r="I130" s="40" t="str">
+      <c r="E131" s="36"/>
+      <c r="F131" s="35"/>
+      <c r="G131" s="37"/>
+      <c r="H131" s="38"/>
+      <c r="I131" s="40" t="str">
         <f t="shared" si="30"/>
         <v xml:space="preserve">,`user_id` INT </v>
       </c>
-      <c r="J130" s="41" t="str">
+      <c r="J131" s="41" t="str">
         <f t="shared" si="31"/>
         <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A131" s="2"/>
-      <c r="B131" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E131" s="7"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="9"/>
-      <c r="I131" s="27" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
-      </c>
-      <c r="J131" s="29" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" s="2"/>
       <c r="B132" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>8</v>
@@ -5448,119 +5461,119 @@
       <c r="H132" s="9"/>
       <c r="I132" s="27" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J132" s="29" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" s="2"/>
-      <c r="B133" s="21"/>
-      <c r="C133" s="21"/>
-      <c r="D133" s="21"/>
-      <c r="E133" s="22"/>
-      <c r="F133" s="21"/>
-      <c r="G133" s="23"/>
-      <c r="H133" s="21"/>
-      <c r="I133" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J133" s="29" t="s">
-        <v>33</v>
+      <c r="B133" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" s="7"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="27" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
+      </c>
+      <c r="J133" s="29" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" s="2"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="21"/>
+      <c r="D134" s="21"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="21"/>
+      <c r="G134" s="23"/>
+      <c r="H134" s="21"/>
+      <c r="I134" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J134" s="29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" s="2"/>
-      <c r="B135" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C135" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D135" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E135" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F135" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G135" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H135" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I135" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C135 &amp; "` ("</f>
-        <v>CREATE TABLE `licensehistories` (</v>
-      </c>
-      <c r="J135" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C135 &amp; "` ("</f>
-        <v>CREATE TABLE `licensehistories` (</v>
-      </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" s="2"/>
-      <c r="B136" s="20" t="s">
+      <c r="B136" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C136" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D136" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E136" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F136" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G136" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H136" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I136" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C136 &amp; "` ("</f>
+        <v>CREATE TABLE `licensehistories` (</v>
+      </c>
+      <c r="J136" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C136 &amp; "` ("</f>
+        <v>CREATE TABLE `licensehistories` (</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A137" s="2"/>
+      <c r="B137" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C137" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="6" t="s">
+      <c r="D137" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E136" s="7"/>
-      <c r="F136" s="6" t="s">
+      <c r="E137" s="7"/>
+      <c r="F137" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G136" s="8"/>
-      <c r="H136" s="9"/>
-      <c r="I136" s="28" t="s">
+      <c r="G137" s="8"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J136" s="30" t="s">
+      <c r="J137" s="30" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A137" s="34"/>
-      <c r="B137" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C137" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D137" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E137" s="36"/>
-      <c r="F137" s="35"/>
-      <c r="G137" s="37"/>
-      <c r="H137" s="38"/>
-      <c r="I137" s="40" t="str">
-        <f>"," &amp; IF(A137="","","/* ") &amp; "`" &amp; C137 &amp; "` " &amp; D137 &amp; IF(E137&gt;0,"(" &amp; E137 &amp; ") "," ") &amp; IF(F137&lt;&gt;"","NOT NULL ","") &amp; IF(G137="","","DEFAULT '" &amp; G137 &amp; "' ") &amp; IF(A137="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT </v>
-      </c>
-      <c r="J137" s="41" t="str">
-        <f>"," &amp; IF(A137="","","/* ") &amp; "`" &amp; C137 &amp; "` " &amp; D137 &amp; IF(E137&gt;0,"(" &amp; E137 &amp; ") "," ") &amp; IF(F137&lt;&gt;"","NOT NULL ","") &amp; IF(G137="","","DEFAULT '" &amp; G137 &amp; "' ") &amp; IF(A137="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT </v>
       </c>
     </row>
     <row r="138" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A138" s="34"/>
       <c r="B138" s="39" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C138" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D138" s="35" t="s">
         <v>5</v>
@@ -5571,20 +5584,20 @@
       <c r="H138" s="38"/>
       <c r="I138" s="40" t="str">
         <f>"," &amp; IF(A138="","","/* ") &amp; "`" &amp; C138 &amp; "` " &amp; D138 &amp; IF(E138&gt;0,"(" &amp; E138 &amp; ") "," ") &amp; IF(F138&lt;&gt;"","NOT NULL ","") &amp; IF(G138="","","DEFAULT '" &amp; G138 &amp; "' ") &amp; IF(A138="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <v xml:space="preserve">,`client_id` INT </v>
       </c>
       <c r="J138" s="41" t="str">
         <f>"," &amp; IF(A138="","","/* ") &amp; "`" &amp; C138 &amp; "` " &amp; D138 &amp; IF(E138&gt;0,"(" &amp; E138 &amp; ") "," ") &amp; IF(F138&lt;&gt;"","NOT NULL ","") &amp; IF(G138="","","DEFAULT '" &amp; G138 &amp; "' ") &amp; IF(A138="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <v xml:space="preserve">,`client_id` INT </v>
       </c>
     </row>
     <row r="139" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A139" s="34"/>
       <c r="B139" s="39" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C139" s="35" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D139" s="35" t="s">
         <v>5</v>
@@ -5595,20 +5608,20 @@
       <c r="H139" s="38"/>
       <c r="I139" s="40" t="str">
         <f>"," &amp; IF(A139="","","/* ") &amp; "`" &amp; C139 &amp; "` " &amp; D139 &amp; IF(E139&gt;0,"(" &amp; E139 &amp; ") "," ") &amp; IF(F139&lt;&gt;"","NOT NULL ","") &amp; IF(G139="","","DEFAULT '" &amp; G139 &amp; "' ") &amp; IF(A139="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
       <c r="J139" s="41" t="str">
         <f>"," &amp; IF(A139="","","/* ") &amp; "`" &amp; C139 &amp; "` " &amp; D139 &amp; IF(E139&gt;0,"(" &amp; E139 &amp; ") "," ") &amp; IF(F139&lt;&gt;"","NOT NULL ","") &amp; IF(G139="","","DEFAULT '" &amp; G139 &amp; "' ") &amp; IF(A139="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="140" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A140" s="34"/>
       <c r="B140" s="39" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C140" s="35" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D140" s="35" t="s">
         <v>5</v>
@@ -5619,70 +5632,68 @@
       <c r="H140" s="38"/>
       <c r="I140" s="40" t="str">
         <f>"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
       <c r="J140" s="41" t="str">
         <f>"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
     </row>
     <row r="141" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A141" s="34"/>
       <c r="B141" s="39" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C141" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D141" s="35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E141" s="36"/>
       <c r="F141" s="35"/>
       <c r="G141" s="37"/>
       <c r="H141" s="38"/>
       <c r="I141" s="40" t="str">
-        <f t="shared" ref="I141" si="32">"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
       <c r="J141" s="41" t="str">
-        <f t="shared" ref="J141" si="33">"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="142" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A142" s="34"/>
       <c r="B142" s="39" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C142" s="35" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D142" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E142" s="36">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E142" s="36"/>
       <c r="F142" s="35"/>
       <c r="G142" s="37"/>
       <c r="H142" s="38"/>
       <c r="I142" s="40" t="str">
-        <f>"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
-        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
+        <f t="shared" ref="I142" si="32">"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
       </c>
       <c r="J142" s="41" t="str">
-        <f>"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
-        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
+        <f t="shared" ref="J142" si="33">"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
       </c>
     </row>
     <row r="143" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A143" s="34"/>
       <c r="B143" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C143" s="35" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="D143" s="35" t="s">
         <v>7</v>
@@ -5695,46 +5706,46 @@
       <c r="H143" s="38"/>
       <c r="I143" s="40" t="str">
         <f>"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
       <c r="J143" s="41" t="str">
         <f>"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="144" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A144" s="34"/>
       <c r="B144" s="39" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="C144" s="35" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D144" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E144" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F144" s="35"/>
       <c r="G144" s="37"/>
       <c r="H144" s="38"/>
       <c r="I144" s="40" t="str">
-        <f t="shared" ref="I144:I148" si="34">"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f>"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
       <c r="J144" s="41" t="str">
-        <f t="shared" ref="J144:J148" si="35">"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f>"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="145" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A145" s="34"/>
       <c r="B145" s="39" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="C145" s="35" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="D145" s="35" t="s">
         <v>7</v>
@@ -5746,48 +5757,50 @@
       <c r="G145" s="37"/>
       <c r="H145" s="38"/>
       <c r="I145" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
+        <f t="shared" ref="I145:I149" si="34">"," &amp; IF(A145="","","/* ") &amp; "`" &amp; C145 &amp; "` " &amp; D145 &amp; IF(E145&gt;0,"(" &amp; E145 &amp; ") "," ") &amp; IF(F145&lt;&gt;"","NOT NULL ","") &amp; IF(G145="","","DEFAULT '" &amp; G145 &amp; "' ") &amp; IF(A145="",""," */")</f>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
       <c r="J145" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
+        <f t="shared" ref="J145:J149" si="35">"," &amp; IF(A145="","","/* ") &amp; "`" &amp; C145 &amp; "` " &amp; D145 &amp; IF(E145&gt;0,"(" &amp; E145 &amp; ") "," ") &amp; IF(F145&lt;&gt;"","NOT NULL ","") &amp; IF(G145="","","DEFAULT '" &amp; G145 &amp; "' ") &amp; IF(A145="",""," */")</f>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="146" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A146" s="34"/>
       <c r="B146" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C146" s="35" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="D146" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E146" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E146" s="36">
+        <v>256</v>
+      </c>
       <c r="F146" s="35"/>
       <c r="G146" s="37"/>
       <c r="H146" s="38"/>
       <c r="I146" s="40" t="str">
         <f t="shared" si="34"/>
-        <v xml:space="preserve">,`language_id` INT </v>
+        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
       <c r="J146" s="41" t="str">
         <f t="shared" si="35"/>
-        <v xml:space="preserve">,`language_id` INT </v>
+        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="147" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A147" s="34"/>
       <c r="B147" s="39" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="C147" s="35" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="D147" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E147" s="36"/>
       <c r="F147" s="35"/>
@@ -5795,23 +5808,23 @@
       <c r="H147" s="38"/>
       <c r="I147" s="40" t="str">
         <f t="shared" si="34"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
+        <v xml:space="preserve">,`language_id` INT </v>
       </c>
       <c r="J147" s="41" t="str">
         <f t="shared" si="35"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
+        <v xml:space="preserve">,`language_id` INT </v>
       </c>
     </row>
     <row r="148" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A148" s="34"/>
       <c r="B148" s="39" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C148" s="35" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D148" s="35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E148" s="36"/>
       <c r="F148" s="35"/>
@@ -5819,20 +5832,20 @@
       <c r="H148" s="38"/>
       <c r="I148" s="40" t="str">
         <f t="shared" si="34"/>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
       <c r="J148" s="41" t="str">
         <f t="shared" si="35"/>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="149" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A149" s="34"/>
       <c r="B149" s="39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C149" s="35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D149" s="35" t="s">
         <v>9</v>
@@ -5842,97 +5855,95 @@
       <c r="G149" s="37"/>
       <c r="H149" s="38"/>
       <c r="I149" s="40" t="str">
-        <f>"," &amp; IF(A149="","","/* ") &amp; "`" &amp; C149 &amp; "` " &amp; D149 &amp; IF(E149&gt;0,"(" &amp; E149 &amp; ") "," ") &amp; IF(F149&lt;&gt;"","NOT NULL ","") &amp; IF(G149="","","DEFAULT '" &amp; G149 &amp; "' ") &amp; IF(A149="",""," */")</f>
-        <v xml:space="preserve">,`enddate` DATE </v>
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">,`startdate` DATE </v>
       </c>
       <c r="J149" s="41" t="str">
-        <f>"," &amp; IF(A149="","","/* ") &amp; "`" &amp; C149 &amp; "` " &amp; D149 &amp; IF(E149&gt;0,"(" &amp; E149 &amp; ") "," ") &amp; IF(F149&lt;&gt;"","NOT NULL ","") &amp; IF(G149="","","DEFAULT '" &amp; G149 &amp; "' ") &amp; IF(A149="",""," */")</f>
-        <v xml:space="preserve">,`enddate` DATE </v>
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">,`startdate` DATE </v>
       </c>
     </row>
     <row r="150" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A150" s="34"/>
       <c r="B150" s="39" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="C150" s="35" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="D150" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E150" s="36">
-        <v>256</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E150" s="36"/>
       <c r="F150" s="35"/>
       <c r="G150" s="37"/>
       <c r="H150" s="38"/>
       <c r="I150" s="40" t="str">
-        <f t="shared" ref="I150:I158" si="36">"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
-        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
+        <f>"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
+        <v xml:space="preserve">,`enddate` DATE </v>
       </c>
       <c r="J150" s="41" t="str">
-        <f t="shared" ref="J150:J158" si="37">"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
-        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
+        <f>"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
+        <v xml:space="preserve">,`enddate` DATE </v>
       </c>
     </row>
     <row r="151" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A151" s="34"/>
       <c r="B151" s="39" t="s">
-        <v>29</v>
+        <v>153</v>
       </c>
       <c r="C151" s="35" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="D151" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E151" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E151" s="36">
+        <v>256</v>
+      </c>
       <c r="F151" s="35"/>
       <c r="G151" s="37"/>
       <c r="H151" s="38"/>
       <c r="I151" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`notice` TEXT </v>
+        <f t="shared" ref="I151:I159" si="36">"," &amp; IF(A151="","","/* ") &amp; "`" &amp; C151 &amp; "` " &amp; D151 &amp; IF(E151&gt;0,"(" &amp; E151 &amp; ") "," ") &amp; IF(F151&lt;&gt;"","NOT NULL ","") &amp; IF(G151="","","DEFAULT '" &amp; G151 &amp; "' ") &amp; IF(A151="",""," */")</f>
+        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
       <c r="J151" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`notice` TEXT </v>
+        <f t="shared" ref="J151:J159" si="37">"," &amp; IF(A151="","","/* ") &amp; "`" &amp; C151 &amp; "` " &amp; D151 &amp; IF(E151&gt;0,"(" &amp; E151 &amp; ") "," ") &amp; IF(F151&lt;&gt;"","NOT NULL ","") &amp; IF(G151="","","DEFAULT '" &amp; G151 &amp; "' ") &amp; IF(A151="",""," */")</f>
+        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
     </row>
     <row r="152" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A152" s="34"/>
-      <c r="B152" s="43" t="s">
-        <v>87</v>
+      <c r="B152" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="C152" s="35" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="D152" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E152" s="36">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E152" s="36"/>
       <c r="F152" s="35"/>
       <c r="G152" s="37"/>
       <c r="H152" s="38"/>
       <c r="I152" s="40" t="str">
         <f t="shared" si="36"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
       <c r="J152" s="41" t="str">
         <f t="shared" si="37"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="153" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A153" s="34"/>
       <c r="B153" s="43" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C153" s="35" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="D153" s="35" t="s">
         <v>7</v>
@@ -5945,97 +5956,99 @@
       <c r="H153" s="38"/>
       <c r="I153" s="40" t="str">
         <f t="shared" si="36"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J153" s="41" t="str">
         <f t="shared" si="37"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="154" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A154" s="34"/>
       <c r="B154" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C154" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D154" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E154" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E154" s="36">
+        <v>256</v>
+      </c>
       <c r="F154" s="35"/>
       <c r="G154" s="37"/>
       <c r="H154" s="38"/>
       <c r="I154" s="40" t="str">
         <f t="shared" si="36"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J154" s="41" t="str">
         <f t="shared" si="37"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="155" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A155" s="34"/>
       <c r="B155" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C155" s="35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D155" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E155" s="36">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E155" s="36"/>
       <c r="F155" s="35"/>
       <c r="G155" s="37"/>
       <c r="H155" s="38"/>
       <c r="I155" s="40" t="str">
         <f t="shared" si="36"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
       <c r="J155" s="41" t="str">
         <f t="shared" si="37"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
     </row>
     <row r="156" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A156" s="34"/>
       <c r="B156" s="43" t="s">
-        <v>161</v>
+        <v>52</v>
       </c>
       <c r="C156" s="35" t="s">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="D156" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E156" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E156" s="36">
+        <v>64</v>
+      </c>
       <c r="F156" s="35"/>
       <c r="G156" s="37"/>
       <c r="H156" s="38"/>
       <c r="I156" s="40" t="str">
         <f t="shared" si="36"/>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
       <c r="J156" s="41" t="str">
         <f t="shared" si="37"/>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
     <row r="157" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A157" s="34"/>
       <c r="B157" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C157" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D157" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E157" s="36"/>
       <c r="F157" s="35"/>
@@ -6043,20 +6056,20 @@
       <c r="H157" s="38"/>
       <c r="I157" s="40" t="str">
         <f t="shared" si="36"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J157" s="41" t="str">
         <f t="shared" si="37"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="158" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A158" s="34"/>
       <c r="B158" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C158" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D158" s="35" t="s">
         <v>8</v>
@@ -6067,408 +6080,437 @@
       <c r="H158" s="38"/>
       <c r="I158" s="40" t="str">
         <f t="shared" si="36"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J158" s="41" t="str">
         <f t="shared" si="37"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A159" s="34"/>
+      <c r="B159" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C159" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D159" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" s="36"/>
+      <c r="F159" s="35"/>
+      <c r="G159" s="37"/>
+      <c r="H159" s="38"/>
+      <c r="I159" s="40" t="str">
+        <f t="shared" si="36"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A159" s="2"/>
-      <c r="B159" s="21"/>
-      <c r="C159" s="21"/>
-      <c r="D159" s="21"/>
-      <c r="E159" s="22"/>
-      <c r="F159" s="21"/>
-      <c r="G159" s="23"/>
-      <c r="H159" s="21"/>
-      <c r="I159" s="28" t="s">
+      <c r="J159" s="41" t="str">
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A160" s="2"/>
+      <c r="B160" s="21"/>
+      <c r="C160" s="21"/>
+      <c r="D160" s="21"/>
+      <c r="E160" s="22"/>
+      <c r="F160" s="21"/>
+      <c r="G160" s="23"/>
+      <c r="H160" s="21"/>
+      <c r="I160" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J159" s="29" t="s">
+      <c r="J160" s="29" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="expression" dxfId="75" priority="187">
+    <cfRule type="expression" dxfId="75" priority="188">
       <formula>A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A7 A41:A42 A133:A134 A79:A81 A122:A123 A13:A14 A83:A93 A97:A98 A31:A33 A35 A107:A110 A116:A117">
-    <cfRule type="cellIs" dxfId="74" priority="186" operator="greaterThan">
+  <conditionalFormatting sqref="A5:A7 A42:A43 A134:A135 A80:A82 A123:A124 A13:A14 A84:A94 A98:A99 A31:A33 A35 A108:A111 A117:A118">
+    <cfRule type="cellIs" dxfId="74" priority="187" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A11:A12">
-    <cfRule type="cellIs" dxfId="73" priority="185" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="186" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="cellIs" dxfId="72" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="185" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="71" priority="183" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:A38">
-    <cfRule type="cellIs" dxfId="70" priority="179" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100:A103">
-    <cfRule type="cellIs" dxfId="69" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="184" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:A39">
+    <cfRule type="cellIs" dxfId="70" priority="180" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101:A104">
+    <cfRule type="cellIs" dxfId="69" priority="178" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A126">
+    <cfRule type="cellIs" dxfId="68" priority="177" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="cellIs" dxfId="67" priority="171" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="cellIs" dxfId="66" priority="169" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:A63 A44:A45 A47">
+    <cfRule type="cellIs" dxfId="65" priority="170" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53 A55">
+    <cfRule type="cellIs" dxfId="64" priority="164" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56 A58">
+    <cfRule type="cellIs" dxfId="63" priority="163" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="cellIs" dxfId="62" priority="162" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="cellIs" dxfId="61" priority="161" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="cellIs" dxfId="60" priority="160" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="cellIs" dxfId="59" priority="159" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A122">
+    <cfRule type="cellIs" dxfId="58" priority="156" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A120">
+    <cfRule type="cellIs" dxfId="57" priority="155" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A127:A130">
+    <cfRule type="cellIs" dxfId="56" priority="154" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A132:A133">
+    <cfRule type="cellIs" dxfId="55" priority="153" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A160 A136">
+    <cfRule type="cellIs" dxfId="54" priority="152" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A116">
+    <cfRule type="cellIs" dxfId="53" priority="146" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="cellIs" dxfId="52" priority="138" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="cellIs" dxfId="51" priority="137" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A113">
+    <cfRule type="cellIs" dxfId="50" priority="136" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
+    <cfRule type="cellIs" dxfId="49" priority="135" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:A20 A15:A17">
+    <cfRule type="cellIs" dxfId="48" priority="124" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="cellIs" dxfId="47" priority="120" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="cellIs" dxfId="46" priority="98" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115">
+    <cfRule type="cellIs" dxfId="45" priority="119" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A137">
+    <cfRule type="cellIs" dxfId="44" priority="108" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="cellIs" dxfId="43" priority="90" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" dxfId="42" priority="97" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="cellIs" dxfId="41" priority="96" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="cellIs" dxfId="40" priority="95" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="cellIs" dxfId="39" priority="94" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A119">
+    <cfRule type="cellIs" dxfId="38" priority="93" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A121">
+    <cfRule type="cellIs" dxfId="37" priority="92" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125">
-    <cfRule type="cellIs" dxfId="68" priority="176" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="cellIs" dxfId="67" priority="170" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="66" priority="168" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:A62 A43:A44 A46">
-    <cfRule type="cellIs" dxfId="65" priority="169" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52 A54">
-    <cfRule type="cellIs" dxfId="64" priority="163" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55 A57">
-    <cfRule type="cellIs" dxfId="63" priority="162" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="62" priority="161" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="cellIs" dxfId="61" priority="160" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="cellIs" dxfId="60" priority="159" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="cellIs" dxfId="59" priority="158" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A121">
-    <cfRule type="cellIs" dxfId="58" priority="155" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A119">
-    <cfRule type="cellIs" dxfId="57" priority="154" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A126:A129">
-    <cfRule type="cellIs" dxfId="56" priority="153" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A131:A132">
-    <cfRule type="cellIs" dxfId="55" priority="152" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A159 A135">
-    <cfRule type="cellIs" dxfId="54" priority="151" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A115">
-    <cfRule type="cellIs" dxfId="53" priority="145" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="cellIs" dxfId="52" priority="137" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82">
-    <cfRule type="cellIs" dxfId="51" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="91" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112">
-    <cfRule type="cellIs" dxfId="50" priority="135" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A113">
-    <cfRule type="cellIs" dxfId="49" priority="134" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:A20 A15:A17">
-    <cfRule type="cellIs" dxfId="48" priority="123" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="cellIs" dxfId="47" priority="119" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="cellIs" dxfId="46" priority="97" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A114">
-    <cfRule type="cellIs" dxfId="45" priority="118" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A136">
-    <cfRule type="cellIs" dxfId="44" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="76" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A138">
+    <cfRule type="cellIs" dxfId="34" priority="46" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A149:A150 A143:A144">
+    <cfRule type="cellIs" dxfId="33" priority="59" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A152">
+    <cfRule type="cellIs" dxfId="32" priority="58" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A148">
+    <cfRule type="cellIs" dxfId="31" priority="57" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A146">
+    <cfRule type="cellIs" dxfId="30" priority="56" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A153:A156">
+    <cfRule type="cellIs" dxfId="29" priority="55" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A158:A159">
+    <cfRule type="cellIs" dxfId="28" priority="54" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A142">
+    <cfRule type="cellIs" dxfId="27" priority="53" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A139">
+    <cfRule type="cellIs" dxfId="26" priority="52" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A140">
+    <cfRule type="cellIs" dxfId="25" priority="51" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A141">
+    <cfRule type="cellIs" dxfId="24" priority="50" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A145">
+    <cfRule type="cellIs" dxfId="23" priority="49" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A147">
+    <cfRule type="cellIs" dxfId="22" priority="48" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A151">
+    <cfRule type="cellIs" dxfId="21" priority="47" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78:A79 A64:A65 A69">
+    <cfRule type="cellIs" dxfId="19" priority="45" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:A25 A21:A22">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="cellIs" dxfId="16" priority="37" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:A74">
+    <cfRule type="cellIs" dxfId="15" priority="22" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="cellIs" dxfId="13" priority="34" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106:A107">
+    <cfRule type="cellIs" dxfId="12" priority="33" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76:A77">
+    <cfRule type="cellIs" dxfId="11" priority="32" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:A61">
+    <cfRule type="cellIs" dxfId="10" priority="31" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:A41">
+    <cfRule type="cellIs" dxfId="9" priority="30" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="cellIs" dxfId="8" priority="29" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75">
+    <cfRule type="cellIs" dxfId="7" priority="28" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A157">
+    <cfRule type="cellIs" dxfId="6" priority="25" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A131">
+    <cfRule type="cellIs" dxfId="5" priority="26" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:A30 A26:A27">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="43" priority="89" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="cellIs" dxfId="42" priority="96" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="cellIs" dxfId="41" priority="95" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="cellIs" dxfId="40" priority="94" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="cellIs" dxfId="39" priority="93" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A118">
-    <cfRule type="cellIs" dxfId="38" priority="92" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A120">
-    <cfRule type="cellIs" dxfId="37" priority="91" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A124">
-    <cfRule type="cellIs" dxfId="36" priority="90" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A111">
-    <cfRule type="cellIs" dxfId="35" priority="75" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A137">
-    <cfRule type="cellIs" dxfId="34" priority="45" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A148:A149 A142:A143">
-    <cfRule type="cellIs" dxfId="33" priority="58" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A151">
-    <cfRule type="cellIs" dxfId="32" priority="57" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A147">
-    <cfRule type="cellIs" dxfId="31" priority="56" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A145">
-    <cfRule type="cellIs" dxfId="30" priority="55" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A152:A155">
-    <cfRule type="cellIs" dxfId="29" priority="54" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A157:A158">
-    <cfRule type="cellIs" dxfId="28" priority="53" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A141">
-    <cfRule type="cellIs" dxfId="27" priority="52" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A138">
-    <cfRule type="cellIs" dxfId="26" priority="51" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A139">
-    <cfRule type="cellIs" dxfId="25" priority="50" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A140">
-    <cfRule type="cellIs" dxfId="24" priority="49" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A144">
-    <cfRule type="cellIs" dxfId="23" priority="48" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A146">
-    <cfRule type="cellIs" dxfId="22" priority="47" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A150">
-    <cfRule type="cellIs" dxfId="21" priority="46" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A77:A78 A63:A64 A68">
-    <cfRule type="cellIs" dxfId="19" priority="44" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A25 A21:A22">
-    <cfRule type="cellIs" dxfId="18" priority="23" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" dxfId="16" priority="36" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:A73">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="cellIs" dxfId="14" priority="20" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="cellIs" dxfId="13" priority="33" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105:A106">
-    <cfRule type="cellIs" dxfId="12" priority="32" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75:A76">
-    <cfRule type="cellIs" dxfId="11" priority="31" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:A60">
-    <cfRule type="cellIs" dxfId="10" priority="30" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:A40">
-    <cfRule type="cellIs" dxfId="9" priority="29" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="cellIs" dxfId="8" priority="28" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A74">
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A156">
-    <cfRule type="cellIs" dxfId="6" priority="24" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A130">
-    <cfRule type="cellIs" dxfId="5" priority="25" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:A30 A26:A27">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D12 D16:D18 D32:D40 D44:D60 D136:D158 D110:D132 D22:D23 D80:D106 D27:D28 D64:D76">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D12 D16:D18 D65:D77 D45:D61 D137:D159 D111:D133 D22:D23 D81:D107 D27:D28 D32:D35 D36:D41">
       <formula1>TYPE</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add orderym to orders change parchase_no length to 30
</commit_message>
<xml_diff>
--- a/document/sql_creator.xlsx
+++ b/document/sql_creator.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="180">
   <si>
     <t>属性</t>
     <rPh sb="0" eb="2">
@@ -960,6 +960,20 @@
     <rPh sb="5" eb="7">
       <t>クブン</t>
     </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>受注年月</t>
+    <rPh sb="0" eb="2">
+      <t>ジュチュウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ネンゲツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>orderym</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1405,7 +1419,27 @@
     <cellStyle name="メモ" xfId="1" builtinId="10"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="78">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2379,10 +2413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J160"/>
+  <dimension ref="A1:J161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -4235,11 +4269,11 @@
         <v>138</v>
       </c>
       <c r="I82" s="40" t="str">
-        <f t="shared" ref="I82:I94" si="16">"," &amp; IF(A82="","","/* ") &amp; "`" &amp; C82 &amp; "` " &amp; D82 &amp; IF(E82&gt;0,"(" &amp; E82 &amp; ") "," ") &amp; IF(F82&lt;&gt;"","NOT NULL ","") &amp; IF(G82="","","DEFAULT '" &amp; G82 &amp; "' ") &amp; IF(A82="",""," */")</f>
+        <f t="shared" ref="I82:I95" si="16">"," &amp; IF(A82="","","/* ") &amp; "`" &amp; C82 &amp; "` " &amp; D82 &amp; IF(E82&gt;0,"(" &amp; E82 &amp; ") "," ") &amp; IF(F82&lt;&gt;"","NOT NULL ","") &amp; IF(G82="","","DEFAULT '" &amp; G82 &amp; "' ") &amp; IF(A82="",""," */")</f>
         <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
       </c>
       <c r="J82" s="41" t="str">
-        <f t="shared" ref="J82:J94" si="17">"," &amp; IF(A82="","","/* ") &amp; "`" &amp; C82 &amp; "` " &amp; D82 &amp; IF(E82&gt;0,"(" &amp; E82 &amp; ") "," ") &amp; IF(F82&lt;&gt;"","NOT NULL ","") &amp; IF(G82="","","DEFAULT '" &amp; G82 &amp; "' ") &amp; IF(A82="",""," */")</f>
+        <f t="shared" ref="J82:J95" si="17">"," &amp; IF(A82="","","/* ") &amp; "`" &amp; C82 &amp; "` " &amp; D82 &amp; IF(E82&gt;0,"(" &amp; E82 &amp; ") "," ") &amp; IF(F82&lt;&gt;"","NOT NULL ","") &amp; IF(G82="","","DEFAULT '" &amp; G82 &amp; "' ") &amp; IF(A82="",""," */")</f>
         <v xml:space="preserve">,`company_code` VARCHAR(20) NOT NULL </v>
       </c>
     </row>
@@ -4322,36 +4356,36 @@
     <row r="86" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A86" s="34"/>
       <c r="B86" s="39" t="s">
-        <v>111</v>
+        <v>178</v>
       </c>
       <c r="C86" s="35" t="s">
-        <v>123</v>
+        <v>179</v>
       </c>
       <c r="D86" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E86" s="36">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F86" s="35"/>
       <c r="G86" s="37"/>
       <c r="H86" s="38"/>
       <c r="I86" s="40" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
+        <f t="shared" ref="I86" si="18">"," &amp; IF(A86="","","/* ") &amp; "`" &amp; C86 &amp; "` " &amp; D86 &amp; IF(E86&gt;0,"(" &amp; E86 &amp; ") "," ") &amp; IF(F86&lt;&gt;"","NOT NULL ","") &amp; IF(G86="","","DEFAULT '" &amp; G86 &amp; "' ") &amp; IF(A86="",""," */")</f>
+        <v xml:space="preserve">,`orderym` VARCHAR(6) </v>
       </c>
       <c r="J86" s="41" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
+        <f t="shared" ref="J86" si="19">"," &amp; IF(A86="","","/* ") &amp; "`" &amp; C86 &amp; "` " &amp; D86 &amp; IF(E86&gt;0,"(" &amp; E86 &amp; ") "," ") &amp; IF(F86&lt;&gt;"","NOT NULL ","") &amp; IF(G86="","","DEFAULT '" &amp; G86 &amp; "' ") &amp; IF(A86="",""," */")</f>
+        <v xml:space="preserve">,`orderym` VARCHAR(6) </v>
       </c>
     </row>
     <row r="87" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A87" s="34"/>
       <c r="B87" s="39" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C87" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D87" s="35" t="s">
         <v>7</v>
@@ -4364,20 +4398,20 @@
       <c r="H87" s="38"/>
       <c r="I87" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
       </c>
       <c r="J87" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="88" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A88" s="34"/>
       <c r="B88" s="39" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C88" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D88" s="35" t="s">
         <v>7</v>
@@ -4387,49 +4421,51 @@
       </c>
       <c r="F88" s="35"/>
       <c r="G88" s="37"/>
-      <c r="H88" s="38" t="s">
-        <v>134</v>
-      </c>
+      <c r="H88" s="38"/>
       <c r="I88" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
       </c>
       <c r="J88" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`order_detail_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="89" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A89" s="34"/>
       <c r="B89" s="39" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C89" s="35" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D89" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E89" s="36">
+        <v>20</v>
+      </c>
       <c r="F89" s="35"/>
       <c r="G89" s="37"/>
-      <c r="H89" s="38"/>
+      <c r="H89" s="38" t="s">
+        <v>134</v>
+      </c>
       <c r="I89" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`delivery_date` DATE </v>
+        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
       </c>
       <c r="J89" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`delivery_date` DATE </v>
+        <v xml:space="preserve">,`purchase_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="90" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A90" s="34"/>
       <c r="B90" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>9</v>
@@ -4440,148 +4476,148 @@
       <c r="H90" s="38"/>
       <c r="I90" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`sales_date` DATE </v>
+        <v xml:space="preserve">,`delivery_date` DATE </v>
       </c>
       <c r="J90" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`sales_date` DATE </v>
+        <v xml:space="preserve">,`delivery_date` DATE </v>
       </c>
     </row>
     <row r="91" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A91" s="34"/>
       <c r="B91" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C91" s="35" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D91" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E91" s="36">
-        <v>64</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E91" s="36"/>
       <c r="F91" s="35"/>
       <c r="G91" s="37"/>
       <c r="H91" s="38"/>
       <c r="I91" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
+        <v xml:space="preserve">,`sales_date` DATE </v>
       </c>
       <c r="J91" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
+        <v xml:space="preserve">,`sales_date` DATE </v>
       </c>
     </row>
     <row r="92" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A92" s="34"/>
       <c r="B92" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D92" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E92" s="36">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="F92" s="35"/>
       <c r="G92" s="37"/>
       <c r="H92" s="38"/>
       <c r="I92" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
+        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
       </c>
       <c r="J92" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
+        <v xml:space="preserve">,`status_msg` VARCHAR(64) </v>
       </c>
     </row>
     <row r="93" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A93" s="34"/>
       <c r="B93" s="39" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C93" s="35" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="D93" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E93" s="36">
-        <v>20</v>
+        <v>256</v>
       </c>
       <c r="F93" s="35"/>
       <c r="G93" s="37"/>
       <c r="H93" s="38"/>
       <c r="I93" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
+        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
       </c>
       <c r="J93" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
+        <v xml:space="preserve">,`product_category` VARCHAR(256) </v>
       </c>
     </row>
     <row r="94" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A94" s="34"/>
       <c r="B94" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C94" s="35" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="D94" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E94" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F94" s="35"/>
       <c r="G94" s="37"/>
       <c r="H94" s="38"/>
       <c r="I94" s="40" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
       </c>
       <c r="J94" s="41" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <v xml:space="preserve">,`product_code` VARCHAR(20) </v>
       </c>
     </row>
     <row r="95" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A95" s="34"/>
       <c r="B95" s="39" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="D95" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E95" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E95" s="36">
+        <v>256</v>
+      </c>
       <c r="F95" s="35"/>
       <c r="G95" s="37"/>
       <c r="H95" s="38"/>
       <c r="I95" s="40" t="str">
-        <f t="shared" ref="I95:I96" si="18">"," &amp; IF(A95="","","/* ") &amp; "`" &amp; C95 &amp; "` " &amp; D95 &amp; IF(E95&gt;0,"(" &amp; E95 &amp; ") "," ") &amp; IF(F95&lt;&gt;"","NOT NULL ","") &amp; IF(G95="","","DEFAULT '" &amp; G95 &amp; "' ") &amp; IF(A95="",""," */")</f>
-        <v xml:space="preserve">,`quantity` INT </v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
       <c r="J95" s="41" t="str">
-        <f t="shared" ref="J95:J96" si="19">"," &amp; IF(A95="","","/* ") &amp; "`" &amp; C95 &amp; "` " &amp; D95 &amp; IF(E95&gt;0,"(" &amp; E95 &amp; ") "," ") &amp; IF(F95&lt;&gt;"","NOT NULL ","") &amp; IF(G95="","","DEFAULT '" &amp; G95 &amp; "' ") &amp; IF(A95="",""," */")</f>
-        <v xml:space="preserve">,`quantity` INT </v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="96" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A96" s="34"/>
       <c r="B96" s="39" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C96" s="35" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="D96" s="35" t="s">
         <v>5</v>
@@ -4591,100 +4627,100 @@
       <c r="G96" s="37"/>
       <c r="H96" s="38"/>
       <c r="I96" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="I96:I97" si="20">"," &amp; IF(A96="","","/* ") &amp; "`" &amp; C96 &amp; "` " &amp; D96 &amp; IF(E96&gt;0,"(" &amp; E96 &amp; ") "," ") &amp; IF(F96&lt;&gt;"","NOT NULL ","") &amp; IF(G96="","","DEFAULT '" &amp; G96 &amp; "' ") &amp; IF(A96="",""," */")</f>
+        <v xml:space="preserve">,`quantity` INT </v>
+      </c>
+      <c r="J96" s="41" t="str">
+        <f t="shared" ref="J96:J97" si="21">"," &amp; IF(A96="","","/* ") &amp; "`" &amp; C96 &amp; "` " &amp; D96 &amp; IF(E96&gt;0,"(" &amp; E96 &amp; ") "," ") &amp; IF(F96&lt;&gt;"","NOT NULL ","") &amp; IF(G96="","","DEFAULT '" &amp; G96 &amp; "' ") &amp; IF(A96="",""," */")</f>
+        <v xml:space="preserve">,`quantity` INT </v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A97" s="34"/>
+      <c r="B97" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C97" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="D97" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" s="36"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="38"/>
+      <c r="I97" s="40" t="str">
+        <f t="shared" si="20"/>
         <v xml:space="preserve">,`price` INT </v>
       </c>
-      <c r="J96" s="41" t="str">
-        <f t="shared" si="19"/>
+      <c r="J97" s="41" t="str">
+        <f t="shared" si="21"/>
         <v xml:space="preserve">,`price` INT </v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A97" s="2"/>
-      <c r="B97" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E97" s="7">
-        <v>256</v>
-      </c>
-      <c r="F97" s="6"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="9"/>
-      <c r="I97" s="27" t="str">
-        <f>"," &amp; IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; IF(A97="",""," */")</f>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
-      </c>
-      <c r="J97" s="29" t="str">
-        <f>"," &amp; IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; IF(A97="",""," */")</f>
-        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" s="2"/>
       <c r="B98" s="20" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E98" s="7">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="8"/>
       <c r="H98" s="9"/>
       <c r="I98" s="27" t="str">
         <f>"," &amp; IF(A98="","","/* ") &amp; "`" &amp; C98 &amp; "` " &amp; D98 &amp; IF(E98&gt;0,"(" &amp; E98 &amp; ") "," ") &amp; IF(F98&lt;&gt;"","NOT NULL ","") &amp; IF(G98="","","DEFAULT '" &amp; G98 &amp; "' ") &amp; IF(A98="",""," */")</f>
-        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
       </c>
       <c r="J98" s="29" t="str">
         <f>"," &amp; IF(A98="","","/* ") &amp; "`" &amp; C98 &amp; "` " &amp; D98 &amp; IF(E98&gt;0,"(" &amp; E98 &amp; ") "," ") &amp; IF(F98&lt;&gt;"","NOT NULL ","") &amp; IF(G98="","","DEFAULT '" &amp; G98 &amp; "' ") &amp; IF(A98="",""," */")</f>
+        <v xml:space="preserve">,`sales_dept` VARCHAR(256) </v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A99" s="2"/>
+      <c r="B99" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="7">
+        <v>128</v>
+      </c>
+      <c r="F99" s="6"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="27" t="str">
+        <f>"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
         <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
-    </row>
-    <row r="99" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="34"/>
-      <c r="B99" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C99" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="D99" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E99" s="36"/>
-      <c r="F99" s="35"/>
-      <c r="G99" s="37"/>
-      <c r="H99" s="38"/>
-      <c r="I99" s="40" t="str">
+      <c r="J99" s="29" t="str">
         <f>"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
-        <v xml:space="preserve">,`product_detail` TEXT </v>
-      </c>
-      <c r="J99" s="41" t="str">
-        <f>"," &amp; IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; IF(A99="",""," */")</f>
-        <v xml:space="preserve">,`product_detail` TEXT </v>
+        <v xml:space="preserve">,`sales_staff` VARCHAR(128) </v>
       </c>
     </row>
     <row r="100" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A100" s="34"/>
       <c r="B100" s="39" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C100" s="35" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D100" s="35" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E100" s="36"/>
       <c r="F100" s="35"/>
@@ -4692,46 +4728,44 @@
       <c r="H100" s="38"/>
       <c r="I100" s="40" t="str">
         <f>"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`product_detail` TEXT </v>
       </c>
       <c r="J100" s="41" t="str">
         <f>"," &amp; IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; IF(A100="",""," */")</f>
+        <v xml:space="preserve">,`product_detail` TEXT </v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A101" s="34"/>
+      <c r="B101" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C101" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D101" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E101" s="36"/>
+      <c r="F101" s="35"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="38"/>
+      <c r="I101" s="40" t="str">
+        <f>"," &amp; IF(A101="","","/* ") &amp; "`" &amp; C101 &amp; "` " &amp; D101 &amp; IF(E101&gt;0,"(" &amp; E101 &amp; ") "," ") &amp; IF(F101&lt;&gt;"","NOT NULL ","") &amp; IF(G101="","","DEFAULT '" &amp; G101 &amp; "' ") &amp; IF(A101="",""," */")</f>
         <v xml:space="preserve">,`status_id` INT </v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A101" s="2"/>
-      <c r="B101" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E101" s="7">
-        <v>256</v>
-      </c>
-      <c r="F101" s="6"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="9"/>
-      <c r="I101" s="27" t="str">
-        <f t="shared" ref="I101:I107" si="20">"," &amp; IF(A101="","","/* ") &amp; "`" &amp; C101 &amp; "` " &amp; D101 &amp; IF(E101&gt;0,"(" &amp; E101 &amp; ") "," ") &amp; IF(F101&lt;&gt;"","NOT NULL ","") &amp; IF(G101="","","DEFAULT '" &amp; G101 &amp; "' ") &amp; IF(A101="",""," */")</f>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
-      </c>
-      <c r="J101" s="29" t="str">
-        <f t="shared" ref="J101:J107" si="21">"," &amp; IF(A101="","","/* ") &amp; "`" &amp; C101 &amp; "` " &amp; D101 &amp; IF(E101&gt;0,"(" &amp; E101 &amp; ") "," ") &amp; IF(F101&lt;&gt;"","NOT NULL ","") &amp; IF(G101="","","DEFAULT '" &amp; G101 &amp; "' ") &amp; IF(A101="",""," */")</f>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+      <c r="J101" s="41" t="str">
+        <f>"," &amp; IF(A101="","","/* ") &amp; "`" &amp; C101 &amp; "` " &amp; D101 &amp; IF(E101&gt;0,"(" &amp; E101 &amp; ") "," ") &amp; IF(F101&lt;&gt;"","NOT NULL ","") &amp; IF(G101="","","DEFAULT '" &amp; G101 &amp; "' ") &amp; IF(A101="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="2"/>
       <c r="B102" s="43" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>7</v>
@@ -4743,119 +4777,121 @@
       <c r="G102" s="8"/>
       <c r="H102" s="9"/>
       <c r="I102" s="27" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" ref="I102:I108" si="22">"," &amp; IF(A102="","","/* ") &amp; "`" &amp; C102 &amp; "` " &amp; D102 &amp; IF(E102&gt;0,"(" &amp; E102 &amp; ") "," ") &amp; IF(F102&lt;&gt;"","NOT NULL ","") &amp; IF(G102="","","DEFAULT '" &amp; G102 &amp; "' ") &amp; IF(A102="",""," */")</f>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J102" s="29" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" ref="J102:J108" si="23">"," &amp; IF(A102="","","/* ") &amp; "`" &amp; C102 &amp; "` " &amp; D102 &amp; IF(E102&gt;0,"(" &amp; E102 &amp; ") "," ") &amp; IF(F102&lt;&gt;"","NOT NULL ","") &amp; IF(G102="","","DEFAULT '" &amp; G102 &amp; "' ") &amp; IF(A102="",""," */")</f>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="2"/>
       <c r="B103" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E103" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="E103" s="7">
+        <v>256</v>
+      </c>
       <c r="F103" s="6"/>
       <c r="G103" s="8"/>
       <c r="H103" s="9"/>
       <c r="I103" s="27" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J103" s="29" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" s="2"/>
       <c r="B104" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E104" s="7">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E104" s="7"/>
       <c r="F104" s="6"/>
       <c r="G104" s="8"/>
       <c r="H104" s="9"/>
       <c r="I104" s="27" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+      <c r="J104" s="29" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A105" s="2"/>
+      <c r="B105" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" s="7">
+        <v>64</v>
+      </c>
+      <c r="F105" s="6"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="27" t="str">
+        <f t="shared" si="22"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
-      <c r="J104" s="29" t="str">
-        <f t="shared" si="21"/>
+      <c r="J105" s="29" t="str">
+        <f t="shared" si="23"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="34"/>
-      <c r="B105" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="C105" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D105" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E105" s="36"/>
-      <c r="F105" s="35"/>
-      <c r="G105" s="37"/>
-      <c r="H105" s="38"/>
-      <c r="I105" s="40" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-      <c r="J105" s="41" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="106" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A106" s="34"/>
       <c r="B106" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C106" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D106" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E106" s="36"/>
       <c r="F106" s="35"/>
       <c r="G106" s="37"/>
       <c r="H106" s="38"/>
       <c r="I106" s="40" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J106" s="41" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="107" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A107" s="34"/>
       <c r="B107" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C107" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D107" s="35" t="s">
         <v>8</v>
@@ -4865,144 +4901,144 @@
       <c r="G107" s="37"/>
       <c r="H107" s="38"/>
       <c r="I107" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+      <c r="J107" s="41" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A108" s="34"/>
+      <c r="B108" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C108" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D108" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="36"/>
+      <c r="F108" s="35"/>
+      <c r="G108" s="37"/>
+      <c r="H108" s="38"/>
+      <c r="I108" s="40" t="str">
+        <f t="shared" si="22"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-      <c r="J107" s="41" t="str">
-        <f t="shared" si="21"/>
+      <c r="J108" s="41" t="str">
+        <f t="shared" si="23"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A108" s="2"/>
-      <c r="B108" s="21"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="21"/>
-      <c r="E108" s="22"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="23"/>
-      <c r="H108" s="21"/>
-      <c r="I108" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J108" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" s="2"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="21"/>
+      <c r="E109" s="22"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="23"/>
+      <c r="H109" s="21"/>
+      <c r="I109" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J109" s="29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A110" s="2"/>
-      <c r="B110" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C110" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D110" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F110" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G110" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H110" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I110" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C110 &amp; "` ("</f>
-        <v>CREATE TABLE `licenses` (</v>
-      </c>
-      <c r="J110" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C110 &amp; "` ("</f>
-        <v>CREATE TABLE `licenses` (</v>
-      </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A111" s="2"/>
-      <c r="B111" s="20" t="s">
+      <c r="B111" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C111" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F111" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G111" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H111" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I111" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C111 &amp; "` ("</f>
+        <v>CREATE TABLE `licenses` (</v>
+      </c>
+      <c r="J111" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C111 &amp; "` ("</f>
+        <v>CREATE TABLE `licenses` (</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A112" s="2"/>
+      <c r="B112" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C112" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="6" t="s">
+      <c r="D112" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E111" s="7"/>
-      <c r="F111" s="6" t="s">
+      <c r="E112" s="7"/>
+      <c r="F112" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G111" s="8"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="28" t="s">
+      <c r="G112" s="8"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J111" s="30" t="s">
+      <c r="J112" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="34"/>
-      <c r="B112" s="39" t="s">
+    <row r="113" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A113" s="34"/>
+      <c r="B113" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C112" s="35" t="s">
+      <c r="C113" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D112" s="35" t="s">
+      <c r="D113" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E112" s="36"/>
-      <c r="F112" s="35"/>
-      <c r="G112" s="37"/>
-      <c r="H112" s="38"/>
-      <c r="I112" s="40" t="str">
-        <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
+      <c r="E113" s="36"/>
+      <c r="F113" s="35"/>
+      <c r="G113" s="37"/>
+      <c r="H113" s="38"/>
+      <c r="I113" s="40" t="str">
+        <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT </v>
       </c>
-      <c r="J112" s="41" t="str">
-        <f>"," &amp; IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; IF(A112="",""," */")</f>
+      <c r="J113" s="41" t="str">
+        <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
         <v xml:space="preserve">,`client_id` INT </v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A113" s="2"/>
-      <c r="B113" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E113" s="7"/>
-      <c r="F113" s="6"/>
-      <c r="G113" s="8"/>
-      <c r="H113" s="9"/>
-      <c r="I113" s="27" t="str">
-        <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
-      </c>
-      <c r="J113" s="29" t="str">
-        <f>"," &amp; IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; IF(A113="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A114" s="2"/>
       <c r="B114" s="20" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>5</v>
@@ -5013,20 +5049,20 @@
       <c r="H114" s="9"/>
       <c r="I114" s="27" t="str">
         <f>"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
       <c r="J114" s="29" t="str">
         <f>"," &amp; IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; IF(A114="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A115" s="2"/>
       <c r="B115" s="20" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>5</v>
@@ -5037,220 +5073,220 @@
       <c r="H115" s="9"/>
       <c r="I115" s="27" t="str">
         <f>"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
       <c r="J115" s="29" t="str">
         <f>"," &amp; IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; IF(A115="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A116" s="2"/>
       <c r="B116" s="20" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E116" s="7"/>
       <c r="F116" s="6"/>
       <c r="G116" s="8"/>
       <c r="H116" s="9"/>
       <c r="I116" s="27" t="str">
-        <f t="shared" ref="I116:I122" si="22">"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
       <c r="J116" s="29" t="str">
-        <f t="shared" ref="J116:J122" si="23">"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; IF(A116="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A117" s="2"/>
       <c r="B117" s="20" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E117" s="7">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E117" s="7"/>
       <c r="F117" s="6"/>
       <c r="G117" s="8"/>
       <c r="H117" s="9"/>
       <c r="I117" s="27" t="str">
-        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
+        <f t="shared" ref="I117:I123" si="24">"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
+      </c>
+      <c r="J117" s="29" t="str">
+        <f t="shared" ref="J117:J123" si="25">"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A118" s="2"/>
+      <c r="B118" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" s="7">
+        <v>20</v>
+      </c>
+      <c r="F118" s="6"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="27" t="str">
+        <f>"," &amp; IF(A118="","","/* ") &amp; "`" &amp; C118 &amp; "` " &amp; D118 &amp; IF(E118&gt;0,"(" &amp; E118 &amp; ") "," ") &amp; IF(F118&lt;&gt;"","NOT NULL ","") &amp; IF(G118="","","DEFAULT '" &amp; G118 &amp; "' ") &amp; IF(A118="",""," */")</f>
         <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
-      <c r="J117" s="29" t="str">
-        <f>"," &amp; IF(A117="","","/* ") &amp; "`" &amp; C117 &amp; "` " &amp; D117 &amp; IF(E117&gt;0,"(" &amp; E117 &amp; ") "," ") &amp; IF(F117&lt;&gt;"","NOT NULL ","") &amp; IF(G117="","","DEFAULT '" &amp; G117 &amp; "' ") &amp; IF(A117="",""," */")</f>
+      <c r="J118" s="29" t="str">
+        <f>"," &amp; IF(A118="","","/* ") &amp; "`" &amp; C118 &amp; "` " &amp; D118 &amp; IF(E118&gt;0,"(" &amp; E118 &amp; ") "," ") &amp; IF(F118&lt;&gt;"","NOT NULL ","") &amp; IF(G118="","","DEFAULT '" &amp; G118 &amp; "' ") &amp; IF(A118="",""," */")</f>
         <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A118" s="34"/>
-      <c r="B118" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="C118" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D118" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E118" s="36">
-        <v>20</v>
-      </c>
-      <c r="F118" s="35"/>
-      <c r="G118" s="37"/>
-      <c r="H118" s="38"/>
-      <c r="I118" s="40" t="str">
-        <f>"," &amp; IF(A118="","","/* ") &amp; "`" &amp; C118 &amp; "` " &amp; D118 &amp; IF(E118&gt;0,"(" &amp; E118 &amp; ") "," ") &amp; IF(F118&lt;&gt;"","NOT NULL ","") &amp; IF(G118="","","DEFAULT '" &amp; G118 &amp; "' ") &amp; IF(A118="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
-      </c>
-      <c r="J118" s="41" t="str">
-        <f>"," &amp; IF(A118="","","/* ") &amp; "`" &amp; C118 &amp; "` " &amp; D118 &amp; IF(E118&gt;0,"(" &amp; E118 &amp; ") "," ") &amp; IF(F118&lt;&gt;"","NOT NULL ","") &amp; IF(G118="","","DEFAULT '" &amp; G118 &amp; "' ") &amp; IF(A118="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="119" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A119" s="34"/>
       <c r="B119" s="39" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="C119" s="35" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D119" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F119" s="35"/>
       <c r="G119" s="37"/>
       <c r="H119" s="38"/>
       <c r="I119" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f>"," &amp; IF(A119="","","/* ") &amp; "`" &amp; C119 &amp; "` " &amp; D119 &amp; IF(E119&gt;0,"(" &amp; E119 &amp; ") "," ") &amp; IF(F119&lt;&gt;"","NOT NULL ","") &amp; IF(G119="","","DEFAULT '" &amp; G119 &amp; "' ") &amp; IF(A119="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+      </c>
+      <c r="J119" s="41" t="str">
+        <f>"," &amp; IF(A119="","","/* ") &amp; "`" &amp; C119 &amp; "` " &amp; D119 &amp; IF(E119&gt;0,"(" &amp; E119 &amp; ") "," ") &amp; IF(F119&lt;&gt;"","NOT NULL ","") &amp; IF(G119="","","DEFAULT '" &amp; G119 &amp; "' ") &amp; IF(A119="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A120" s="34"/>
+      <c r="B120" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C120" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D120" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E120" s="36">
+        <v>256</v>
+      </c>
+      <c r="F120" s="35"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="38"/>
+      <c r="I120" s="40" t="str">
+        <f t="shared" si="24"/>
         <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
-      <c r="J119" s="41" t="str">
-        <f t="shared" si="23"/>
+      <c r="J120" s="41" t="str">
+        <f t="shared" si="25"/>
         <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A120" s="2"/>
-      <c r="B120" s="20" t="s">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A121" s="2"/>
+      <c r="B121" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C120" s="6" t="s">
+      <c r="C121" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D120" s="6" t="s">
+      <c r="D121" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E120" s="7">
+      <c r="E121" s="7">
         <v>256</v>
       </c>
-      <c r="F120" s="6"/>
-      <c r="G120" s="8"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="27" t="str">
-        <f t="shared" si="22"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="9"/>
+      <c r="I121" s="27" t="str">
+        <f t="shared" si="24"/>
         <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
-      <c r="J120" s="29" t="str">
-        <f t="shared" si="23"/>
+      <c r="J121" s="29" t="str">
+        <f t="shared" si="25"/>
         <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
     </row>
-    <row r="121" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A121" s="34"/>
-      <c r="B121" s="39" t="s">
+    <row r="122" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A122" s="34"/>
+      <c r="B122" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="C121" s="35" t="s">
+      <c r="C122" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="D121" s="35" t="s">
+      <c r="D122" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E121" s="36"/>
-      <c r="F121" s="35"/>
-      <c r="G121" s="37"/>
-      <c r="H121" s="38"/>
-      <c r="I121" s="40" t="str">
-        <f t="shared" ref="I121" si="24">"," &amp; IF(A121="","","/* ") &amp; "`" &amp; C121 &amp; "` " &amp; D121 &amp; IF(E121&gt;0,"(" &amp; E121 &amp; ") "," ") &amp; IF(F121&lt;&gt;"","NOT NULL ","") &amp; IF(G121="","","DEFAULT '" &amp; G121 &amp; "' ") &amp; IF(A121="",""," */")</f>
+      <c r="E122" s="36"/>
+      <c r="F122" s="35"/>
+      <c r="G122" s="37"/>
+      <c r="H122" s="38"/>
+      <c r="I122" s="40" t="str">
+        <f t="shared" ref="I122" si="26">"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
         <v xml:space="preserve">,`language_id` INT </v>
       </c>
-      <c r="J121" s="41" t="str">
-        <f t="shared" ref="J121" si="25">"," &amp; IF(A121="","","/* ") &amp; "`" &amp; C121 &amp; "` " &amp; D121 &amp; IF(E121&gt;0,"(" &amp; E121 &amp; ") "," ") &amp; IF(F121&lt;&gt;"","NOT NULL ","") &amp; IF(G121="","","DEFAULT '" &amp; G121 &amp; "' ") &amp; IF(A121="",""," */")</f>
+      <c r="J122" s="41" t="str">
+        <f t="shared" ref="J122" si="27">"," &amp; IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; IF(A122="",""," */")</f>
         <v xml:space="preserve">,`language_id` INT </v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A122" s="2"/>
-      <c r="B122" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D122" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E122" s="7"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="8"/>
-      <c r="H122" s="9"/>
-      <c r="I122" s="27" t="str">
-        <f t="shared" si="22"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
-      </c>
-      <c r="J122" s="29" t="str">
-        <f t="shared" si="23"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A123" s="2"/>
       <c r="B123" s="20" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E123" s="7"/>
       <c r="F123" s="6"/>
       <c r="G123" s="8"/>
       <c r="H123" s="9"/>
       <c r="I123" s="27" t="str">
-        <f t="shared" ref="I123" si="26">"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
       <c r="J123" s="29" t="str">
-        <f t="shared" ref="J123" si="27">"," &amp; IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; IF(A123="",""," */")</f>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A124" s="2"/>
       <c r="B124" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>9</v>
@@ -5260,97 +5296,95 @@
       <c r="G124" s="8"/>
       <c r="H124" s="9"/>
       <c r="I124" s="27" t="str">
-        <f>"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
+        <f t="shared" ref="I124" si="28">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
+        <v xml:space="preserve">,`startdate` DATE </v>
+      </c>
+      <c r="J124" s="29" t="str">
+        <f t="shared" ref="J124" si="29">"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
+        <v xml:space="preserve">,`startdate` DATE </v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A125" s="2"/>
+      <c r="B125" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="7"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="8"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="27" t="str">
+        <f>"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
         <v xml:space="preserve">,`enddate` DATE </v>
       </c>
-      <c r="J124" s="29" t="str">
-        <f>"," &amp; IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; IF(A124="",""," */")</f>
+      <c r="J125" s="29" t="str">
+        <f>"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
         <v xml:space="preserve">,`enddate` DATE </v>
       </c>
     </row>
-    <row r="125" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A125" s="34"/>
-      <c r="B125" s="39" t="s">
+    <row r="126" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A126" s="34"/>
+      <c r="B126" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="C125" s="35" t="s">
+      <c r="C126" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="D125" s="35" t="s">
+      <c r="D126" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E125" s="36">
+      <c r="E126" s="36">
         <v>256</v>
       </c>
-      <c r="F125" s="35"/>
-      <c r="G125" s="37"/>
-      <c r="H125" s="38"/>
-      <c r="I125" s="40" t="str">
-        <f t="shared" ref="I125" si="28">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
+      <c r="F126" s="35"/>
+      <c r="G126" s="37"/>
+      <c r="H126" s="38"/>
+      <c r="I126" s="40" t="str">
+        <f t="shared" ref="I126" si="30">"," &amp; IF(A126="","","/* ") &amp; "`" &amp; C126 &amp; "` " &amp; D126 &amp; IF(E126&gt;0,"(" &amp; E126 &amp; ") "," ") &amp; IF(F126&lt;&gt;"","NOT NULL ","") &amp; IF(G126="","","DEFAULT '" &amp; G126 &amp; "' ") &amp; IF(A126="",""," */")</f>
         <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
-      <c r="J125" s="41" t="str">
-        <f t="shared" ref="J125" si="29">"," &amp; IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; IF(A125="",""," */")</f>
+      <c r="J126" s="41" t="str">
+        <f t="shared" ref="J126" si="31">"," &amp; IF(A126="","","/* ") &amp; "`" &amp; C126 &amp; "` " &amp; D126 &amp; IF(E126&gt;0,"(" &amp; E126 &amp; ") "," ") &amp; IF(F126&lt;&gt;"","NOT NULL ","") &amp; IF(G126="","","DEFAULT '" &amp; G126 &amp; "' ") &amp; IF(A126="",""," */")</f>
         <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A126" s="2"/>
-      <c r="B126" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E126" s="7"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="8"/>
-      <c r="H126" s="9"/>
-      <c r="I126" s="27" t="str">
-        <f t="shared" ref="I126:I133" si="30">"," &amp; IF(A126="","","/* ") &amp; "`" &amp; C126 &amp; "` " &amp; D126 &amp; IF(E126&gt;0,"(" &amp; E126 &amp; ") "," ") &amp; IF(F126&lt;&gt;"","NOT NULL ","") &amp; IF(G126="","","DEFAULT '" &amp; G126 &amp; "' ") &amp; IF(A126="",""," */")</f>
-        <v xml:space="preserve">,`notice` TEXT </v>
-      </c>
-      <c r="J126" s="29" t="str">
-        <f t="shared" ref="J126:J133" si="31">"," &amp; IF(A126="","","/* ") &amp; "`" &amp; C126 &amp; "` " &amp; D126 &amp; IF(E126&gt;0,"(" &amp; E126 &amp; ") "," ") &amp; IF(F126&lt;&gt;"","NOT NULL ","") &amp; IF(G126="","","DEFAULT '" &amp; G126 &amp; "' ") &amp; IF(A126="",""," */")</f>
-        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A127" s="2"/>
-      <c r="B127" s="43" t="s">
-        <v>87</v>
+      <c r="B127" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E127" s="7">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E127" s="7"/>
       <c r="F127" s="6"/>
       <c r="G127" s="8"/>
       <c r="H127" s="9"/>
       <c r="I127" s="27" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" ref="I127:I134" si="32">"," &amp; IF(A127="","","/* ") &amp; "`" &amp; C127 &amp; "` " &amp; D127 &amp; IF(E127&gt;0,"(" &amp; E127 &amp; ") "," ") &amp; IF(F127&lt;&gt;"","NOT NULL ","") &amp; IF(G127="","","DEFAULT '" &amp; G127 &amp; "' ") &amp; IF(A127="",""," */")</f>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
       <c r="J127" s="29" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" ref="J127:J134" si="33">"," &amp; IF(A127="","","/* ") &amp; "`" &amp; C127 &amp; "` " &amp; D127 &amp; IF(E127&gt;0,"(" &amp; E127 &amp; ") "," ") &amp; IF(F127&lt;&gt;"","NOT NULL ","") &amp; IF(G127="","","DEFAULT '" &amp; G127 &amp; "' ") &amp; IF(A127="",""," */")</f>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A128" s="2"/>
       <c r="B128" s="43" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>7</v>
@@ -5362,119 +5396,121 @@
       <c r="G128" s="8"/>
       <c r="H128" s="9"/>
       <c r="I128" s="27" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J128" s="29" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129" s="2"/>
       <c r="B129" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E129" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="E129" s="7">
+        <v>256</v>
+      </c>
       <c r="F129" s="6"/>
       <c r="G129" s="8"/>
       <c r="H129" s="9"/>
       <c r="I129" s="27" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J129" s="29" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130" s="2"/>
       <c r="B130" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E130" s="7">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E130" s="7"/>
       <c r="F130" s="6"/>
       <c r="G130" s="8"/>
       <c r="H130" s="9"/>
       <c r="I130" s="27" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+      <c r="J130" s="29" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">,`size` INT </v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A131" s="2"/>
+      <c r="B131" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E131" s="7">
+        <v>64</v>
+      </c>
+      <c r="F131" s="6"/>
+      <c r="G131" s="8"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="27" t="str">
+        <f t="shared" si="32"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
-      <c r="J130" s="29" t="str">
-        <f t="shared" si="31"/>
+      <c r="J131" s="29" t="str">
+        <f t="shared" si="33"/>
         <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
-    <row r="131" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A131" s="34"/>
-      <c r="B131" s="43" t="s">
+    <row r="132" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A132" s="34"/>
+      <c r="B132" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="C131" s="35" t="s">
+      <c r="C132" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="D131" s="35" t="s">
+      <c r="D132" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="E131" s="36"/>
-      <c r="F131" s="35"/>
-      <c r="G131" s="37"/>
-      <c r="H131" s="38"/>
-      <c r="I131" s="40" t="str">
-        <f t="shared" si="30"/>
+      <c r="E132" s="36"/>
+      <c r="F132" s="35"/>
+      <c r="G132" s="37"/>
+      <c r="H132" s="38"/>
+      <c r="I132" s="40" t="str">
+        <f t="shared" si="32"/>
         <v xml:space="preserve">,`user_id` INT </v>
       </c>
-      <c r="J131" s="41" t="str">
-        <f t="shared" si="31"/>
+      <c r="J132" s="41" t="str">
+        <f t="shared" si="33"/>
         <v xml:space="preserve">,`user_id` INT </v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A132" s="2"/>
-      <c r="B132" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E132" s="7"/>
-      <c r="F132" s="6"/>
-      <c r="G132" s="8"/>
-      <c r="H132" s="9"/>
-      <c r="I132" s="27" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
-      </c>
-      <c r="J132" s="29" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" s="2"/>
       <c r="B133" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>8</v>
@@ -5484,120 +5520,120 @@
       <c r="G133" s="8"/>
       <c r="H133" s="9"/>
       <c r="I133" s="27" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
       <c r="J133" s="29" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve">,`modified` DATETIME </v>
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" s="2"/>
-      <c r="B134" s="21"/>
-      <c r="C134" s="21"/>
-      <c r="D134" s="21"/>
-      <c r="E134" s="22"/>
-      <c r="F134" s="21"/>
-      <c r="G134" s="23"/>
-      <c r="H134" s="21"/>
-      <c r="I134" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J134" s="29" t="s">
-        <v>33</v>
+      <c r="B134" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="7"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="27" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
+      </c>
+      <c r="J134" s="29" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" s="2"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="21"/>
+      <c r="D135" s="21"/>
+      <c r="E135" s="22"/>
+      <c r="F135" s="21"/>
+      <c r="G135" s="23"/>
+      <c r="H135" s="21"/>
+      <c r="I135" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J135" s="29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" s="2"/>
-      <c r="B136" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C136" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D136" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E136" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F136" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G136" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H136" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I136" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C136 &amp; "` ("</f>
-        <v>CREATE TABLE `licensehistories` (</v>
-      </c>
-      <c r="J136" s="29" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C136 &amp; "` ("</f>
-        <v>CREATE TABLE `licensehistories` (</v>
-      </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137" s="2"/>
-      <c r="B137" s="20" t="s">
+      <c r="B137" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C137" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E137" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F137" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G137" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H137" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I137" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C137 &amp; "` ("</f>
+        <v>CREATE TABLE `licensehistories` (</v>
+      </c>
+      <c r="J137" s="29" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C137 &amp; "` ("</f>
+        <v>CREATE TABLE `licensehistories` (</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A138" s="2"/>
+      <c r="B138" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C137" s="6" t="s">
+      <c r="C138" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D137" s="6" t="s">
+      <c r="D138" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E137" s="7"/>
-      <c r="F137" s="6" t="s">
+      <c r="E138" s="7"/>
+      <c r="F138" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G137" s="8"/>
-      <c r="H137" s="9"/>
-      <c r="I137" s="28" t="s">
+      <c r="G138" s="8"/>
+      <c r="H138" s="9"/>
+      <c r="I138" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J137" s="30" t="s">
+      <c r="J138" s="30" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A138" s="34"/>
-      <c r="B138" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C138" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D138" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E138" s="36"/>
-      <c r="F138" s="35"/>
-      <c r="G138" s="37"/>
-      <c r="H138" s="38"/>
-      <c r="I138" s="40" t="str">
-        <f>"," &amp; IF(A138="","","/* ") &amp; "`" &amp; C138 &amp; "` " &amp; D138 &amp; IF(E138&gt;0,"(" &amp; E138 &amp; ") "," ") &amp; IF(F138&lt;&gt;"","NOT NULL ","") &amp; IF(G138="","","DEFAULT '" &amp; G138 &amp; "' ") &amp; IF(A138="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT </v>
-      </c>
-      <c r="J138" s="41" t="str">
-        <f>"," &amp; IF(A138="","","/* ") &amp; "`" &amp; C138 &amp; "` " &amp; D138 &amp; IF(E138&gt;0,"(" &amp; E138 &amp; ") "," ") &amp; IF(F138&lt;&gt;"","NOT NULL ","") &amp; IF(G138="","","DEFAULT '" &amp; G138 &amp; "' ") &amp; IF(A138="",""," */")</f>
-        <v xml:space="preserve">,`client_id` INT </v>
       </c>
     </row>
     <row r="139" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A139" s="34"/>
       <c r="B139" s="39" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C139" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D139" s="35" t="s">
         <v>5</v>
@@ -5608,20 +5644,20 @@
       <c r="H139" s="38"/>
       <c r="I139" s="40" t="str">
         <f>"," &amp; IF(A139="","","/* ") &amp; "`" &amp; C139 &amp; "` " &amp; D139 &amp; IF(E139&gt;0,"(" &amp; E139 &amp; ") "," ") &amp; IF(F139&lt;&gt;"","NOT NULL ","") &amp; IF(G139="","","DEFAULT '" &amp; G139 &amp; "' ") &amp; IF(A139="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <v xml:space="preserve">,`client_id` INT </v>
       </c>
       <c r="J139" s="41" t="str">
         <f>"," &amp; IF(A139="","","/* ") &amp; "`" &amp; C139 &amp; "` " &amp; D139 &amp; IF(E139&gt;0,"(" &amp; E139 &amp; ") "," ") &amp; IF(F139&lt;&gt;"","NOT NULL ","") &amp; IF(G139="","","DEFAULT '" &amp; G139 &amp; "' ") &amp; IF(A139="",""," */")</f>
-        <v xml:space="preserve">,`customer_id` INT </v>
+        <v xml:space="preserve">,`client_id` INT </v>
       </c>
     </row>
     <row r="140" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A140" s="34"/>
       <c r="B140" s="39" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C140" s="35" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D140" s="35" t="s">
         <v>5</v>
@@ -5632,20 +5668,20 @@
       <c r="H140" s="38"/>
       <c r="I140" s="40" t="str">
         <f>"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
       <c r="J140" s="41" t="str">
         <f>"," &amp; IF(A140="","","/* ") &amp; "`" &amp; C140 &amp; "` " &amp; D140 &amp; IF(E140&gt;0,"(" &amp; E140 &amp; ") "," ") &amp; IF(F140&lt;&gt;"","NOT NULL ","") &amp; IF(G140="","","DEFAULT '" &amp; G140 &amp; "' ") &amp; IF(A140="",""," */")</f>
-        <v xml:space="preserve">,`order_id` INT </v>
+        <v xml:space="preserve">,`customer_id` INT </v>
       </c>
     </row>
     <row r="141" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A141" s="34"/>
       <c r="B141" s="39" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C141" s="35" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D141" s="35" t="s">
         <v>5</v>
@@ -5656,70 +5692,68 @@
       <c r="H141" s="38"/>
       <c r="I141" s="40" t="str">
         <f>"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
       <c r="J141" s="41" t="str">
         <f>"," &amp; IF(A141="","","/* ") &amp; "`" &amp; C141 &amp; "` " &amp; D141 &amp; IF(E141&gt;0,"(" &amp; E141 &amp; ") "," ") &amp; IF(F141&lt;&gt;"","NOT NULL ","") &amp; IF(G141="","","DEFAULT '" &amp; G141 &amp; "' ") &amp; IF(A141="",""," */")</f>
-        <v xml:space="preserve">,`status_id` INT </v>
+        <v xml:space="preserve">,`order_id` INT </v>
       </c>
     </row>
     <row r="142" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A142" s="34"/>
       <c r="B142" s="39" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C142" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D142" s="35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E142" s="36"/>
       <c r="F142" s="35"/>
       <c r="G142" s="37"/>
       <c r="H142" s="38"/>
       <c r="I142" s="40" t="str">
-        <f t="shared" ref="I142" si="32">"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
       <c r="J142" s="41" t="str">
-        <f t="shared" ref="J142" si="33">"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
-        <v xml:space="preserve">,`issued` DATE </v>
+        <f>"," &amp; IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; IF(A142="",""," */")</f>
+        <v xml:space="preserve">,`status_id` INT </v>
       </c>
     </row>
     <row r="143" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A143" s="34"/>
       <c r="B143" s="39" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C143" s="35" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D143" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E143" s="36">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E143" s="36"/>
       <c r="F143" s="35"/>
       <c r="G143" s="37"/>
       <c r="H143" s="38"/>
       <c r="I143" s="40" t="str">
-        <f>"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
-        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
+        <f t="shared" ref="I143" si="34">"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
       </c>
       <c r="J143" s="41" t="str">
-        <f>"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
-        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
+        <f t="shared" ref="J143" si="35">"," &amp; IF(A143="","","/* ") &amp; "`" &amp; C143 &amp; "` " &amp; D143 &amp; IF(E143&gt;0,"(" &amp; E143 &amp; ") "," ") &amp; IF(F143&lt;&gt;"","NOT NULL ","") &amp; IF(G143="","","DEFAULT '" &amp; G143 &amp; "' ") &amp; IF(A143="",""," */")</f>
+        <v xml:space="preserve">,`issued` DATE </v>
       </c>
     </row>
     <row r="144" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A144" s="34"/>
       <c r="B144" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C144" s="35" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="D144" s="35" t="s">
         <v>7</v>
@@ -5732,46 +5766,46 @@
       <c r="H144" s="38"/>
       <c r="I144" s="40" t="str">
         <f>"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
       <c r="J144" s="41" t="str">
         <f>"," &amp; IF(A144="","","/* ") &amp; "`" &amp; C144 &amp; "` " &amp; D144 &amp; IF(E144&gt;0,"(" &amp; E144 &amp; ") "," ") &amp; IF(F144&lt;&gt;"","NOT NULL ","") &amp; IF(G144="","","DEFAULT '" &amp; G144 &amp; "' ") &amp; IF(A144="",""," */")</f>
-        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
+        <v xml:space="preserve">,`license_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="145" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A145" s="34"/>
       <c r="B145" s="39" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="C145" s="35" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D145" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E145" s="36">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="F145" s="35"/>
       <c r="G145" s="37"/>
       <c r="H145" s="38"/>
       <c r="I145" s="40" t="str">
-        <f t="shared" ref="I145:I149" si="34">"," &amp; IF(A145="","","/* ") &amp; "`" &amp; C145 &amp; "` " &amp; D145 &amp; IF(E145&gt;0,"(" &amp; E145 &amp; ") "," ") &amp; IF(F145&lt;&gt;"","NOT NULL ","") &amp; IF(G145="","","DEFAULT '" &amp; G145 &amp; "' ") &amp; IF(A145="",""," */")</f>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f>"," &amp; IF(A145="","","/* ") &amp; "`" &amp; C145 &amp; "` " &amp; D145 &amp; IF(E145&gt;0,"(" &amp; E145 &amp; ") "," ") &amp; IF(F145&lt;&gt;"","NOT NULL ","") &amp; IF(G145="","","DEFAULT '" &amp; G145 &amp; "' ") &amp; IF(A145="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
       <c r="J145" s="41" t="str">
-        <f t="shared" ref="J145:J149" si="35">"," &amp; IF(A145="","","/* ") &amp; "`" &amp; C145 &amp; "` " &amp; D145 &amp; IF(E145&gt;0,"(" &amp; E145 &amp; ") "," ") &amp; IF(F145&lt;&gt;"","NOT NULL ","") &amp; IF(G145="","","DEFAULT '" &amp; G145 &amp; "' ") &amp; IF(A145="",""," */")</f>
-        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
+        <f>"," &amp; IF(A145="","","/* ") &amp; "`" &amp; C145 &amp; "` " &amp; D145 &amp; IF(E145&gt;0,"(" &amp; E145 &amp; ") "," ") &amp; IF(F145&lt;&gt;"","NOT NULL ","") &amp; IF(G145="","","DEFAULT '" &amp; G145 &amp; "' ") &amp; IF(A145="",""," */")</f>
+        <v xml:space="preserve">,`relate_no` VARCHAR(20) </v>
       </c>
     </row>
     <row r="146" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A146" s="34"/>
       <c r="B146" s="39" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="C146" s="35" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="D146" s="35" t="s">
         <v>7</v>
@@ -5783,93 +5817,95 @@
       <c r="G146" s="37"/>
       <c r="H146" s="38"/>
       <c r="I146" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
+        <f t="shared" ref="I146:I150" si="36">"," &amp; IF(A146="","","/* ") &amp; "`" &amp; C146 &amp; "` " &amp; D146 &amp; IF(E146&gt;0,"(" &amp; E146 &amp; ") "," ") &amp; IF(F146&lt;&gt;"","NOT NULL ","") &amp; IF(G146="","","DEFAULT '" &amp; G146 &amp; "' ") &amp; IF(A146="",""," */")</f>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
       <c r="J146" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
+        <f t="shared" ref="J146:J150" si="37">"," &amp; IF(A146="","","/* ") &amp; "`" &amp; C146 &amp; "` " &amp; D146 &amp; IF(E146&gt;0,"(" &amp; E146 &amp; ") "," ") &amp; IF(F146&lt;&gt;"","NOT NULL ","") &amp; IF(G146="","","DEFAULT '" &amp; G146 &amp; "' ") &amp; IF(A146="",""," */")</f>
+        <v xml:space="preserve">,`product_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="147" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A147" s="34"/>
       <c r="B147" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C147" s="35" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="D147" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E147" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E147" s="36">
+        <v>256</v>
+      </c>
       <c r="F147" s="35"/>
       <c r="G147" s="37"/>
       <c r="H147" s="38"/>
       <c r="I147" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`language_id` INT </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
       <c r="J147" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`language_id` INT </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`license_name` VARCHAR(256) </v>
       </c>
     </row>
     <row r="148" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A148" s="34"/>
       <c r="B148" s="39" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="C148" s="35" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="D148" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E148" s="36"/>
       <c r="F148" s="35"/>
       <c r="G148" s="37"/>
       <c r="H148" s="38"/>
       <c r="I148" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`language_id` INT </v>
       </c>
       <c r="J148" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`license_qty` INT </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`language_id` INT </v>
       </c>
     </row>
     <row r="149" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A149" s="34"/>
       <c r="B149" s="39" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C149" s="35" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D149" s="35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E149" s="36"/>
       <c r="F149" s="35"/>
       <c r="G149" s="37"/>
       <c r="H149" s="38"/>
       <c r="I149" s="40" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
       <c r="J149" s="41" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve">,`startdate` DATE </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`license_qty` INT </v>
       </c>
     </row>
     <row r="150" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A150" s="34"/>
       <c r="B150" s="39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C150" s="35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D150" s="35" t="s">
         <v>9</v>
@@ -5879,97 +5915,95 @@
       <c r="G150" s="37"/>
       <c r="H150" s="38"/>
       <c r="I150" s="40" t="str">
-        <f>"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
-        <v xml:space="preserve">,`enddate` DATE </v>
+        <f t="shared" si="36"/>
+        <v xml:space="preserve">,`startdate` DATE </v>
       </c>
       <c r="J150" s="41" t="str">
-        <f>"," &amp; IF(A150="","","/* ") &amp; "`" &amp; C150 &amp; "` " &amp; D150 &amp; IF(E150&gt;0,"(" &amp; E150 &amp; ") "," ") &amp; IF(F150&lt;&gt;"","NOT NULL ","") &amp; IF(G150="","","DEFAULT '" &amp; G150 &amp; "' ") &amp; IF(A150="",""," */")</f>
-        <v xml:space="preserve">,`enddate` DATE </v>
+        <f t="shared" si="37"/>
+        <v xml:space="preserve">,`startdate` DATE </v>
       </c>
     </row>
     <row r="151" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A151" s="34"/>
       <c r="B151" s="39" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="C151" s="35" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="D151" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E151" s="36">
-        <v>256</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E151" s="36"/>
       <c r="F151" s="35"/>
       <c r="G151" s="37"/>
       <c r="H151" s="38"/>
       <c r="I151" s="40" t="str">
-        <f t="shared" ref="I151:I159" si="36">"," &amp; IF(A151="","","/* ") &amp; "`" &amp; C151 &amp; "` " &amp; D151 &amp; IF(E151&gt;0,"(" &amp; E151 &amp; ") "," ") &amp; IF(F151&lt;&gt;"","NOT NULL ","") &amp; IF(G151="","","DEFAULT '" &amp; G151 &amp; "' ") &amp; IF(A151="",""," */")</f>
-        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
+        <f>"," &amp; IF(A151="","","/* ") &amp; "`" &amp; C151 &amp; "` " &amp; D151 &amp; IF(E151&gt;0,"(" &amp; E151 &amp; ") "," ") &amp; IF(F151&lt;&gt;"","NOT NULL ","") &amp; IF(G151="","","DEFAULT '" &amp; G151 &amp; "' ") &amp; IF(A151="",""," */")</f>
+        <v xml:space="preserve">,`enddate` DATE </v>
       </c>
       <c r="J151" s="41" t="str">
-        <f t="shared" ref="J151:J159" si="37">"," &amp; IF(A151="","","/* ") &amp; "`" &amp; C151 &amp; "` " &amp; D151 &amp; IF(E151&gt;0,"(" &amp; E151 &amp; ") "," ") &amp; IF(F151&lt;&gt;"","NOT NULL ","") &amp; IF(G151="","","DEFAULT '" &amp; G151 &amp; "' ") &amp; IF(A151="",""," */")</f>
-        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
+        <f>"," &amp; IF(A151="","","/* ") &amp; "`" &amp; C151 &amp; "` " &amp; D151 &amp; IF(E151&gt;0,"(" &amp; E151 &amp; ") "," ") &amp; IF(F151&lt;&gt;"","NOT NULL ","") &amp; IF(G151="","","DEFAULT '" &amp; G151 &amp; "' ") &amp; IF(A151="",""," */")</f>
+        <v xml:space="preserve">,`enddate` DATE </v>
       </c>
     </row>
     <row r="152" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A152" s="34"/>
       <c r="B152" s="39" t="s">
-        <v>29</v>
+        <v>153</v>
       </c>
       <c r="C152" s="35" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="D152" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E152" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E152" s="36">
+        <v>256</v>
+      </c>
       <c r="F152" s="35"/>
       <c r="G152" s="37"/>
       <c r="H152" s="38"/>
       <c r="I152" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`notice` TEXT </v>
+        <f t="shared" ref="I152:I160" si="38">"," &amp; IF(A152="","","/* ") &amp; "`" &amp; C152 &amp; "` " &amp; D152 &amp; IF(E152&gt;0,"(" &amp; E152 &amp; ") "," ") &amp; IF(F152&lt;&gt;"","NOT NULL ","") &amp; IF(G152="","","DEFAULT '" &amp; G152 &amp; "' ") &amp; IF(A152="",""," */")</f>
+        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
       <c r="J152" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`notice` TEXT </v>
+        <f t="shared" ref="J152:J160" si="39">"," &amp; IF(A152="","","/* ") &amp; "`" &amp; C152 &amp; "` " &amp; D152 &amp; IF(E152&gt;0,"(" &amp; E152 &amp; ") "," ") &amp; IF(F152&lt;&gt;"","NOT NULL ","") &amp; IF(G152="","","DEFAULT '" &amp; G152 &amp; "' ") &amp; IF(A152="",""," */")</f>
+        <v xml:space="preserve">,`license_key` VARCHAR(256) </v>
       </c>
     </row>
     <row r="153" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A153" s="34"/>
-      <c r="B153" s="43" t="s">
-        <v>87</v>
+      <c r="B153" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="C153" s="35" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="D153" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E153" s="36">
-        <v>256</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E153" s="36"/>
       <c r="F153" s="35"/>
       <c r="G153" s="37"/>
       <c r="H153" s="38"/>
       <c r="I153" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" si="38"/>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
       <c r="J153" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`file` VARCHAR(256) </v>
+        <f t="shared" si="39"/>
+        <v xml:space="preserve">,`notice` TEXT </v>
       </c>
     </row>
     <row r="154" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A154" s="34"/>
       <c r="B154" s="43" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C154" s="35" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="D154" s="35" t="s">
         <v>7</v>
@@ -5981,119 +6015,121 @@
       <c r="G154" s="37"/>
       <c r="H154" s="38"/>
       <c r="I154" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="38"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
       <c r="J154" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
+        <f t="shared" si="39"/>
+        <v xml:space="preserve">,`file` VARCHAR(256) </v>
       </c>
     </row>
     <row r="155" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A155" s="34"/>
       <c r="B155" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C155" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D155" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E155" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E155" s="36">
+        <v>256</v>
+      </c>
       <c r="F155" s="35"/>
       <c r="G155" s="37"/>
       <c r="H155" s="38"/>
       <c r="I155" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="38"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
       <c r="J155" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`size` INT </v>
+        <f t="shared" si="39"/>
+        <v xml:space="preserve">,`dir` VARCHAR(256) </v>
       </c>
     </row>
     <row r="156" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A156" s="34"/>
       <c r="B156" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C156" s="35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D156" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E156" s="36">
-        <v>64</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E156" s="36"/>
       <c r="F156" s="35"/>
       <c r="G156" s="37"/>
       <c r="H156" s="38"/>
       <c r="I156" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <f t="shared" si="38"/>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
       <c r="J156" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`type` VARCHAR(64) </v>
+        <f t="shared" si="39"/>
+        <v xml:space="preserve">,`size` INT </v>
       </c>
     </row>
     <row r="157" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A157" s="34"/>
       <c r="B157" s="43" t="s">
-        <v>161</v>
+        <v>52</v>
       </c>
       <c r="C157" s="35" t="s">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="D157" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="E157" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="E157" s="36">
+        <v>64</v>
+      </c>
       <c r="F157" s="35"/>
       <c r="G157" s="37"/>
       <c r="H157" s="38"/>
       <c r="I157" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="38"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
       <c r="J157" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`user_id` INT </v>
+        <f t="shared" si="39"/>
+        <v xml:space="preserve">,`type` VARCHAR(64) </v>
       </c>
     </row>
     <row r="158" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A158" s="34"/>
       <c r="B158" s="43" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C158" s="35" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="D158" s="35" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E158" s="36"/>
       <c r="F158" s="35"/>
       <c r="G158" s="37"/>
       <c r="H158" s="38"/>
       <c r="I158" s="40" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="38"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
       <c r="J158" s="41" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
+        <f t="shared" si="39"/>
+        <v xml:space="preserve">,`user_id` INT </v>
       </c>
     </row>
     <row r="159" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A159" s="34"/>
       <c r="B159" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C159" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D159" s="35" t="s">
         <v>8</v>
@@ -6103,414 +6139,443 @@
       <c r="G159" s="37"/>
       <c r="H159" s="38"/>
       <c r="I159" s="40" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+      <c r="J159" s="41" t="str">
+        <f t="shared" si="39"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A160" s="34"/>
+      <c r="B160" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C160" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D160" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" s="36"/>
+      <c r="F160" s="35"/>
+      <c r="G160" s="37"/>
+      <c r="H160" s="38"/>
+      <c r="I160" s="40" t="str">
+        <f t="shared" si="38"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
-      <c r="J159" s="41" t="str">
-        <f t="shared" si="37"/>
+      <c r="J160" s="41" t="str">
+        <f t="shared" si="39"/>
         <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A160" s="2"/>
-      <c r="B160" s="21"/>
-      <c r="C160" s="21"/>
-      <c r="D160" s="21"/>
-      <c r="E160" s="22"/>
-      <c r="F160" s="21"/>
-      <c r="G160" s="23"/>
-      <c r="H160" s="21"/>
-      <c r="I160" s="28" t="s">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A161" s="2"/>
+      <c r="B161" s="21"/>
+      <c r="C161" s="21"/>
+      <c r="D161" s="21"/>
+      <c r="E161" s="22"/>
+      <c r="F161" s="21"/>
+      <c r="G161" s="23"/>
+      <c r="H161" s="21"/>
+      <c r="I161" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J160" s="29" t="s">
+      <c r="J161" s="29" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="expression" dxfId="75" priority="188">
+    <cfRule type="expression" dxfId="77" priority="189">
       <formula>A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A7 A42:A43 A134:A135 A80:A82 A123:A124 A13:A14 A84:A94 A98:A99 A31:A33 A35 A108:A111 A117:A118">
-    <cfRule type="cellIs" dxfId="74" priority="187" operator="greaterThan">
+  <conditionalFormatting sqref="A5:A7 A42:A43 A135:A136 A80:A82 A124:A125 A13:A14 A84:A85 A99:A100 A31:A33 A35 A109:A112 A118:A119 A87:A95">
+    <cfRule type="cellIs" dxfId="76" priority="188" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A11:A12">
-    <cfRule type="cellIs" dxfId="73" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="187" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="cellIs" dxfId="72" priority="185" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="186" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="71" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="185" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:A39">
-    <cfRule type="cellIs" dxfId="70" priority="180" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101:A104">
-    <cfRule type="cellIs" dxfId="69" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="181" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102:A105">
+    <cfRule type="cellIs" dxfId="71" priority="179" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A127">
+    <cfRule type="cellIs" dxfId="70" priority="178" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="cellIs" dxfId="69" priority="172" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="cellIs" dxfId="68" priority="170" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:A63 A44:A45 A47">
+    <cfRule type="cellIs" dxfId="67" priority="171" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53 A55">
+    <cfRule type="cellIs" dxfId="66" priority="165" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56 A58">
+    <cfRule type="cellIs" dxfId="65" priority="164" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="cellIs" dxfId="64" priority="163" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="cellIs" dxfId="63" priority="162" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="cellIs" dxfId="62" priority="161" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="cellIs" dxfId="61" priority="160" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A123">
+    <cfRule type="cellIs" dxfId="60" priority="157" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A121">
+    <cfRule type="cellIs" dxfId="59" priority="156" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A128:A131">
+    <cfRule type="cellIs" dxfId="58" priority="155" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A133:A134">
+    <cfRule type="cellIs" dxfId="57" priority="154" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A161 A137">
+    <cfRule type="cellIs" dxfId="56" priority="153" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A117">
+    <cfRule type="cellIs" dxfId="55" priority="147" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="cellIs" dxfId="54" priority="139" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="cellIs" dxfId="53" priority="138" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
+    <cfRule type="cellIs" dxfId="52" priority="137" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115">
+    <cfRule type="cellIs" dxfId="51" priority="136" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:A20 A15:A17">
+    <cfRule type="cellIs" dxfId="50" priority="125" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="cellIs" dxfId="49" priority="121" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="cellIs" dxfId="48" priority="99" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A116">
+    <cfRule type="cellIs" dxfId="47" priority="120" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A138">
+    <cfRule type="cellIs" dxfId="46" priority="109" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="cellIs" dxfId="45" priority="91" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" dxfId="44" priority="98" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="cellIs" dxfId="43" priority="97" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="cellIs" dxfId="42" priority="96" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="cellIs" dxfId="41" priority="95" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A120">
+    <cfRule type="cellIs" dxfId="40" priority="94" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A122">
+    <cfRule type="cellIs" dxfId="39" priority="93" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A126">
-    <cfRule type="cellIs" dxfId="68" priority="177" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97">
-    <cfRule type="cellIs" dxfId="67" priority="171" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="66" priority="169" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:A63 A44:A45 A47">
-    <cfRule type="cellIs" dxfId="65" priority="170" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53 A55">
-    <cfRule type="cellIs" dxfId="64" priority="164" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56 A58">
-    <cfRule type="cellIs" dxfId="63" priority="163" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="cellIs" dxfId="62" priority="162" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="cellIs" dxfId="61" priority="161" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="cellIs" dxfId="60" priority="160" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="59" priority="159" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A122">
-    <cfRule type="cellIs" dxfId="58" priority="156" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A120">
-    <cfRule type="cellIs" dxfId="57" priority="155" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A127:A130">
-    <cfRule type="cellIs" dxfId="56" priority="154" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A132:A133">
-    <cfRule type="cellIs" dxfId="55" priority="153" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A160 A136">
-    <cfRule type="cellIs" dxfId="54" priority="152" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A116">
-    <cfRule type="cellIs" dxfId="53" priority="146" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="cellIs" dxfId="52" priority="138" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="cellIs" dxfId="51" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="92" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113">
-    <cfRule type="cellIs" dxfId="50" priority="136" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A114">
-    <cfRule type="cellIs" dxfId="49" priority="135" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:A20 A15:A17">
-    <cfRule type="cellIs" dxfId="48" priority="124" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="cellIs" dxfId="47" priority="120" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="cellIs" dxfId="46" priority="98" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A115">
-    <cfRule type="cellIs" dxfId="45" priority="119" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A137">
-    <cfRule type="cellIs" dxfId="44" priority="108" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="cellIs" dxfId="43" priority="90" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="cellIs" dxfId="42" priority="97" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="cellIs" dxfId="41" priority="96" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="cellIs" dxfId="40" priority="95" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="cellIs" dxfId="39" priority="94" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A119">
-    <cfRule type="cellIs" dxfId="38" priority="93" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A121">
-    <cfRule type="cellIs" dxfId="37" priority="92" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A125">
-    <cfRule type="cellIs" dxfId="36" priority="91" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A112">
-    <cfRule type="cellIs" dxfId="35" priority="76" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A138">
-    <cfRule type="cellIs" dxfId="34" priority="46" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A149:A150 A143:A144">
-    <cfRule type="cellIs" dxfId="33" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="77" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A139">
+    <cfRule type="cellIs" dxfId="36" priority="47" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A150:A151 A144:A145">
+    <cfRule type="cellIs" dxfId="35" priority="60" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A153">
+    <cfRule type="cellIs" dxfId="34" priority="59" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A149">
+    <cfRule type="cellIs" dxfId="33" priority="58" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A147">
+    <cfRule type="cellIs" dxfId="32" priority="57" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A154:A157">
+    <cfRule type="cellIs" dxfId="31" priority="56" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A159:A160">
+    <cfRule type="cellIs" dxfId="30" priority="55" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A143">
+    <cfRule type="cellIs" dxfId="29" priority="54" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A140">
+    <cfRule type="cellIs" dxfId="28" priority="53" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A141">
+    <cfRule type="cellIs" dxfId="27" priority="52" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A142">
+    <cfRule type="cellIs" dxfId="26" priority="51" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A146">
+    <cfRule type="cellIs" dxfId="25" priority="50" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A148">
+    <cfRule type="cellIs" dxfId="24" priority="49" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152">
-    <cfRule type="cellIs" dxfId="32" priority="58" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A148">
-    <cfRule type="cellIs" dxfId="31" priority="57" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A146">
-    <cfRule type="cellIs" dxfId="30" priority="56" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A153:A156">
-    <cfRule type="cellIs" dxfId="29" priority="55" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A158:A159">
-    <cfRule type="cellIs" dxfId="28" priority="54" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A142">
-    <cfRule type="cellIs" dxfId="27" priority="53" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A139">
-    <cfRule type="cellIs" dxfId="26" priority="52" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A140">
-    <cfRule type="cellIs" dxfId="25" priority="51" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A141">
-    <cfRule type="cellIs" dxfId="24" priority="50" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A145">
-    <cfRule type="cellIs" dxfId="23" priority="49" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A147">
-    <cfRule type="cellIs" dxfId="22" priority="48" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A151">
-    <cfRule type="cellIs" dxfId="21" priority="47" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="48" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78:A79 A64:A65 A69">
-    <cfRule type="cellIs" dxfId="19" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="46" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A25 A21:A22">
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="19" priority="24" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="cellIs" dxfId="18" priority="38" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:A74">
     <cfRule type="cellIs" dxfId="17" priority="23" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="cellIs" dxfId="16" priority="37" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:A74">
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="cellIs" dxfId="13" priority="34" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106:A107">
-    <cfRule type="cellIs" dxfId="12" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="35" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A107:A108">
+    <cfRule type="cellIs" dxfId="14" priority="34" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76:A77">
-    <cfRule type="cellIs" dxfId="11" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="33" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:A61">
-    <cfRule type="cellIs" dxfId="10" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="32" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:A41">
-    <cfRule type="cellIs" dxfId="9" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="31" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="cellIs" dxfId="8" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="30" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A75">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A157">
-    <cfRule type="cellIs" dxfId="6" priority="25" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A131">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="29" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A158">
+    <cfRule type="cellIs" dxfId="8" priority="26" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A132">
+    <cfRule type="cellIs" dxfId="7" priority="27" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:A30 A26:A27">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D12 D16:D18 D65:D77 D45:D61 D137:D159 D111:D133 D22:D23 D81:D107 D27:D28 D32:D35 D36:D41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D12 D16:D18 D65:D77 D45:D61 D138:D160 D112:D134 D22:D23 D27:D28 D32:D41 D81:D108">
       <formula1>TYPE</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>